<commit_message>
Tested euclidean with moving image as input only
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Network</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed and Moving Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed Input</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -414,9 +420,6 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -471,6 +474,8 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -990,7 +995,7 @@
     <col customWidth="1" min="9" max="9" style="1" width="8.8671875"/>
     <col customWidth="1" min="10" max="10" style="1" width="7.9296875"/>
     <col bestFit="1" customWidth="1" min="11" max="11" style="1" width="14.59765625"/>
-    <col customWidth="1" min="12" max="12" style="1" width="16.06640625"/>
+    <col customWidth="1" min="12" max="12" style="1" width="26.8515625"/>
     <col customWidth="1" min="13" max="13" style="1" width="15.42578125"/>
     <col customWidth="1" min="14" max="14" style="1" width="14.5703125"/>
     <col customWidth="1" min="15" max="16" style="1" width="8.5703125"/>
@@ -1032,21 +1037,21 @@
       <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="2">
@@ -1071,14 +1076,14 @@
         <v>16</v>
       </c>
       <c r="K2" s="2"/>
-      <c r="L2" s="12"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" s="1" customFormat="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="13">
+      <c r="A3" s="8"/>
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2">
@@ -1103,16 +1108,16 @@
         <v>16</v>
       </c>
       <c r="K3" s="2"/>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13">
+      <c r="A4" s="8"/>
+      <c r="B4" s="12">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2">
@@ -1137,68 +1142,68 @@
         <v>18</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="A5" s="9"/>
-      <c r="B5" s="14">
+      <c r="A5" s="8"/>
+      <c r="B5" s="13">
         <v>4</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="17"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>168</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>300</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>8</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="20">
         <v>32</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="23"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" ht="15.75">
-      <c r="A7" s="24"/>
-      <c r="B7" s="19">
+      <c r="A7" s="23"/>
+      <c r="B7" s="18">
         <v>2</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="2">
@@ -1222,17 +1227,17 @@
       <c r="J7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="24"/>
-      <c r="B8" s="19">
+      <c r="A8" s="23"/>
+      <c r="B8" s="18">
         <v>3</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="2">
@@ -1256,208 +1261,212 @@
       <c r="J8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="12"/>
+      <c r="L8" s="11"/>
     </row>
     <row r="9" ht="15.75">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="15">
         <v>168</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>300</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>2</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>48</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="17"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="23"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" ht="15.75">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26">
         <v>2</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="23"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26">
         <v>2</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="23"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="22"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26">
         <v>2</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="17"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="16"/>
     </row>
     <row r="16">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="18">
         <v>1</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20">
         <v>1</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>100</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <v>1</v>
       </c>
-      <c r="G16" s="21">
-        <v>16</v>
-      </c>
-      <c r="H16" s="21" t="s">
+      <c r="G16" s="20">
+        <v>32</v>
+      </c>
+      <c r="H16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="I16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="21"/>
-      <c r="L16" s="23"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="27" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17" ht="15.75">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26">
         <v>2</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16">
+      <c r="C17" s="14"/>
+      <c r="D17" s="15">
         <v>1</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="15">
         <v>100</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="15">
         <v>1</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="15">
         <v>32</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="I17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="17"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="28" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Built creation for SIMPLE data set
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Network</t>
   </si>
@@ -21,6 +21,9 @@
     <t>Training</t>
   </si>
   <si>
+    <t xml:space="preserve">Data Set</t>
+  </si>
+  <si>
     <t xml:space="preserve">Train Size</t>
   </si>
   <si>
@@ -81,6 +84,9 @@
     <t>Unet</t>
   </si>
   <si>
+    <t>LASTEN</t>
+  </si>
+  <si>
     <t xml:space="preserve">384 x 384</t>
   </si>
   <si>
@@ -117,16 +123,25 @@
     <t>6_euclidean</t>
   </si>
   <si>
-    <t>112x112</t>
-  </si>
-  <si>
-    <t>custom</t>
+    <t>SIMPLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 /250</t>
+  </si>
+  <si>
+    <t>224x224</t>
+  </si>
+  <si>
+    <t>maed</t>
   </si>
   <si>
     <t xml:space="preserve">Fixed and Moving Input</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed Input</t>
+    <t>msed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moving Input</t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -420,6 +435,9 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -458,6 +476,9 @@
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,6 +486,9 @@
     <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -474,7 +498,11 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -986,24 +1014,24 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="22"/>
     <col customWidth="1" min="2" max="2" style="1" width="11.328125"/>
-    <col customWidth="1" min="3" max="3" style="1" width="10.52734375"/>
-    <col customWidth="1" min="4" max="4" style="1" width="10.66796875"/>
-    <col customWidth="1" min="5" max="5" style="1" width="9.19921875"/>
-    <col customWidth="1" min="6" max="6" style="1" width="12.328125"/>
-    <col customWidth="1" min="7" max="7" style="1" width="13.19921875"/>
-    <col customWidth="1" min="8" max="8" style="1" width="12.328125"/>
-    <col customWidth="1" min="9" max="9" style="1" width="8.8671875"/>
-    <col customWidth="1" min="10" max="10" style="1" width="7.9296875"/>
-    <col bestFit="1" customWidth="1" min="11" max="11" style="1" width="14.59765625"/>
-    <col customWidth="1" min="12" max="12" style="1" width="26.8515625"/>
-    <col customWidth="1" min="13" max="13" style="1" width="15.42578125"/>
-    <col customWidth="1" min="14" max="14" style="1" width="14.5703125"/>
-    <col customWidth="1" min="15" max="16" style="1" width="8.5703125"/>
-    <col customWidth="1" min="17" max="17" style="1" width="14.42578125"/>
-    <col customWidth="1" min="18" max="18" style="1" width="15.42578125"/>
-    <col customWidth="1" min="19" max="1026" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1027" max="1029" style="1" width="9.140625"/>
-    <col min="1030" max="16384" width="9.140625"/>
+    <col customWidth="1" min="3" max="4" style="1" width="10.52734375"/>
+    <col customWidth="1" min="5" max="5" style="1" width="10.66796875"/>
+    <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
+    <col customWidth="1" min="7" max="7" style="1" width="12.328125"/>
+    <col customWidth="1" min="8" max="8" style="1" width="13.19921875"/>
+    <col customWidth="1" min="9" max="9" style="1" width="12.328125"/>
+    <col customWidth="1" min="10" max="10" style="1" width="8.8671875"/>
+    <col customWidth="1" min="11" max="11" style="1" width="7.9296875"/>
+    <col bestFit="1" customWidth="1" min="12" max="12" style="1" width="14.59765625"/>
+    <col customWidth="1" min="13" max="13" style="1" width="26.8515625"/>
+    <col customWidth="1" min="14" max="14" style="1" width="15.42578125"/>
+    <col customWidth="1" min="15" max="15" style="1" width="14.5703125"/>
+    <col customWidth="1" min="16" max="17" style="1" width="8.5703125"/>
+    <col customWidth="1" min="18" max="18" style="1" width="14.42578125"/>
+    <col customWidth="1" min="19" max="19" style="1" width="15.42578125"/>
+    <col customWidth="1" min="20" max="1027" style="1" width="8.5703125"/>
+    <col customWidth="1" min="1028" max="1030" style="1" width="9.140625"/>
+    <col min="1031" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75">
@@ -1019,52 +1047,53 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="M1" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>3000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>14</v>
@@ -1075,28 +1104,29 @@
       <c r="J2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="L2" s="11"/>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="12"/>
     </row>
     <row r="3" s="1" customFormat="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12">
+      <c r="A3" s="9"/>
+      <c r="B3" s="13">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>3000</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>14</v>
@@ -1107,30 +1137,31 @@
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="11" t="s">
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" s="1" customFormat="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12">
+      <c r="A4" s="9"/>
+      <c r="B4" s="13">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
         <v>168</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>300</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>16</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>14</v>
@@ -1139,334 +1170,379 @@
         <v>15</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
+      <c r="A5" s="9"/>
+      <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
       <c r="L5" s="16"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="18">
+      <c r="A6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="20">
+      <c r="C6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="22">
         <v>168</v>
       </c>
-      <c r="E6" s="20">
+      <c r="F6" s="22">
         <v>300</v>
       </c>
-      <c r="F6" s="20">
+      <c r="G6" s="22">
         <v>8</v>
       </c>
-      <c r="G6" s="20">
+      <c r="H6" s="22">
         <v>32</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="I6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="24"/>
+    </row>
+    <row r="7" ht="15.75">
+      <c r="A7" s="25"/>
+      <c r="B7" s="19">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="D7" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="E7" s="2">
+        <v>168</v>
+      </c>
+      <c r="F7" s="2">
+        <v>300</v>
+      </c>
+      <c r="G7" s="2">
+        <v>8</v>
+      </c>
+      <c r="H7" s="2">
+        <v>48</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="J7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L6" s="22"/>
-    </row>
-    <row r="7" ht="15.75">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18">
+      <c r="K7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="12"/>
+    </row>
+    <row r="8" ht="15.75">
+      <c r="A8" s="25"/>
+      <c r="B8" s="19">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2">
+        <v>168</v>
+      </c>
+      <c r="F8" s="2">
+        <v>300</v>
+      </c>
+      <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="H8" s="2">
+        <v>32</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="12"/>
+    </row>
+    <row r="9" ht="15.75">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="16">
         <v>168</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F9" s="16">
         <v>300</v>
       </c>
-      <c r="F7" s="2">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="G9" s="16">
+        <v>2</v>
+      </c>
+      <c r="H9" s="16">
         <v>48</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" s="24" t="s">
+      <c r="I9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="11"/>
-    </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2">
-        <v>168</v>
-      </c>
-      <c r="E8" s="2">
-        <v>300</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="L9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="24"/>
+    </row>
+    <row r="11" ht="15.75">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29">
         <v>2</v>
       </c>
-      <c r="G8" s="2">
-        <v>32</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="11"/>
-    </row>
-    <row r="9" ht="15.75">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26">
-        <v>4</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="15">
-        <v>168</v>
-      </c>
-      <c r="E9" s="15">
-        <v>300</v>
-      </c>
-      <c r="F9" s="15">
-        <v>2</v>
-      </c>
-      <c r="G9" s="15">
-        <v>48</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="22"/>
-    </row>
-    <row r="11" ht="15.75">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26">
-        <v>2</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
       <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
-        <v>31</v>
+      <c r="A12" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="22"/>
+      <c r="M12" s="24"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="16"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>32</v>
+      <c r="A14" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="22"/>
+      <c r="M14" s="24"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29">
         <v>2</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
       <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16">
-      <c r="A16" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="18">
+      <c r="A16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="19">
         <v>1</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="22">
         <v>1</v>
       </c>
-      <c r="E16" s="20">
-        <v>100</v>
-      </c>
-      <c r="F16" s="20">
+      <c r="F16" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="22">
         <v>1</v>
       </c>
-      <c r="G16" s="20">
+      <c r="H16" s="22">
         <v>32</v>
       </c>
-      <c r="H16" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="K16" s="20"/>
-      <c r="L16" s="27" t="s">
+      <c r="I16" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="22"/>
+      <c r="M16" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="25"/>
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="26" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" ht="15.75">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26">
-        <v>2</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="15">
+      <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="E17" s="15">
-        <v>100</v>
-      </c>
-      <c r="F17" s="15">
+      <c r="F17" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="2">
         <v>1</v>
       </c>
-      <c r="G17" s="15">
+      <c r="H17" s="2">
         <v>32</v>
       </c>
-      <c r="H17" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="15"/>
-      <c r="L17" s="28" t="s">
-        <v>37</v>
-      </c>
+      <c r="I17" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29">
+        <v>3</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1475,7 +1551,7 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Developed generator for SIMPLE data set
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Network</t>
   </si>
@@ -39,6 +39,9 @@
     <t xml:space="preserve">Image Size</t>
   </si>
   <si>
+    <t>Augment</t>
+  </si>
+  <si>
     <t>Loss</t>
   </si>
   <si>
@@ -142,6 +145,15 @@
   </si>
   <si>
     <t xml:space="preserve">Moving Input</t>
+  </si>
+  <si>
+    <t>SIMPLEA</t>
+  </si>
+  <si>
+    <t>SIMPLEN</t>
+  </si>
+  <si>
+    <t>SIMPLED</t>
   </si>
 </sst>
 </file>
@@ -417,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -476,9 +488,6 @@
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,9 +495,6 @@
     <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,12 +504,12 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1019,19 +1025,19 @@
     <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
     <col customWidth="1" min="7" max="7" style="1" width="12.328125"/>
     <col customWidth="1" min="8" max="8" style="1" width="13.19921875"/>
-    <col customWidth="1" min="9" max="9" style="1" width="12.328125"/>
-    <col customWidth="1" min="10" max="10" style="1" width="8.8671875"/>
-    <col customWidth="1" min="11" max="11" style="1" width="7.9296875"/>
-    <col bestFit="1" customWidth="1" min="12" max="12" style="1" width="14.59765625"/>
-    <col customWidth="1" min="13" max="13" style="1" width="26.8515625"/>
-    <col customWidth="1" min="14" max="14" style="1" width="15.42578125"/>
-    <col customWidth="1" min="15" max="15" style="1" width="14.5703125"/>
-    <col customWidth="1" min="16" max="17" style="1" width="8.5703125"/>
-    <col customWidth="1" min="18" max="18" style="1" width="14.42578125"/>
-    <col customWidth="1" min="19" max="19" style="1" width="15.42578125"/>
-    <col customWidth="1" min="20" max="1027" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1028" max="1030" style="1" width="9.140625"/>
-    <col min="1031" max="16384" width="9.140625"/>
+    <col customWidth="1" min="9" max="10" style="1" width="12.328125"/>
+    <col customWidth="1" min="11" max="11" style="1" width="8.8671875"/>
+    <col customWidth="1" min="12" max="12" style="1" width="7.9296875"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" style="1" width="14.59765625"/>
+    <col customWidth="1" min="14" max="14" style="1" width="26.8515625"/>
+    <col customWidth="1" min="15" max="15" style="1" width="15.42578125"/>
+    <col customWidth="1" min="16" max="16" style="1" width="14.5703125"/>
+    <col customWidth="1" min="17" max="18" style="1" width="8.5703125"/>
+    <col customWidth="1" min="19" max="19" style="1" width="14.42578125"/>
+    <col customWidth="1" min="20" max="20" style="1" width="15.42578125"/>
+    <col customWidth="1" min="21" max="1028" style="1" width="8.5703125"/>
+    <col customWidth="1" min="1029" max="1031" style="1" width="9.140625"/>
+    <col min="1032" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75">
@@ -1047,43 +1053,46 @@
       <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="10">
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
@@ -1096,19 +1105,22 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="J2" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="12"/>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="12"/>
     </row>
     <row r="3" s="1" customFormat="1">
       <c r="A3" s="9"/>
@@ -1116,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
@@ -1129,20 +1141,23 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="J3" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="12" t="s">
+      <c r="L3" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1">
@@ -1151,7 +1166,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -1164,20 +1179,23 @@
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="K4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" ht="15.75">
@@ -1195,57 +1213,61 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="17"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" ht="15.75">
       <c r="A6" s="18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="19">
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="22">
+        <v>24</v>
+      </c>
+      <c r="E6" s="21">
         <v>168</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>300</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>8</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>32</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="J6" s="21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="24"/>
+      <c r="M6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="23"/>
     </row>
     <row r="7" ht="15.75">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="19">
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="26" t="s">
         <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E7" s="2">
         <v>168</v>
@@ -1260,29 +1282,32 @@
         <v>48</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="2" t="s">
         <v>25</v>
+      </c>
+      <c r="J7" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="12"/>
+      <c r="L7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="19">
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="26" t="s">
         <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E8" s="2">
         <v>168</v>
@@ -1297,29 +1322,32 @@
         <v>32</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="J8" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="12"/>
+      <c r="L8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" ht="15.75">
-      <c r="A9" s="28"/>
-      <c r="B9" s="29">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27">
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="30" t="s">
         <v>23</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="E9" s="16">
         <v>168</v>
@@ -1334,41 +1362,45 @@
         <v>48</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="J9" s="16" t="b">
+        <v>1</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="17"/>
+        <v>27</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="17"/>
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="19">
         <v>1</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="24"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" ht="15.75">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27">
         <v>2</v>
       </c>
       <c r="C11" s="15"/>
@@ -1381,30 +1413,32 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16"/>
-      <c r="M11" s="17"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="12">
       <c r="A12" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="24"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27">
         <v>2</v>
       </c>
       <c r="C13" s="15"/>
@@ -1417,30 +1451,32 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
-      <c r="M13" s="17"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="17"/>
     </row>
     <row r="14">
       <c r="A14" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="20"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="24"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27">
         <v>2</v>
       </c>
       <c r="C15" s="15"/>
@@ -1453,59 +1489,63 @@
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
-      <c r="M15" s="17"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="17"/>
     </row>
     <row r="16">
-      <c r="A16" s="25" t="s">
-        <v>35</v>
+      <c r="A16" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="B16" s="19">
         <v>1</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="22">
+        <v>37</v>
+      </c>
+      <c r="E16" s="21">
         <v>1</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="22">
-        <v>1</v>
-      </c>
-      <c r="H16" s="22">
+        <v>38</v>
+      </c>
+      <c r="G16" s="21">
+        <v>1</v>
+      </c>
+      <c r="H16" s="21">
         <v>32</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="J16" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="J16" s="21" t="b">
+        <v>0</v>
+      </c>
       <c r="K16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="31" t="s">
         <v>40</v>
       </c>
+      <c r="L16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="23" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="19">
         <v>2</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="26" t="s">
-        <v>36</v>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
-      <c r="F17" s="26" t="s">
-        <v>37</v>
+      <c r="F17" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -1513,36 +1553,94 @@
       <c r="H17" s="2">
         <v>32</v>
       </c>
-      <c r="I17" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="J17" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="32" t="s">
+      <c r="I17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" ht="15.75">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29">
+      <c r="L17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="24"/>
+      <c r="B18" s="19">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="33"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="2">
+        <v>168</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <v>32</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="24"/>
+      <c r="B19" s="19">
+        <v>4</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" ht="15.75">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1551,7 +1649,7 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A16:A20"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Custom loss test added
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Network</t>
   </si>
@@ -33,6 +33,9 @@
     <t xml:space="preserve">Batch Size</t>
   </si>
   <si>
+    <t>Depth</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature Maps</t>
   </si>
   <si>
@@ -48,6 +51,21 @@
     <t>Score</t>
   </si>
   <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Regularizer</t>
+  </si>
+  <si>
+    <t>Dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gap Filling</t>
+  </si>
+  <si>
     <t xml:space="preserve">Score Value</t>
   </si>
   <si>
@@ -138,12 +156,21 @@
     <t>maed</t>
   </si>
   <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Fixed+Moving</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fixed and Moving Input</t>
   </si>
   <si>
     <t>msed</t>
   </si>
   <si>
+    <t>Moving</t>
+  </si>
+  <si>
     <t xml:space="preserve">Moving Input</t>
   </si>
   <si>
@@ -154,6 +181,24 @@
   </si>
   <si>
     <t>SIMPLED</t>
+  </si>
+  <si>
+    <t>Moving+Fixed</t>
+  </si>
+  <si>
+    <t>Moving+Gradient</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>Possibilities</t>
   </si>
 </sst>
 </file>
@@ -172,15 +217,82 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6DE3C5"/>
+        <bgColor rgb="FF6DE3C5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFA0A0"/>
+        <bgColor rgb="FFBFA0A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB07DDB"/>
+        <bgColor rgb="FFB07DDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF57070"/>
+        <bgColor rgb="FFF57070"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB0A892"/>
+        <bgColor rgb="FFB0A892"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE07FDD"/>
+        <bgColor rgb="FFE07FDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF30ABAB"/>
+        <bgColor rgb="FF30ABAB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0EB4C"/>
+        <bgColor rgb="FFE0EB4C"/>
+      </patternFill>
+    </fill>
+    <fill/>
   </fills>
-  <borders count="22">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -425,11 +537,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="51">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -447,6 +609,9 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,6 +666,73 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1014,21 +1246,25 @@
     <col customWidth="1" min="3" max="4" style="1" width="10.52734375"/>
     <col customWidth="1" min="5" max="5" style="1" width="10.66796875"/>
     <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
-    <col customWidth="1" min="7" max="7" style="1" width="12.328125"/>
-    <col customWidth="1" min="8" max="8" style="1" width="13.19921875"/>
-    <col customWidth="1" min="9" max="10" style="1" width="12.328125"/>
-    <col customWidth="1" min="11" max="11" style="1" width="8.8671875"/>
-    <col customWidth="1" min="12" max="12" style="1" width="7.9296875"/>
-    <col bestFit="1" customWidth="1" min="13" max="13" style="1" width="14.59765625"/>
-    <col customWidth="1" min="14" max="14" style="1" width="26.8515625"/>
-    <col customWidth="1" min="15" max="15" style="1" width="15.42578125"/>
-    <col customWidth="1" min="16" max="16" style="1" width="14.5703125"/>
-    <col customWidth="1" min="17" max="18" style="1" width="8.5703125"/>
-    <col customWidth="1" min="19" max="19" style="1" width="14.42578125"/>
-    <col customWidth="1" min="20" max="20" style="1" width="15.42578125"/>
-    <col customWidth="1" min="21" max="1028" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1029" max="1031" style="1" width="9.140625"/>
-    <col min="1032" max="16384" width="9.140625"/>
+    <col customWidth="1" min="7" max="8" style="1" width="12.328125"/>
+    <col customWidth="1" min="9" max="9" style="1" width="13.19921875"/>
+    <col customWidth="1" min="10" max="11" style="1" width="12.328125"/>
+    <col customWidth="1" min="12" max="12" style="1" width="8.8671875"/>
+    <col customWidth="1" min="13" max="13" style="1" width="7.9296875"/>
+    <col customWidth="1" min="14" max="14" style="1" width="11.57421875"/>
+    <col customWidth="1" min="15" max="15" style="1" width="17.7109375"/>
+    <col customWidth="1" min="16" max="16" style="1" width="13.7109375"/>
+    <col customWidth="1" min="17" max="18" style="1" width="15.7109375"/>
+    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="14.59765625"/>
+    <col customWidth="1" min="20" max="20" style="1" width="26.8515625"/>
+    <col customWidth="1" min="21" max="21" style="1" width="15.42578125"/>
+    <col customWidth="1" min="22" max="22" style="1" width="14.5703125"/>
+    <col customWidth="1" min="23" max="24" style="1" width="8.5703125"/>
+    <col customWidth="1" min="25" max="25" style="1" width="14.42578125"/>
+    <col customWidth="1" min="26" max="26" style="1" width="15.42578125"/>
+    <col customWidth="1" min="27" max="1034" style="1" width="8.5703125"/>
+    <col customWidth="1" min="1035" max="1037" style="1" width="9.140625"/>
+    <col min="1038" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="15.75">
@@ -1053,7 +1289,7 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -1074,16 +1310,34 @@
       <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>14</v>
+      <c r="C2" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
@@ -1095,31 +1349,37 @@
       <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="2" t="b">
+        <v>21</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="12"/>
     </row>
     <row r="3" s="1" customFormat="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12">
+      <c r="A3" s="9"/>
+      <c r="B3" s="13">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>14</v>
+      <c r="C3" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
@@ -1131,33 +1391,39 @@
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="2" t="b">
+        <v>21</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="11" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" s="1" customFormat="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12">
+      <c r="A4" s="9"/>
+      <c r="B4" s="13">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>14</v>
+      <c r="C4" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -1169,96 +1435,114 @@
       <c r="G4" s="2">
         <v>16</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2" t="b">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="11" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="15.75">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
+      <c r="A5" s="9"/>
+      <c r="B5" s="14">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="17"/>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="18">
+      <c r="A6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20">
+      <c r="C6" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="21">
         <v>168</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
         <v>300</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="21">
         <v>8</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="21"/>
+      <c r="I6" s="21">
         <v>32</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="20" t="b">
+      <c r="J6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>27</v>
+      <c r="L6" s="21" t="s">
+        <v>32</v>
       </c>
       <c r="M6" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="22"/>
+        <v>33</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" ht="15.75">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18">
+      <c r="A7" s="24"/>
+      <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>23</v>
+      <c r="C7" s="11" t="s">
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2">
         <v>168</v>
@@ -1269,36 +1553,42 @@
       <c r="G7" s="2">
         <v>8</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
         <v>48</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2" t="b">
+      <c r="J7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="L7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="12"/>
+    </row>
+    <row r="8" ht="15.75">
+      <c r="A8" s="24"/>
+      <c r="B8" s="19">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="11"/>
-    </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18">
-        <v>3</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E8" s="2">
         <v>168</v>
@@ -1309,266 +1599,350 @@
       <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
         <v>32</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="T8" s="12"/>
+    </row>
+    <row r="9" ht="15.75">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="2" t="b">
+      <c r="E9" s="16">
+        <v>168</v>
+      </c>
+      <c r="F9" s="16">
+        <v>300</v>
+      </c>
+      <c r="G9" s="16">
+        <v>2</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16">
+        <v>48</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="N8" s="11"/>
-    </row>
-    <row r="9" ht="15.75">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26">
-        <v>4</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="15">
-        <v>168</v>
-      </c>
-      <c r="F9" s="15">
-        <v>300</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="L9" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="17"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="23"/>
+    </row>
+    <row r="11" ht="15.75">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27">
         <v>2</v>
       </c>
-      <c r="H9" s="15">
-        <v>48</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="22"/>
-    </row>
-    <row r="11" ht="15.75">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26">
-        <v>2</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
       <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="17"/>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="s">
-        <v>34</v>
+      <c r="A12" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="22"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+      <c r="T12" s="23"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
       <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="17"/>
     </row>
     <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>35</v>
+      <c r="A14" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="22"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="23"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27">
         <v>2</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
       <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="17"/>
     </row>
     <row r="16">
-      <c r="A16" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="18">
+      <c r="A16" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="19">
         <v>1</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="20">
+      <c r="C16" s="20"/>
+      <c r="D16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="21">
         <v>1</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="20">
+      <c r="F16" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="21">
         <v>1</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="21">
+        <v>4</v>
+      </c>
+      <c r="I16" s="21">
         <v>32</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="20"/>
-      <c r="N16" s="22" t="s">
-        <v>41</v>
+      <c r="J16" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="P16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="21"/>
+      <c r="T16" s="23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="23"/>
-      <c r="B17" s="18">
+      <c r="A17" s="24"/>
+      <c r="B17" s="19">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E17" s="2">
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
       </c>
       <c r="H17" s="2">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2">
         <v>32</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>42</v>
+      <c r="J17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="2"/>
+      <c r="T17" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="23"/>
-      <c r="B18" s="18">
+      <c r="A18" s="24"/>
+      <c r="B18" s="19">
         <v>3</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E18" s="2">
         <v>168</v>
@@ -1580,64 +1954,923 @@
         <v>4</v>
       </c>
       <c r="H18" s="2">
+        <v>4</v>
+      </c>
+      <c r="I18" s="2">
         <v>32</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>42</v>
+      <c r="J18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="2">
+        <v>50</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="2">
         <v>51.599499999999999</v>
       </c>
-      <c r="N18" s="11"/>
+      <c r="T18" s="12"/>
     </row>
     <row r="19">
-      <c r="A19" s="23"/>
-      <c r="B19" s="18">
+      <c r="A19" s="24"/>
+      <c r="B19" s="19">
         <v>4</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F19" s="2">
+        <v>100</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
+        <v>4</v>
+      </c>
+      <c r="I19" s="2">
+        <v>32</v>
+      </c>
+      <c r="J19" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="11"/>
-    </row>
-    <row r="20" ht="15.75">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26">
+      <c r="K19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O19" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="12"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="24"/>
+      <c r="B20" s="19">
         <v>5</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F20" s="2">
+        <v>100</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2">
+        <v>4</v>
+      </c>
+      <c r="I20" s="2">
+        <v>32</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="2"/>
+      <c r="T20" s="12"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="24"/>
+      <c r="B21" s="19">
+        <v>6</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F21" s="2">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="32">
+        <v>4</v>
+      </c>
+      <c r="I21" s="33">
+        <v>32</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="P21" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="T21" s="12"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="24"/>
+      <c r="B22" s="19">
+        <v>7</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F22" s="2">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2">
+        <v>4</v>
+      </c>
+      <c r="I22" s="2">
+        <v>32</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="16"/>
+      <c r="M22" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="2"/>
+      <c r="T22" s="12"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="24"/>
+      <c r="B23" s="19">
+        <v>8</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F23" s="2">
+        <v>100</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2">
+        <v>4</v>
+      </c>
+      <c r="I23" s="2">
+        <v>32</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="P23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="2"/>
+      <c r="T23" s="12"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="24"/>
+      <c r="B24" s="19">
+        <v>9</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F24" s="2">
+        <v>100</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2">
+        <v>4</v>
+      </c>
+      <c r="I24" s="2">
+        <v>32</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O24" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="P24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24" s="2"/>
+      <c r="T24" s="12"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="19">
+        <v>10</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F25" s="2">
+        <v>100</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2">
+        <v>4</v>
+      </c>
+      <c r="I25" s="2">
+        <v>32</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O25" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R25" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="12"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="24"/>
+      <c r="B26" s="19">
+        <v>11</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F26" s="2">
+        <v>100</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <v>4</v>
+      </c>
+      <c r="I26" s="2">
+        <v>32</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O26" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="12"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="24"/>
+      <c r="B27" s="19">
+        <v>12</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F27" s="2">
+        <v>100</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2">
+        <v>4</v>
+      </c>
+      <c r="I27" s="2">
+        <v>32</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N27" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P27" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="12"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="24"/>
+      <c r="B28" s="19">
+        <v>13</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F28" s="2">
+        <v>100</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <v>4</v>
+      </c>
+      <c r="I28" s="2">
+        <v>32</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N28" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P28" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="12"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="24"/>
+      <c r="B29" s="19">
+        <v>14</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F29" s="2">
+        <v>100</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2">
+        <v>4</v>
+      </c>
+      <c r="I29" s="2">
+        <v>32</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="O29" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="P29" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29" s="2"/>
+      <c r="T29" s="12"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="24"/>
+      <c r="B30" s="19">
+        <v>15</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F30" s="2">
+        <v>100</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2">
+        <v>4</v>
+      </c>
+      <c r="I30" s="2">
+        <v>32</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P30" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R30" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="12"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="24"/>
+      <c r="B31" s="19">
+        <v>16</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F31" s="2">
+        <v>100</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2">
+        <v>4</v>
+      </c>
+      <c r="I31" s="33">
+        <v>48</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="12"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="24"/>
+      <c r="B32" s="19">
+        <v>17</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F32" s="2">
+        <v>100</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2">
+        <v>4</v>
+      </c>
+      <c r="I32" s="2">
+        <v>32</v>
+      </c>
+      <c r="J32" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" s="2"/>
+      <c r="T32" s="12"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="24"/>
+      <c r="B33" s="19">
+        <v>18</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F33" s="2">
+        <v>100</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="32">
+        <v>6</v>
+      </c>
+      <c r="I33" s="2">
+        <v>32</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S33" s="2"/>
+      <c r="T33" s="12"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="24"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="12"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="24"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="12"/>
+    </row>
+    <row r="36" ht="15.75">
+      <c r="A36" s="26"/>
+      <c r="B36" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49">
+        <v>3</v>
+      </c>
+      <c r="E36" s="49">
+        <v>1</v>
+      </c>
+      <c r="F36" s="49">
+        <v>1</v>
+      </c>
+      <c r="G36" s="49">
+        <v>1</v>
+      </c>
+      <c r="H36" s="49">
+        <v>2</v>
+      </c>
+      <c r="I36" s="49">
+        <v>2</v>
+      </c>
+      <c r="J36" s="49">
+        <v>2</v>
+      </c>
+      <c r="K36" s="49">
+        <v>2</v>
+      </c>
+      <c r="L36" s="49">
+        <v>2</v>
+      </c>
+      <c r="M36" s="49">
+        <v>1</v>
+      </c>
+      <c r="N36" s="49">
+        <v>2</v>
+      </c>
+      <c r="O36" s="49">
+        <v>3</v>
+      </c>
+      <c r="P36" s="49">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="49">
+        <v>2</v>
+      </c>
+      <c r="R36" s="49">
+        <v>2</v>
+      </c>
+      <c r="S36" s="49"/>
+      <c r="T36" s="50">
+        <f>PRODUCT(D36:R36)</f>
+        <v>4608</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1646,7 +2879,7 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A16:A36"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Training 6_4_5_6 ran and 6_7 started
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Julian\workspace\endolas\experiments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="62">
   <si>
     <t>Network</t>
   </si>
@@ -21,25 +27,25 @@
     <t>Training</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train Size</t>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Train Size</t>
   </si>
   <si>
     <t>Epochs</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch Size</t>
+    <t>Batch Size</t>
   </si>
   <si>
     <t>Depth</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature Maps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Size</t>
+    <t>Feature Maps</t>
+  </si>
+  <si>
+    <t>Image Size</t>
   </si>
   <si>
     <t>Augment</t>
@@ -63,10 +69,10 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t xml:space="preserve">Gap Filling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score Value</t>
+    <t>Gap Filling</t>
+  </si>
+  <si>
+    <t>Score Value</t>
   </si>
   <si>
     <t>Note</t>
@@ -90,13 +96,13 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Dropout</t>
+    <t>No Dropout</t>
   </si>
   <si>
     <t>MAE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Preprocessing</t>
+    <t>No Preprocessing</t>
   </si>
   <si>
     <t>2_segmentation</t>
@@ -108,7 +114,7 @@
     <t>LASTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">384 x 384</t>
+    <t>384 x 384</t>
   </si>
   <si>
     <t>Dice</t>
@@ -147,7 +153,7 @@
     <t>SIMPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">100 /250</t>
+    <t>100 /250</t>
   </si>
   <si>
     <t>224x224</t>
@@ -162,7 +168,7 @@
     <t>Fixed+Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed and Moving Input</t>
+    <t>Fixed and Moving Input</t>
   </si>
   <si>
     <t>msed</t>
@@ -171,7 +177,7 @@
     <t>Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Moving Input</t>
+    <t>Moving Input</t>
   </si>
   <si>
     <t>SIMPLEA</t>
@@ -204,17 +210,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="64"/>
       <name val="Arial Unicode MS"/>
-      <color indexed="64"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="14">
@@ -290,7 +296,12 @@
         <bgColor rgb="FFE0EB4C"/>
       </patternFill>
     </fill>
-    <fill/>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="1"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -589,444 +600,175 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="53">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1229,45 +971,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMW36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="M10" activeCellId="0" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="22"/>
-    <col customWidth="1" min="2" max="2" style="1" width="11.328125"/>
-    <col customWidth="1" min="3" max="4" style="1" width="10.52734375"/>
-    <col customWidth="1" min="5" max="5" style="1" width="10.66796875"/>
-    <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
-    <col customWidth="1" min="7" max="8" style="1" width="12.328125"/>
-    <col customWidth="1" min="9" max="9" style="1" width="13.19921875"/>
-    <col customWidth="1" min="10" max="11" style="1" width="12.328125"/>
-    <col customWidth="1" min="12" max="12" style="1" width="8.8671875"/>
-    <col customWidth="1" min="13" max="13" style="1" width="7.9296875"/>
-    <col customWidth="1" min="14" max="14" style="1" width="11.57421875"/>
-    <col customWidth="1" min="15" max="15" style="1" width="17.7109375"/>
-    <col customWidth="1" min="16" max="16" style="1" width="13.7109375"/>
-    <col customWidth="1" min="17" max="18" style="1" width="15.7109375"/>
-    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="14.59765625"/>
-    <col customWidth="1" min="20" max="20" style="1" width="26.8515625"/>
-    <col customWidth="1" min="21" max="21" style="1" width="15.42578125"/>
-    <col customWidth="1" min="22" max="22" style="1" width="14.5703125"/>
-    <col customWidth="1" min="23" max="24" style="1" width="8.5703125"/>
-    <col customWidth="1" min="25" max="25" style="1" width="14.42578125"/>
-    <col customWidth="1" min="26" max="26" style="1" width="15.42578125"/>
-    <col customWidth="1" min="27" max="1034" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1035" max="1037" style="1" width="9.140625"/>
-    <col min="1038" max="16384" width="9.140625"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="8.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" style="1" customWidth="1"/>
+    <col min="27" max="1034" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1035" max="1037" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1329,14 +1072,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2"/>
@@ -1371,14 +1114,14 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="12"/>
-    </row>
-    <row r="3" s="1" customFormat="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="13">
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1">
+      <c r="A3" s="47"/>
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="2"/>
@@ -1413,16 +1156,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="13">
+    <row r="4" spans="1:20" s="1" customFormat="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="12">
         <v>3</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2"/>
@@ -1457,88 +1200,88 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" ht="15.75">
-      <c r="A5" s="9"/>
-      <c r="B5" s="14">
+    <row r="5" spans="1:20">
+      <c r="A5" s="47"/>
+      <c r="B5" s="13">
         <v>4</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="17"/>
-    </row>
-    <row r="6" ht="15.75">
-      <c r="A6" s="18" t="s">
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="16"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>168</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>300</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="19">
         <v>8</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21">
+      <c r="H6" s="19"/>
+      <c r="I6" s="19">
         <v>32</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="21" t="b">
+      <c r="K6" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="22" t="s">
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="23"/>
-    </row>
-    <row r="7" ht="15.75">
-      <c r="A7" s="24"/>
-      <c r="B7" s="19">
+      <c r="T6" s="21"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="49"/>
+      <c r="B7" s="17">
         <v>2</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1574,17 +1317,17 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="25" t="s">
+      <c r="S7" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="T7" s="12"/>
-    </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="24"/>
-      <c r="B8" s="19">
+      <c r="T7" s="11"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="49"/>
+      <c r="B8" s="17">
         <v>3</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1620,271 +1363,271 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="12"/>
-    </row>
-    <row r="9" ht="15.75">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27">
+      <c r="T8" s="11"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="50"/>
+      <c r="B9" s="23">
         <v>4</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>168</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="15">
         <v>300</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="15">
         <v>2</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15">
         <v>48</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="16" t="b">
+      <c r="K9" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16" t="s">
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="17"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="18" t="s">
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="23"/>
-    </row>
-    <row r="11" ht="15.75">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27">
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="21"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="50"/>
+      <c r="B11" s="23">
         <v>2</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="17"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="18" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="48" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="21"/>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-      <c r="T12" s="23"/>
-    </row>
-    <row r="13" ht="15.75">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27">
+      <c r="C12" s="18"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="21"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="50"/>
+      <c r="B13" s="23">
         <v>2</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="17"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="18" t="s">
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="16"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="48" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="23"/>
-    </row>
-    <row r="15" ht="15.75">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27">
+      <c r="C14" s="18"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="21"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="50"/>
+      <c r="B15" s="23">
         <v>2</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="17"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="24" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="16"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>1</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="19">
         <v>1</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="19">
         <v>1</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="19">
         <v>4</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="19">
         <v>32</v>
       </c>
-      <c r="J16" s="21" t="s">
+      <c r="J16" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="21" t="s">
+      <c r="K16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="M16" s="19" t="s">
         <v>46</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="P16" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="21"/>
-      <c r="T16" s="23" t="s">
+      <c r="P16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="51"/>
+      <c r="T16" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="24"/>
-      <c r="B17" s="19">
+    <row r="17" spans="1:20">
+      <c r="A17" s="49"/>
+      <c r="B17" s="17">
         <v>2</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1906,7 +1649,7 @@
       <c r="J17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="2" t="s">
@@ -1918,29 +1661,29 @@
       <c r="N17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P17" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R17" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="12" t="s">
+      <c r="P17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="52"/>
+      <c r="T17" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="24"/>
-      <c r="B18" s="19">
+    <row r="18" spans="1:20">
+      <c r="A18" s="49"/>
+      <c r="B18" s="17">
         <v>3</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
@@ -1962,7 +1705,7 @@
       <c r="J18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="29" t="s">
+      <c r="K18" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
@@ -1974,30 +1717,30 @@
       <c r="N18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O18" s="29" t="s">
+      <c r="O18" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R18" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S18" s="2">
+      <c r="P18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="52">
         <v>51.599499999999999</v>
       </c>
-      <c r="T18" s="12"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="24"/>
-      <c r="B19" s="19">
+      <c r="T18" s="11"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="49"/>
+      <c r="B19" s="17">
         <v>4</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="30" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="26" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="2">
@@ -2013,43 +1756,45 @@
       <c r="I19" s="2">
         <v>32</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="29" t="s">
+      <c r="K19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="25" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O19" s="29" t="s">
+      <c r="O19" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="12"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="24"/>
-      <c r="B20" s="19">
+      <c r="P19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" s="52">
+        <v>25.949000000000002</v>
+      </c>
+      <c r="T19" s="11"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="49"/>
+      <c r="B20" s="17">
         <v>5</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="31" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="27" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="2">
@@ -2065,43 +1810,45 @@
       <c r="I20" s="2">
         <v>32</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" s="29" t="s">
+      <c r="K20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="25" t="s">
         <v>50</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O20" s="29" t="s">
+      <c r="O20" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="12"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="24"/>
-      <c r="B21" s="19">
+      <c r="P20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="52">
+        <v>25.6374</v>
+      </c>
+      <c r="T20" s="11"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="49"/>
+      <c r="B21" s="17">
         <v>6</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="31" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="27" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="2">
@@ -2111,49 +1858,51 @@
         <v>100</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="32">
+      <c r="H21" s="28">
         <v>4</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="29">
         <v>32</v>
       </c>
-      <c r="J21" s="34" t="s">
+      <c r="J21" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="M21" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="N21" s="37" t="s">
+      <c r="K21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="38" t="s">
+      <c r="O21" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="P21" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="R21" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="12"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="24"/>
-      <c r="B22" s="19">
+      <c r="P21" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="52">
+        <v>22.849799999999998</v>
+      </c>
+      <c r="T21" s="11"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="49"/>
+      <c r="B22" s="17">
         <v>7</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="2">
@@ -2172,40 +1921,40 @@
       <c r="J22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="36" t="s">
+      <c r="K22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="M22" s="36" t="s">
+      <c r="M22" s="32" t="s">
         <v>46</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="29" t="s">
+      <c r="O22" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="12"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="24"/>
-      <c r="B23" s="19">
+      <c r="P22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="52"/>
+      <c r="T22" s="11"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="49"/>
+      <c r="B23" s="17">
         <v>8</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="29" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="25" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="2">
@@ -2221,42 +1970,42 @@
       <c r="I23" s="2">
         <v>32</v>
       </c>
-      <c r="J23" s="29" t="s">
+      <c r="J23" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" s="29" t="s">
+      <c r="K23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" s="25" t="s">
         <v>50</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O23" s="38" t="s">
+      <c r="O23" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="P23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S23" s="2"/>
-      <c r="T23" s="12"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="24"/>
-      <c r="B24" s="19">
+      <c r="P23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="52"/>
+      <c r="T23" s="11"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="49"/>
+      <c r="B24" s="17">
         <v>9</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="2" t="s">
         <v>55</v>
       </c>
@@ -2276,7 +2025,7 @@
       <c r="J24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K24" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -2288,27 +2037,27 @@
       <c r="N24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O24" s="38" t="s">
+      <c r="O24" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="P24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R24" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S24" s="2"/>
-      <c r="T24" s="12"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="19">
+      <c r="P24" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R24" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S24" s="52"/>
+      <c r="T24" s="11"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="49"/>
+      <c r="B25" s="17">
         <v>10</v>
       </c>
-      <c r="C25" s="11"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2328,39 +2077,39 @@
       <c r="J25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="42" t="b">
+      <c r="K25" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="L25" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="29" t="s">
+      <c r="L25" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="25" t="s">
         <v>50</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O25" s="29" t="s">
+      <c r="O25" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P25" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q25" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R25" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S25" s="2"/>
-      <c r="T25" s="12"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="24"/>
-      <c r="B26" s="19">
+      <c r="P25" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q25" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R25" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S25" s="52"/>
+      <c r="T25" s="11"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="49"/>
+      <c r="B26" s="17">
         <v>11</v>
       </c>
-      <c r="C26" s="11"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="2" t="s">
         <v>55</v>
       </c>
@@ -2380,7 +2129,7 @@
       <c r="J26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K26" s="29" t="s">
+      <c r="K26" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L26" s="2" t="s">
@@ -2392,27 +2141,27 @@
       <c r="N26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O26" s="29" t="s">
+      <c r="O26" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P26" s="39" t="s">
+      <c r="P26" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="Q26" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R26" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="2"/>
-      <c r="T26" s="12"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="24"/>
-      <c r="B27" s="19">
+      <c r="Q26" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26" s="52"/>
+      <c r="T26" s="11"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="49"/>
+      <c r="B27" s="17">
         <v>12</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="2" t="s">
         <v>55</v>
       </c>
@@ -2432,7 +2181,7 @@
       <c r="J27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L27" s="2" t="s">
@@ -2441,30 +2190,30 @@
       <c r="M27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="N27" s="25" t="s">
         <v>47</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P27" s="39" t="s">
+      <c r="P27" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="Q27" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R27" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S27" s="2"/>
-      <c r="T27" s="12"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="24"/>
-      <c r="B28" s="19">
+      <c r="Q27" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" s="52"/>
+      <c r="T27" s="11"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="49"/>
+      <c r="B28" s="17">
         <v>13</v>
       </c>
-      <c r="C28" s="11"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2484,7 +2233,7 @@
       <c r="J28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L28" s="2" t="s">
@@ -2493,30 +2242,30 @@
       <c r="M28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="43" t="s">
+      <c r="N28" s="39" t="s">
         <v>60</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P28" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R28" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S28" s="2"/>
-      <c r="T28" s="12"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="24"/>
-      <c r="B29" s="19">
+      <c r="P28" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q28" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28" s="52"/>
+      <c r="T28" s="11"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="49"/>
+      <c r="B29" s="17">
         <v>14</v>
       </c>
-      <c r="C29" s="11"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="2" t="s">
         <v>55</v>
       </c>
@@ -2536,7 +2285,7 @@
       <c r="J29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="29" t="s">
+      <c r="K29" s="25" t="s">
         <v>21</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -2545,30 +2294,30 @@
       <c r="M29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="29" t="s">
+      <c r="N29" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="O29" s="29" t="s">
+      <c r="O29" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="P29" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="44" t="b">
+      <c r="P29" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="R29" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="12"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="24"/>
-      <c r="B30" s="19">
+      <c r="R29" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29" s="52"/>
+      <c r="T29" s="11"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="49"/>
+      <c r="B30" s="17">
         <v>15</v>
       </c>
-      <c r="C30" s="11"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="2" t="s">
         <v>55</v>
       </c>
@@ -2603,24 +2352,24 @@
       <c r="O30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P30" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q30" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R30" s="45" t="b">
+      <c r="P30" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="R30" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="12"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="24"/>
-      <c r="B31" s="19">
+      <c r="S30" s="52"/>
+      <c r="T30" s="11"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="49"/>
+      <c r="B31" s="17">
         <v>16</v>
       </c>
-      <c r="C31" s="11"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="2" t="s">
         <v>55</v>
       </c>
@@ -2634,7 +2383,7 @@
       <c r="H31" s="2">
         <v>4</v>
       </c>
-      <c r="I31" s="33">
+      <c r="I31" s="29">
         <v>48</v>
       </c>
       <c r="J31" s="2" t="s">
@@ -2661,18 +2410,18 @@
       <c r="Q31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R31" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S31" s="2"/>
-      <c r="T31" s="12"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="24"/>
-      <c r="B32" s="19">
+      <c r="R31" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S31" s="52"/>
+      <c r="T31" s="11"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="49"/>
+      <c r="B32" s="17">
         <v>17</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
@@ -2689,7 +2438,7 @@
       <c r="I32" s="2">
         <v>32</v>
       </c>
-      <c r="J32" s="34" t="s">
+      <c r="J32" s="30" t="s">
         <v>22</v>
       </c>
       <c r="K32" s="2" t="s">
@@ -2713,18 +2462,18 @@
       <c r="Q32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S32" s="2"/>
-      <c r="T32" s="12"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="24"/>
-      <c r="B33" s="19">
+      <c r="R32" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" s="52"/>
+      <c r="T32" s="11"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="49"/>
+      <c r="B33" s="17">
         <v>18</v>
       </c>
-      <c r="C33" s="11"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="2" t="s">
         <v>55</v>
       </c>
@@ -2735,7 +2484,7 @@
         <v>100</v>
       </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="32">
+      <c r="H33" s="28">
         <v>6</v>
       </c>
       <c r="I33" s="2">
@@ -2768,18 +2517,18 @@
       <c r="R33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S33" s="2"/>
-      <c r="T33" s="12"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="24"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="11"/>
+      <c r="S33" s="52"/>
+      <c r="T33" s="11"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="49"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="46"/>
+      <c r="H34" s="42"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -2791,17 +2540,17 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
-      <c r="T34" s="12"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="24"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="11"/>
+      <c r="T34" s="11"/>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="49"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="46"/>
+      <c r="H35" s="42"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2813,77 +2562,76 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-      <c r="T35" s="12"/>
-    </row>
-    <row r="36" ht="15.75">
-      <c r="A36" s="26"/>
-      <c r="B36" s="47" t="s">
+      <c r="T35" s="11"/>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="50"/>
+      <c r="B36" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49">
+      <c r="C36" s="44"/>
+      <c r="D36" s="45">
         <v>3</v>
       </c>
-      <c r="E36" s="49">
+      <c r="E36" s="45">
         <v>1</v>
       </c>
-      <c r="F36" s="49">
+      <c r="F36" s="45">
         <v>1</v>
       </c>
-      <c r="G36" s="49">
+      <c r="G36" s="45">
         <v>1</v>
       </c>
-      <c r="H36" s="49">
+      <c r="H36" s="45">
         <v>2</v>
       </c>
-      <c r="I36" s="49">
+      <c r="I36" s="45">
         <v>2</v>
       </c>
-      <c r="J36" s="49">
+      <c r="J36" s="45">
         <v>2</v>
       </c>
-      <c r="K36" s="49">
+      <c r="K36" s="45">
         <v>2</v>
       </c>
-      <c r="L36" s="49">
+      <c r="L36" s="45">
         <v>2</v>
       </c>
-      <c r="M36" s="49">
+      <c r="M36" s="45">
         <v>1</v>
       </c>
-      <c r="N36" s="49">
+      <c r="N36" s="45">
         <v>2</v>
       </c>
-      <c r="O36" s="49">
+      <c r="O36" s="45">
         <v>3</v>
       </c>
-      <c r="P36" s="49">
+      <c r="P36" s="45">
         <v>2</v>
       </c>
-      <c r="Q36" s="49">
+      <c r="Q36" s="45">
         <v>2</v>
       </c>
-      <c r="R36" s="49">
+      <c r="R36" s="45">
         <v>2</v>
       </c>
-      <c r="S36" s="49"/>
-      <c r="T36" s="50">
+      <c r="S36" s="45"/>
+      <c r="T36" s="46">
         <f>PRODUCT(D36:R36)</f>
         <v>4608</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A16:A36"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A36"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="1"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Training 6_8_9_10 set up
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Julian\workspace\endolas\experiments\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Network</t>
   </si>
@@ -27,25 +21,25 @@
     <t>Training</t>
   </si>
   <si>
-    <t>Data Set</t>
-  </si>
-  <si>
-    <t>Train Size</t>
+    <t xml:space="preserve">Data Set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Train Size</t>
   </si>
   <si>
     <t>Epochs</t>
   </si>
   <si>
-    <t>Batch Size</t>
+    <t xml:space="preserve">Batch Size</t>
   </si>
   <si>
     <t>Depth</t>
   </si>
   <si>
-    <t>Feature Maps</t>
-  </si>
-  <si>
-    <t>Image Size</t>
+    <t xml:space="preserve">Feature Maps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image Size</t>
   </si>
   <si>
     <t>Augment</t>
@@ -69,10 +63,10 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t>Gap Filling</t>
-  </si>
-  <si>
-    <t>Score Value</t>
+    <t xml:space="preserve">Gap Filling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score Value</t>
   </si>
   <si>
     <t>Note</t>
@@ -96,13 +90,13 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t>No Dropout</t>
+    <t xml:space="preserve">No Dropout</t>
   </si>
   <si>
     <t>MAE</t>
   </si>
   <si>
-    <t>No Preprocessing</t>
+    <t xml:space="preserve">No Preprocessing</t>
   </si>
   <si>
     <t>2_segmentation</t>
@@ -114,7 +108,7 @@
     <t>LASTEN</t>
   </si>
   <si>
-    <t>384 x 384</t>
+    <t xml:space="preserve">384 x 384</t>
   </si>
   <si>
     <t>Dice</t>
@@ -153,7 +147,7 @@
     <t>SIMPLE</t>
   </si>
   <si>
-    <t>100 /250</t>
+    <t xml:space="preserve">100 /250</t>
   </si>
   <si>
     <t>224x224</t>
@@ -168,7 +162,7 @@
     <t>Fixed+Moving</t>
   </si>
   <si>
-    <t>Fixed and Moving Input</t>
+    <t xml:space="preserve">Fixed and Moving Input</t>
   </si>
   <si>
     <t>msed</t>
@@ -177,7 +171,7 @@
     <t>Moving</t>
   </si>
   <si>
-    <t>Moving Input</t>
+    <t xml:space="preserve">Moving Input</t>
   </si>
   <si>
     <t>SIMPLEA</t>
@@ -192,7 +186,13 @@
     <t>Moving+Fixed</t>
   </si>
   <si>
-    <t>Moving+Gradient</t>
+    <t>Moving+Diff</t>
+  </si>
+  <si>
+    <t>Moving+Diff+Gradient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gradient of Image</t>
   </si>
   <si>
     <t>L1</t>
@@ -210,17 +210,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <color indexed="64"/>
       <sz val="11"/>
-      <color indexed="64"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <name val="Arial Unicode MS"/>
+      <color indexed="64"/>
       <sz val="10"/>
-      <color indexed="64"/>
-      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="14">
@@ -296,12 +296,7 @@
         <bgColor rgb="FFE0EB4C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="1"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
+    <fill/>
   </fills>
   <borders count="26">
     <border>
@@ -600,175 +595,424 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="53">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="45">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -971,46 +1215,45 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMW36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="12.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="12.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
-    <col min="17" max="18" width="15.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="26.85546875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" style="1" customWidth="1"/>
-    <col min="23" max="24" width="8.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="15.42578125" style="1" customWidth="1"/>
-    <col min="27" max="1034" width="8.5703125" style="1" customWidth="1"/>
-    <col min="1035" max="1037" width="9.140625" style="1" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" style="1" width="22"/>
+    <col customWidth="1" min="2" max="2" style="1" width="11.328125"/>
+    <col customWidth="1" min="3" max="4" style="1" width="10.52734375"/>
+    <col customWidth="1" min="5" max="5" style="1" width="10.66796875"/>
+    <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
+    <col customWidth="1" min="7" max="8" style="1" width="12.328125"/>
+    <col customWidth="1" min="9" max="9" style="1" width="13.19921875"/>
+    <col customWidth="1" min="10" max="11" style="1" width="12.328125"/>
+    <col customWidth="1" min="12" max="12" style="1" width="8.8671875"/>
+    <col customWidth="1" min="13" max="13" style="1" width="7.9296875"/>
+    <col customWidth="1" min="14" max="14" style="1" width="11.57421875"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" style="1" width="19.3984375"/>
+    <col customWidth="1" min="16" max="16" style="1" width="13.7109375"/>
+    <col customWidth="1" min="17" max="18" style="1" width="15.7109375"/>
+    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="14.59765625"/>
+    <col customWidth="1" min="20" max="20" style="1" width="26.8515625"/>
+    <col customWidth="1" min="21" max="21" style="1" width="15.42578125"/>
+    <col customWidth="1" min="22" max="22" style="1" width="14.5703125"/>
+    <col customWidth="1" min="23" max="24" style="1" width="8.5703125"/>
+    <col customWidth="1" min="25" max="25" style="1" width="14.42578125"/>
+    <col customWidth="1" min="26" max="26" style="1" width="15.42578125"/>
+    <col customWidth="1" min="27" max="1034" style="1" width="8.5703125"/>
+    <col customWidth="1" min="1035" max="1037" style="1" width="9.140625"/>
+    <col min="1038" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1">
+    <row r="1" s="2" customFormat="1" ht="15.75">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1275,7 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -1050,30 +1293,30 @@
       <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="S1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="47" t="s">
+    <row r="2">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="9">
@@ -1116,8 +1359,8 @@
       <c r="S2" s="2"/>
       <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1">
-      <c r="A3" s="47"/>
+    <row r="3" s="1" customFormat="1">
+      <c r="A3" s="8"/>
       <c r="B3" s="12">
         <v>2</v>
       </c>
@@ -1160,8 +1403,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1">
-      <c r="A4" s="47"/>
+    <row r="4" s="1" customFormat="1">
+      <c r="A4" s="8"/>
       <c r="B4" s="12">
         <v>3</v>
       </c>
@@ -1204,8 +1447,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="47"/>
+    <row r="5" ht="15.75">
+      <c r="A5" s="8"/>
       <c r="B5" s="13">
         <v>4</v>
       </c>
@@ -1228,57 +1471,57 @@
       <c r="S5" s="15"/>
       <c r="T5" s="16"/>
     </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="48" t="s">
+    <row r="6" ht="15.75">
+      <c r="A6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="18">
         <v>1</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="20">
         <v>168</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="20">
         <v>300</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="20">
         <v>8</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19">
+      <c r="H6" s="20"/>
+      <c r="I6" s="20">
         <v>32</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="19" t="b">
+      <c r="K6" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="19" t="s">
+      <c r="M6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="20" t="s">
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="21"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="49"/>
-      <c r="B7" s="17">
+      <c r="T6" s="22"/>
+    </row>
+    <row r="7" ht="15.75">
+      <c r="A7" s="23"/>
+      <c r="B7" s="18">
         <v>2</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1317,14 +1560,14 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="22" t="s">
+      <c r="S7" s="24" t="s">
         <v>35</v>
       </c>
       <c r="T7" s="11"/>
     </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="49"/>
-      <c r="B8" s="17">
+    <row r="8" ht="15.75">
+      <c r="A8" s="23"/>
+      <c r="B8" s="18">
         <v>3</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1363,14 +1606,14 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="22" t="s">
+      <c r="S8" s="24" t="s">
         <v>37</v>
       </c>
       <c r="T8" s="11"/>
     </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="50"/>
-      <c r="B9" s="23">
+    <row r="9" ht="15.75">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26">
         <v>4</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -1414,35 +1657,35 @@
       </c>
       <c r="T9" s="16"/>
     </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="48" t="s">
+    <row r="10">
+      <c r="A10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="18">
         <v>1</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="21"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="50"/>
-      <c r="B11" s="23">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="22"/>
+    </row>
+    <row r="11" ht="15.75">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26">
         <v>2</v>
       </c>
       <c r="C11" s="14"/>
@@ -1464,35 +1707,35 @@
       <c r="S11" s="15"/>
       <c r="T11" s="16"/>
     </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="48" t="s">
+    <row r="12">
+      <c r="A12" s="17" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="21"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="50"/>
-      <c r="B13" s="23">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="22"/>
+    </row>
+    <row r="13" ht="15.75">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26">
         <v>2</v>
       </c>
       <c r="C13" s="14"/>
@@ -1514,35 +1757,35 @@
       <c r="S13" s="15"/>
       <c r="T13" s="16"/>
     </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="48" t="s">
+    <row r="14">
+      <c r="A14" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="21"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="50"/>
-      <c r="B15" s="23">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="22"/>
+    </row>
+    <row r="15" ht="15.75">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26">
         <v>2</v>
       </c>
       <c r="C15" s="14"/>
@@ -1564,67 +1807,67 @@
       <c r="S15" s="15"/>
       <c r="T15" s="16"/>
     </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="49" t="s">
+    <row r="16">
+      <c r="A16" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="18">
         <v>1</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="20">
         <v>1</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="20">
         <v>1</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="20">
         <v>4</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="20">
         <v>32</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="19" t="s">
+      <c r="K16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="20" t="s">
         <v>46</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="24" t="s">
+      <c r="O16" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="P16" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="51"/>
-      <c r="T16" s="21" t="s">
+      <c r="P16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="20"/>
+      <c r="T16" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="49"/>
-      <c r="B17" s="17">
+    <row r="17">
+      <c r="A17" s="23"/>
+      <c r="B17" s="18">
         <v>2</v>
       </c>
       <c r="C17" s="10"/>
@@ -1649,7 +1892,7 @@
       <c r="J17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="K17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="2" t="s">
@@ -1661,26 +1904,26 @@
       <c r="N17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O17" s="25" t="s">
+      <c r="O17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P17" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R17" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S17" s="52"/>
+      <c r="P17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="2"/>
       <c r="T17" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="49"/>
-      <c r="B18" s="17">
+    <row r="18">
+      <c r="A18" s="23"/>
+      <c r="B18" s="18">
         <v>3</v>
       </c>
       <c r="C18" s="10"/>
@@ -1705,7 +1948,7 @@
       <c r="J18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="K18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L18" s="2" t="s">
@@ -1717,30 +1960,30 @@
       <c r="N18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O18" s="25" t="s">
+      <c r="O18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q18" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R18" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S18" s="52">
+      <c r="P18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="2">
         <v>51.599499999999999</v>
       </c>
       <c r="T18" s="11"/>
     </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="49"/>
-      <c r="B19" s="17">
+    <row r="19">
+      <c r="A19" s="23"/>
+      <c r="B19" s="18">
         <v>4</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="27" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="2">
@@ -1756,41 +1999,39 @@
       <c r="I19" s="2">
         <v>32</v>
       </c>
-      <c r="J19" s="25" t="s">
+      <c r="J19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K19" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M19" s="25" t="s">
+      <c r="K19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M19" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O19" s="25" t="s">
+      <c r="O19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P19" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q19" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R19" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S19" s="52">
-        <v>25.949000000000002</v>
-      </c>
+      <c r="P19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" s="2"/>
       <c r="T19" s="11"/>
     </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="49"/>
-      <c r="B20" s="17">
+    <row r="20">
+      <c r="A20" s="23"/>
+      <c r="B20" s="18">
         <v>5</v>
       </c>
       <c r="C20" s="10"/>
@@ -1810,41 +2051,39 @@
       <c r="I20" s="2">
         <v>32</v>
       </c>
-      <c r="J20" s="25" t="s">
+      <c r="J20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M20" s="25" t="s">
+      <c r="K20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M20" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O20" s="25" t="s">
+      <c r="O20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R20" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="52">
-        <v>25.6374</v>
-      </c>
+      <c r="P20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="2"/>
       <c r="T20" s="11"/>
     </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="49"/>
-      <c r="B21" s="17">
+    <row r="21">
+      <c r="A21" s="23"/>
+      <c r="B21" s="18">
         <v>6</v>
       </c>
       <c r="C21" s="10"/>
@@ -1891,18 +2130,16 @@
       <c r="R21" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="S21" s="52">
-        <v>22.849799999999998</v>
-      </c>
+      <c r="S21" s="2"/>
       <c r="T21" s="11"/>
     </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="49"/>
-      <c r="B22" s="17">
+    <row r="22">
+      <c r="A22" s="23"/>
+      <c r="B22" s="18">
         <v>7</v>
       </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="2">
@@ -1921,7 +2158,7 @@
       <c r="J22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="25" t="s">
+      <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L22" s="32" t="s">
@@ -1933,28 +2170,28 @@
       <c r="N22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="25" t="s">
+      <c r="O22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P22" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R22" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="52"/>
+      <c r="P22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="2"/>
       <c r="T22" s="11"/>
     </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="49"/>
-      <c r="B23" s="17">
+    <row r="23">
+      <c r="A23" s="23"/>
+      <c r="B23" s="18">
         <v>8</v>
       </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="2" t="s">
         <v>55</v>
       </c>
       <c r="E23" s="2">
@@ -1970,16 +2207,16 @@
       <c r="I23" s="2">
         <v>32</v>
       </c>
-      <c r="J23" s="25" t="s">
+      <c r="J23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M23" s="25" t="s">
+      <c r="K23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M23" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N23" s="2" t="s">
@@ -1988,21 +2225,21 @@
       <c r="O23" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="P23" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q23" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R23" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S23" s="52"/>
+      <c r="P23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="2"/>
       <c r="T23" s="11"/>
     </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="49"/>
-      <c r="B24" s="17">
+    <row r="24">
+      <c r="A24" s="23"/>
+      <c r="B24" s="18">
         <v>9</v>
       </c>
       <c r="C24" s="10"/>
@@ -2025,7 +2262,7 @@
       <c r="J24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K24" s="25" t="s">
+      <c r="K24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L24" s="2" t="s">
@@ -2040,21 +2277,15 @@
       <c r="O24" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="P24" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q24" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R24" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S24" s="52"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
       <c r="T24" s="11"/>
     </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="49"/>
-      <c r="B25" s="17">
+    <row r="25">
+      <c r="A25" s="23"/>
+      <c r="B25" s="18">
         <v>10</v>
       </c>
       <c r="C25" s="10"/>
@@ -2077,36 +2308,32 @@
       <c r="J25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K25" s="38" t="b">
-        <v>1</v>
-      </c>
-      <c r="L25" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="25" t="s">
+      <c r="K25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M25" s="2" t="s">
         <v>50</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O25" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="P25" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q25" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R25" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S25" s="52"/>
-      <c r="T25" s="11"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="49"/>
-      <c r="B26" s="17">
+      <c r="O25" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="23"/>
+      <c r="B26" s="18">
         <v>11</v>
       </c>
       <c r="C26" s="10"/>
@@ -2129,8 +2356,8 @@
       <c r="J26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K26" s="25" t="s">
-        <v>21</v>
+      <c r="K26" s="31" t="b">
+        <v>1</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>50</v>
@@ -2141,24 +2368,24 @@
       <c r="N26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O26" s="25" t="s">
+      <c r="O26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P26" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q26" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R26" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="52"/>
+      <c r="P26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26" s="2"/>
       <c r="T26" s="11"/>
     </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="49"/>
-      <c r="B27" s="17">
+    <row r="27">
+      <c r="A27" s="23"/>
+      <c r="B27" s="18">
         <v>12</v>
       </c>
       <c r="C27" s="10"/>
@@ -2181,7 +2408,7 @@
       <c r="J27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="25" t="s">
+      <c r="K27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L27" s="2" t="s">
@@ -2190,27 +2417,27 @@
       <c r="M27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="25" t="s">
+      <c r="N27" s="2" t="s">
         <v>47</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="P27" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q27" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R27" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S27" s="52"/>
+        <v>60</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" s="2"/>
       <c r="T27" s="11"/>
     </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="49"/>
-      <c r="B28" s="17">
+    <row r="28">
+      <c r="A28" s="23"/>
+      <c r="B28" s="18">
         <v>13</v>
       </c>
       <c r="C28" s="10"/>
@@ -2233,7 +2460,7 @@
       <c r="J28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="25" t="s">
+      <c r="K28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L28" s="2" t="s">
@@ -2242,27 +2469,27 @@
       <c r="M28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="39" t="s">
-        <v>60</v>
+      <c r="N28" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P28" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q28" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R28" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S28" s="52"/>
+      <c r="P28" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28" s="2"/>
       <c r="T28" s="11"/>
     </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="49"/>
-      <c r="B29" s="17">
+    <row r="29">
+      <c r="A29" s="23"/>
+      <c r="B29" s="18">
         <v>14</v>
       </c>
       <c r="C29" s="10"/>
@@ -2285,7 +2512,7 @@
       <c r="J29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K29" s="25" t="s">
+      <c r="K29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="L29" s="2" t="s">
@@ -2294,27 +2521,27 @@
       <c r="M29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="O29" s="25" t="s">
+      <c r="N29" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P29" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q29" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="R29" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S29" s="52"/>
+      <c r="P29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29" s="2"/>
       <c r="T29" s="11"/>
     </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="49"/>
-      <c r="B30" s="17">
+    <row r="30">
+      <c r="A30" s="23"/>
+      <c r="B30" s="18">
         <v>15</v>
       </c>
       <c r="C30" s="10"/>
@@ -2352,21 +2579,21 @@
       <c r="O30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P30" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q30" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="R30" s="41" t="b">
+      <c r="P30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q30" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="S30" s="52"/>
+      <c r="R30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S30" s="2"/>
       <c r="T30" s="11"/>
     </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="49"/>
-      <c r="B31" s="17">
+    <row r="31">
+      <c r="A31" s="23"/>
+      <c r="B31" s="18">
         <v>16</v>
       </c>
       <c r="C31" s="10"/>
@@ -2383,8 +2610,8 @@
       <c r="H31" s="2">
         <v>4</v>
       </c>
-      <c r="I31" s="29">
-        <v>48</v>
+      <c r="I31" s="2">
+        <v>32</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>45</v>
@@ -2410,15 +2637,15 @@
       <c r="Q31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R31" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S31" s="52"/>
+      <c r="R31" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="S31" s="2"/>
       <c r="T31" s="11"/>
     </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="49"/>
-      <c r="B32" s="17">
+    <row r="32">
+      <c r="A32" s="23"/>
+      <c r="B32" s="18">
         <v>17</v>
       </c>
       <c r="C32" s="10"/>
@@ -2435,11 +2662,11 @@
       <c r="H32" s="2">
         <v>4</v>
       </c>
-      <c r="I32" s="2">
-        <v>32</v>
-      </c>
-      <c r="J32" s="30" t="s">
-        <v>22</v>
+      <c r="I32" s="29">
+        <v>48</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>21</v>
@@ -2462,15 +2689,15 @@
       <c r="Q32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="S32" s="52"/>
+      <c r="R32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" s="2"/>
       <c r="T32" s="11"/>
     </row>
-    <row r="33" spans="1:20">
-      <c r="A33" s="49"/>
-      <c r="B33" s="17">
+    <row r="33">
+      <c r="A33" s="23"/>
+      <c r="B33" s="18">
         <v>18</v>
       </c>
       <c r="C33" s="10"/>
@@ -2484,14 +2711,14 @@
         <v>100</v>
       </c>
       <c r="G33" s="2"/>
-      <c r="H33" s="28">
-        <v>6</v>
+      <c r="H33" s="2">
+        <v>4</v>
       </c>
       <c r="I33" s="2">
         <v>32</v>
       </c>
-      <c r="J33" s="2" t="s">
-        <v>45</v>
+      <c r="J33" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>21</v>
@@ -2517,40 +2744,70 @@
       <c r="R33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S33" s="52"/>
+      <c r="S33" s="2"/>
       <c r="T33" s="11"/>
     </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="49"/>
-      <c r="B34" s="17"/>
+    <row r="34">
+      <c r="A34" s="23"/>
+      <c r="B34" s="18">
+        <v>19</v>
+      </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3360</v>
+      </c>
+      <c r="F34" s="2">
+        <v>100</v>
+      </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
+      <c r="H34" s="28">
+        <v>6</v>
+      </c>
+      <c r="I34" s="2">
+        <v>32</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S34" s="2"/>
       <c r="T34" s="11"/>
     </row>
-    <row r="35" spans="1:20">
-      <c r="A35" s="49"/>
-      <c r="B35" s="17"/>
+    <row r="35">
+      <c r="A35" s="23"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="10"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="42"/>
+      <c r="H35" s="40"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2564,74 +2821,101 @@
       <c r="S35" s="2"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36" spans="1:20">
-      <c r="A36" s="50"/>
-      <c r="B36" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45">
+    <row r="36">
+      <c r="A36" s="23"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="11"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="23"/>
+      <c r="B37" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="43">
         <v>3</v>
       </c>
-      <c r="E36" s="45">
+      <c r="E37" s="43">
         <v>1</v>
       </c>
-      <c r="F36" s="45">
+      <c r="F37" s="43">
         <v>1</v>
       </c>
-      <c r="G36" s="45">
+      <c r="G37" s="43">
         <v>1</v>
       </c>
-      <c r="H36" s="45">
+      <c r="H37" s="43">
         <v>2</v>
       </c>
-      <c r="I36" s="45">
+      <c r="I37" s="43">
         <v>2</v>
       </c>
-      <c r="J36" s="45">
+      <c r="J37" s="43">
         <v>2</v>
       </c>
-      <c r="K36" s="45">
+      <c r="K37" s="43">
         <v>2</v>
       </c>
-      <c r="L36" s="45">
+      <c r="L37" s="43">
         <v>2</v>
       </c>
-      <c r="M36" s="45">
+      <c r="M37" s="43">
         <v>1</v>
       </c>
-      <c r="N36" s="45">
+      <c r="N37" s="43">
         <v>2</v>
       </c>
-      <c r="O36" s="45">
+      <c r="O37" s="43">
         <v>3</v>
       </c>
-      <c r="P36" s="45">
+      <c r="P37" s="43">
         <v>2</v>
       </c>
-      <c r="Q36" s="45">
+      <c r="Q37" s="43">
         <v>2</v>
       </c>
-      <c r="R36" s="45">
+      <c r="R37" s="43">
         <v>2</v>
       </c>
-      <c r="S36" s="45"/>
-      <c r="T36" s="46">
-        <f>PRODUCT(D36:R36)</f>
+      <c r="S37" s="43"/>
+      <c r="T37" s="44">
+        <f>PRODUCT(D37:R37)</f>
         <v>4608</v>
       </c>
+    </row>
+    <row r="38" ht="15.75">
+      <c r="A38" s="25"/>
+      <c r="T38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A16:A36"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A38"/>
   </mergeCells>
-  <printOptions gridLines="1"/>
+  <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adaption made to rerun training 9 and 10
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Julian\workspace\endolas\experiments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="64">
   <si>
     <t>Network</t>
   </si>
@@ -21,25 +27,25 @@
     <t>Training</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train Size</t>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Train Size</t>
   </si>
   <si>
     <t>Epochs</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch Size</t>
+    <t>Batch Size</t>
   </si>
   <si>
     <t>Depth</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature Maps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Size</t>
+    <t>Feature Maps</t>
+  </si>
+  <si>
+    <t>Image Size</t>
   </si>
   <si>
     <t>Augment</t>
@@ -63,10 +69,10 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t xml:space="preserve">Gap Filling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score Value</t>
+    <t>Gap Filling</t>
+  </si>
+  <si>
+    <t>Score Value</t>
   </si>
   <si>
     <t>Note</t>
@@ -90,13 +96,13 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Dropout</t>
+    <t>No Dropout</t>
   </si>
   <si>
     <t>MAE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Preprocessing</t>
+    <t>No Preprocessing</t>
   </si>
   <si>
     <t>2_segmentation</t>
@@ -108,7 +114,7 @@
     <t>LASTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">384 x 384</t>
+    <t>384 x 384</t>
   </si>
   <si>
     <t>Dice</t>
@@ -147,7 +153,7 @@
     <t>SIMPLE</t>
   </si>
   <si>
-    <t xml:space="preserve">100 /250</t>
+    <t>100 /250</t>
   </si>
   <si>
     <t>224x224</t>
@@ -162,7 +168,7 @@
     <t>Fixed+Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed and Moving Input</t>
+    <t>Fixed and Moving Input</t>
   </si>
   <si>
     <t>msed</t>
@@ -171,7 +177,7 @@
     <t>Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Moving Input</t>
+    <t>Moving Input</t>
   </si>
   <si>
     <t>SIMPLEA</t>
@@ -192,7 +198,7 @@
     <t>Moving+Diff+Gradient</t>
   </si>
   <si>
-    <t xml:space="preserve">Gradient of Image</t>
+    <t>Gradient of Image</t>
   </si>
   <si>
     <t>L1</t>
@@ -210,17 +216,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="64"/>
       <name val="Arial Unicode MS"/>
-      <color indexed="64"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="14">
@@ -296,7 +302,12 @@
         <bgColor rgb="FFE0EB4C"/>
       </patternFill>
     </fill>
-    <fill/>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor auto="1"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -595,424 +606,149 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1215,45 +951,46 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMW38"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="M10" activeCellId="0" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="22"/>
-    <col customWidth="1" min="2" max="2" style="1" width="11.328125"/>
-    <col customWidth="1" min="3" max="4" style="1" width="10.52734375"/>
-    <col customWidth="1" min="5" max="5" style="1" width="10.66796875"/>
-    <col customWidth="1" min="6" max="6" style="1" width="9.19921875"/>
-    <col customWidth="1" min="7" max="8" style="1" width="12.328125"/>
-    <col customWidth="1" min="9" max="9" style="1" width="13.19921875"/>
-    <col customWidth="1" min="10" max="11" style="1" width="12.328125"/>
-    <col customWidth="1" min="12" max="12" style="1" width="8.8671875"/>
-    <col customWidth="1" min="13" max="13" style="1" width="7.9296875"/>
-    <col customWidth="1" min="14" max="14" style="1" width="11.57421875"/>
-    <col bestFit="1" customWidth="1" min="15" max="15" style="1" width="19.3984375"/>
-    <col customWidth="1" min="16" max="16" style="1" width="13.7109375"/>
-    <col customWidth="1" min="17" max="18" style="1" width="15.7109375"/>
-    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="14.59765625"/>
-    <col customWidth="1" min="20" max="20" style="1" width="26.8515625"/>
-    <col customWidth="1" min="21" max="21" style="1" width="15.42578125"/>
-    <col customWidth="1" min="22" max="22" style="1" width="14.5703125"/>
-    <col customWidth="1" min="23" max="24" style="1" width="8.5703125"/>
-    <col customWidth="1" min="25" max="25" style="1" width="14.42578125"/>
-    <col customWidth="1" min="26" max="26" style="1" width="15.42578125"/>
-    <col customWidth="1" min="27" max="1034" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1035" max="1037" style="1" width="9.140625"/>
-    <col min="1038" max="16384" width="9.140625"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="8.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" style="1" customWidth="1"/>
+    <col min="27" max="1034" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1035" max="1037" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="15.75">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1315,14 +1052,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2"/>
@@ -1357,14 +1094,14 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" s="1" customFormat="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12">
+      <c r="T2" s="10"/>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1">
+      <c r="A3" s="41"/>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="2"/>
@@ -1399,16 +1136,16 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12">
+    <row r="4" spans="1:20" s="1" customFormat="1">
+      <c r="A4" s="41"/>
+      <c r="B4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2"/>
@@ -1443,88 +1180,88 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" ht="15.75">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
+    <row r="5" spans="1:20">
+      <c r="A5" s="41"/>
+      <c r="B5" s="12">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" ht="15.75">
-      <c r="A6" s="17" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="18">
-        <v>1</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>168</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <v>300</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <v>8</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18">
         <v>32</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="20" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" s="20" t="s">
+      <c r="K6" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="21" t="s">
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" ht="15.75">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18">
+      <c r="T6" s="20"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="43"/>
+      <c r="B7" s="16">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1560,17 +1297,17 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18">
+      <c r="T7" s="10"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="43"/>
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1606,271 +1343,271 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="24" t="s">
+      <c r="S8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9" ht="15.75">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26">
+      <c r="T8" s="10"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="44"/>
+      <c r="B9" s="22">
         <v>4</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>168</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>300</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>2</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
         <v>48</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L9" s="15" t="s">
+      <c r="K9" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="T9" s="15"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="18">
-        <v>1</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="22"/>
-    </row>
-    <row r="11" ht="15.75">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26">
+      <c r="B10" s="16">
+        <v>1</v>
+      </c>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="20"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="44"/>
+      <c r="B11" s="22">
         <v>2</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="15"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="42" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13" ht="15.75">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26">
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="20"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="44"/>
+      <c r="B13" s="22">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="15"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="42" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15" ht="15.75">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26">
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="20"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="44"/>
+      <c r="B15" s="22">
         <v>2</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="23" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="15"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="18">
-        <v>1</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20" t="s">
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="20">
-        <v>1</v>
-      </c>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="18">
+        <v>1</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="20">
-        <v>1</v>
-      </c>
-      <c r="H16" s="20">
+      <c r="G16" s="18">
+        <v>1</v>
+      </c>
+      <c r="H16" s="18">
         <v>4</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="18">
         <v>32</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="20" t="s">
+      <c r="K16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="18" t="s">
         <v>46</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="P16" s="20" t="s">
+      <c r="P16" s="18" t="s">
         <v>21</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="20"/>
-      <c r="T16" s="22" t="s">
+      <c r="R16" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="18"/>
+      <c r="T16" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="23"/>
-      <c r="B17" s="18">
+    <row r="17" spans="1:20">
+      <c r="A17" s="43"/>
+      <c r="B17" s="16">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1917,16 +1654,16 @@
         <v>21</v>
       </c>
       <c r="S17" s="2"/>
-      <c r="T17" s="11" t="s">
+      <c r="T17" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="23"/>
-      <c r="B18" s="18">
+    <row r="18" spans="1:20">
+      <c r="A18" s="43"/>
+      <c r="B18" s="16">
         <v>3</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="2" t="s">
         <v>53</v>
       </c>
@@ -1975,15 +1712,15 @@
       <c r="S18" s="2">
         <v>51.599499999999999</v>
       </c>
-      <c r="T18" s="11"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="23"/>
-      <c r="B19" s="18">
+      <c r="T18" s="10"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="43"/>
+      <c r="B19" s="16">
         <v>4</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="23" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="2">
@@ -2027,15 +1764,15 @@
         <v>21</v>
       </c>
       <c r="S19" s="2"/>
-      <c r="T19" s="11"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="23"/>
-      <c r="B20" s="18">
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="43"/>
+      <c r="B20" s="16">
         <v>5</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="27" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="23" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="2">
@@ -2079,15 +1816,15 @@
         <v>21</v>
       </c>
       <c r="S20" s="2"/>
-      <c r="T20" s="11"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="23"/>
-      <c r="B21" s="18">
+      <c r="T20" s="10"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="43"/>
+      <c r="B21" s="16">
         <v>6</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="27" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="23" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="2">
@@ -2097,48 +1834,48 @@
         <v>100</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="28">
+      <c r="H21" s="24">
         <v>4</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="25">
         <v>32</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="K21" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="M21" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="N21" s="33" t="s">
+      <c r="K21" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="M21" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="N21" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="34" t="s">
+      <c r="O21" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="P21" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="R21" s="37" t="s">
+      <c r="P21" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="33" t="s">
         <v>21</v>
       </c>
       <c r="S21" s="2"/>
-      <c r="T21" s="11"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="23"/>
-      <c r="B22" s="18">
+      <c r="T21" s="10"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="43"/>
+      <c r="B22" s="16">
         <v>7</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
@@ -2161,10 +1898,10 @@
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="32" t="s">
+      <c r="L22" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="M22" s="32" t="s">
+      <c r="M22" s="28" t="s">
         <v>46</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -2183,14 +1920,14 @@
         <v>21</v>
       </c>
       <c r="S22" s="2"/>
-      <c r="T22" s="11"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="23"/>
-      <c r="B23" s="18">
+      <c r="T22" s="10"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="43"/>
+      <c r="B23" s="16">
         <v>8</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="2" t="s">
         <v>55</v>
       </c>
@@ -2222,7 +1959,7 @@
       <c r="N23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O23" s="34" t="s">
+      <c r="O23" s="30" t="s">
         <v>56</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2235,14 +1972,14 @@
         <v>21</v>
       </c>
       <c r="S23" s="2"/>
-      <c r="T23" s="11"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="23"/>
-      <c r="B24" s="18">
+      <c r="T23" s="10"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="43"/>
+      <c r="B24" s="16">
         <v>9</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="2" t="s">
         <v>55</v>
       </c>
@@ -2274,21 +2011,21 @@
       <c r="N24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O24" s="34" t="s">
+      <c r="O24" s="30" t="s">
         <v>57</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
-      <c r="T24" s="11"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="18">
+      <c r="T24" s="10"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="43"/>
+      <c r="B25" s="16">
         <v>10</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="2" t="s">
         <v>55</v>
       </c>
@@ -2320,23 +2057,23 @@
       <c r="N25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O25" s="38" t="s">
+      <c r="O25" s="34" t="s">
         <v>58</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-      <c r="T25" s="39" t="s">
+      <c r="T25" s="35" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="23"/>
-      <c r="B26" s="18">
+    <row r="26" spans="1:20">
+      <c r="A26" s="43"/>
+      <c r="B26" s="16">
         <v>11</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="2" t="s">
         <v>55</v>
       </c>
@@ -2356,7 +2093,7 @@
       <c r="J26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K26" s="31" t="b">
+      <c r="K26" s="27" t="b">
         <v>1</v>
       </c>
       <c r="L26" s="2" t="s">
@@ -2381,14 +2118,14 @@
         <v>21</v>
       </c>
       <c r="S26" s="2"/>
-      <c r="T26" s="11"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="23"/>
-      <c r="B27" s="18">
+      <c r="T26" s="10"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="43"/>
+      <c r="B27" s="16">
         <v>12</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="2" t="s">
         <v>55</v>
       </c>
@@ -2423,7 +2160,7 @@
       <c r="O27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P27" s="35" t="s">
+      <c r="P27" s="31" t="s">
         <v>60</v>
       </c>
       <c r="Q27" s="2" t="s">
@@ -2433,14 +2170,14 @@
         <v>21</v>
       </c>
       <c r="S27" s="2"/>
-      <c r="T27" s="11"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="23"/>
-      <c r="B28" s="18">
+      <c r="T27" s="10"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="43"/>
+      <c r="B28" s="16">
         <v>13</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="2" t="s">
         <v>55</v>
       </c>
@@ -2475,7 +2212,7 @@
       <c r="O28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P28" s="35" t="s">
+      <c r="P28" s="31" t="s">
         <v>61</v>
       </c>
       <c r="Q28" s="2" t="s">
@@ -2485,14 +2222,14 @@
         <v>21</v>
       </c>
       <c r="S28" s="2"/>
-      <c r="T28" s="11"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="23"/>
-      <c r="B29" s="18">
+      <c r="T28" s="10"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="43"/>
+      <c r="B29" s="16">
         <v>14</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="2" t="s">
         <v>55</v>
       </c>
@@ -2504,7 +2241,7 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I29" s="2">
         <v>32</v>
@@ -2521,7 +2258,7 @@
       <c r="M29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="33" t="s">
+      <c r="N29" s="29" t="s">
         <v>62</v>
       </c>
       <c r="O29" s="2" t="s">
@@ -2537,14 +2274,14 @@
         <v>21</v>
       </c>
       <c r="S29" s="2"/>
-      <c r="T29" s="11"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="23"/>
-      <c r="B30" s="18">
+      <c r="T29" s="10"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="43"/>
+      <c r="B30" s="16">
         <v>15</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="2" t="s">
         <v>55</v>
       </c>
@@ -2582,21 +2319,21 @@
       <c r="P30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q30" s="36" t="b">
+      <c r="Q30" s="32" t="b">
         <v>1</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>21</v>
       </c>
       <c r="S30" s="2"/>
-      <c r="T30" s="11"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="23"/>
-      <c r="B31" s="18">
+      <c r="T30" s="10"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="43"/>
+      <c r="B31" s="16">
         <v>16</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="2" t="s">
         <v>55</v>
       </c>
@@ -2637,18 +2374,18 @@
       <c r="Q31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R31" s="37" t="b">
+      <c r="R31" s="33" t="b">
         <v>1</v>
       </c>
       <c r="S31" s="2"/>
-      <c r="T31" s="11"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="23"/>
-      <c r="B32" s="18">
+      <c r="T31" s="10"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="43"/>
+      <c r="B32" s="16">
         <v>17</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="2" t="s">
         <v>55</v>
       </c>
@@ -2662,7 +2399,7 @@
       <c r="H32" s="2">
         <v>4</v>
       </c>
-      <c r="I32" s="29">
+      <c r="I32" s="25">
         <v>48</v>
       </c>
       <c r="J32" s="2" t="s">
@@ -2693,14 +2430,14 @@
         <v>21</v>
       </c>
       <c r="S32" s="2"/>
-      <c r="T32" s="11"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="23"/>
-      <c r="B33" s="18">
+      <c r="T32" s="10"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="43"/>
+      <c r="B33" s="16">
         <v>18</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="2" t="s">
         <v>55</v>
       </c>
@@ -2717,7 +2454,7 @@
       <c r="I33" s="2">
         <v>32</v>
       </c>
-      <c r="J33" s="30" t="s">
+      <c r="J33" s="26" t="s">
         <v>22</v>
       </c>
       <c r="K33" s="2" t="s">
@@ -2745,14 +2482,14 @@
         <v>21</v>
       </c>
       <c r="S33" s="2"/>
-      <c r="T33" s="11"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="23"/>
-      <c r="B34" s="18">
+      <c r="T33" s="10"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="43"/>
+      <c r="B34" s="16">
         <v>19</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="2" t="s">
         <v>55</v>
       </c>
@@ -2763,7 +2500,7 @@
         <v>100</v>
       </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="28">
+      <c r="H34" s="24">
         <v>6</v>
       </c>
       <c r="I34" s="2">
@@ -2797,17 +2534,17 @@
         <v>21</v>
       </c>
       <c r="S34" s="2"/>
-      <c r="T34" s="11"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="23"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="10"/>
+      <c r="T34" s="10"/>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="43"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="9"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="40"/>
+      <c r="H35" s="36"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
@@ -2819,17 +2556,17 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-      <c r="T35" s="11"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="23"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="10"/>
+      <c r="T35" s="10"/>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="43"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="40"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
@@ -2841,81 +2578,79 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
-      <c r="T36" s="11"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="23"/>
-      <c r="B37" s="41" t="s">
+      <c r="T36" s="10"/>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="43"/>
+      <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43">
+      <c r="C37" s="38"/>
+      <c r="D37" s="39">
         <v>3</v>
       </c>
-      <c r="E37" s="43">
-        <v>1</v>
-      </c>
-      <c r="F37" s="43">
-        <v>1</v>
-      </c>
-      <c r="G37" s="43">
-        <v>1</v>
-      </c>
-      <c r="H37" s="43">
+      <c r="E37" s="39">
+        <v>1</v>
+      </c>
+      <c r="F37" s="39">
+        <v>1</v>
+      </c>
+      <c r="G37" s="39">
+        <v>1</v>
+      </c>
+      <c r="H37" s="39">
         <v>2</v>
       </c>
-      <c r="I37" s="43">
+      <c r="I37" s="39">
         <v>2</v>
       </c>
-      <c r="J37" s="43">
+      <c r="J37" s="39">
         <v>2</v>
       </c>
-      <c r="K37" s="43">
+      <c r="K37" s="39">
         <v>2</v>
       </c>
-      <c r="L37" s="43">
+      <c r="L37" s="39">
         <v>2</v>
       </c>
-      <c r="M37" s="43">
-        <v>1</v>
-      </c>
-      <c r="N37" s="43">
+      <c r="M37" s="39">
+        <v>1</v>
+      </c>
+      <c r="N37" s="39">
         <v>2</v>
       </c>
-      <c r="O37" s="43">
+      <c r="O37" s="39">
         <v>3</v>
       </c>
-      <c r="P37" s="43">
+      <c r="P37" s="39">
         <v>2</v>
       </c>
-      <c r="Q37" s="43">
+      <c r="Q37" s="39">
         <v>2</v>
       </c>
-      <c r="R37" s="43">
+      <c r="R37" s="39">
         <v>2</v>
       </c>
-      <c r="S37" s="43"/>
-      <c r="T37" s="44">
+      <c r="S37" s="39"/>
+      <c r="T37" s="40">
         <f>PRODUCT(D37:R37)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="38" ht="15.75">
-      <c r="A38" s="25"/>
-      <c r="T38" s="1"/>
+    <row r="38" spans="1:20">
+      <c r="A38" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A16:A38"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A38"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="1"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Training 6_10 to 6_13 ran
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="65">
   <si>
     <t>Network</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Possibilities</t>
+  </si>
+  <si>
+    <t>0.01 LR, 0.99 Momentum</t>
   </si>
 </sst>
 </file>
@@ -229,7 +232,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +311,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -608,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -718,17 +727,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMW38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1053,7 +1065,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="8">
@@ -1097,7 +1109,7 @@
       <c r="T2" s="10"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1">
-      <c r="A3" s="41"/>
+      <c r="A3" s="43"/>
       <c r="B3" s="11">
         <v>2</v>
       </c>
@@ -1141,7 +1153,7 @@
       </c>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1">
-      <c r="A4" s="41"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="11">
         <v>3</v>
       </c>
@@ -1185,7 +1197,7 @@
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="41"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="12">
         <v>4</v>
       </c>
@@ -1209,7 +1221,7 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="44" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="16">
@@ -1257,7 +1269,7 @@
       <c r="T6" s="20"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="43"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="16">
         <v>2</v>
       </c>
@@ -1303,7 +1315,7 @@
       <c r="T7" s="10"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="43"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="16">
         <v>3</v>
       </c>
@@ -1349,7 +1361,7 @@
       <c r="T8" s="10"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="44"/>
+      <c r="A9" s="42"/>
       <c r="B9" s="22">
         <v>4</v>
       </c>
@@ -1395,7 +1407,7 @@
       <c r="T9" s="15"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="16">
@@ -1421,7 +1433,7 @@
       <c r="T10" s="20"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="44"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="22">
         <v>2</v>
       </c>
@@ -1445,7 +1457,7 @@
       <c r="T11" s="15"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="44" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4">
@@ -1471,7 +1483,7 @@
       <c r="T12" s="20"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="44"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="22">
         <v>2</v>
       </c>
@@ -1495,7 +1507,7 @@
       <c r="T13" s="15"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="44" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
@@ -1521,7 +1533,7 @@
       <c r="T14" s="20"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="44"/>
+      <c r="A15" s="42"/>
       <c r="B15" s="22">
         <v>2</v>
       </c>
@@ -1545,7 +1557,7 @@
       <c r="T15" s="15"/>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="41" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="16">
@@ -1603,7 +1615,7 @@
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="43"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="16">
         <v>2</v>
       </c>
@@ -1659,7 +1671,7 @@
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="43"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="16">
         <v>3</v>
       </c>
@@ -1715,7 +1727,7 @@
       <c r="T18" s="10"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="43"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="16">
         <v>4</v>
       </c>
@@ -1729,7 +1741,9 @@
       <c r="F19" s="2">
         <v>100</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2">
+        <v>4</v>
+      </c>
       <c r="H19" s="2">
         <v>4</v>
       </c>
@@ -1767,7 +1781,7 @@
       <c r="T19" s="10"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="43"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="16">
         <v>5</v>
       </c>
@@ -1781,7 +1795,9 @@
       <c r="F20" s="2">
         <v>100</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2">
+        <v>4</v>
+      </c>
       <c r="H20" s="2">
         <v>4</v>
       </c>
@@ -1819,7 +1835,7 @@
       <c r="T20" s="10"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="43"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="16">
         <v>6</v>
       </c>
@@ -1833,7 +1849,9 @@
       <c r="F21" s="2">
         <v>100</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>4</v>
+      </c>
       <c r="H21" s="24">
         <v>4</v>
       </c>
@@ -1871,7 +1889,7 @@
       <c r="T21" s="10"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="43"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="16">
         <v>7</v>
       </c>
@@ -1885,7 +1903,9 @@
       <c r="F22" s="2">
         <v>100</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>4</v>
+      </c>
       <c r="H22" s="2">
         <v>4</v>
       </c>
@@ -1923,7 +1943,7 @@
       <c r="T22" s="10"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="43"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="16">
         <v>8</v>
       </c>
@@ -1937,7 +1957,9 @@
       <c r="F23" s="2">
         <v>100</v>
       </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>4</v>
+      </c>
       <c r="H23" s="2">
         <v>4</v>
       </c>
@@ -1975,7 +1997,7 @@
       <c r="T23" s="10"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="43"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="16">
         <v>9</v>
       </c>
@@ -1989,7 +2011,9 @@
       <c r="F24" s="2">
         <v>100</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2">
+        <v>4</v>
+      </c>
       <c r="H24" s="2">
         <v>4</v>
       </c>
@@ -2021,7 +2045,7 @@
       <c r="T24" s="10"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="43"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="16">
         <v>10</v>
       </c>
@@ -2035,7 +2059,9 @@
       <c r="F25" s="2">
         <v>100</v>
       </c>
-      <c r="G25" s="2"/>
+      <c r="G25" s="2">
+        <v>4</v>
+      </c>
       <c r="H25" s="2">
         <v>4</v>
       </c>
@@ -2069,7 +2095,7 @@
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="43"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="16">
         <v>11</v>
       </c>
@@ -2083,7 +2109,9 @@
       <c r="F26" s="2">
         <v>100</v>
       </c>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2">
+        <v>4</v>
+      </c>
       <c r="H26" s="2">
         <v>4</v>
       </c>
@@ -2093,8 +2121,8 @@
       <c r="J26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K26" s="27" t="b">
-        <v>1</v>
+      <c r="K26" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>50</v>
@@ -2108,8 +2136,8 @@
       <c r="O26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P26" s="2" t="s">
-        <v>21</v>
+      <c r="P26" s="31" t="s">
+        <v>60</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>21</v>
@@ -2121,7 +2149,7 @@
       <c r="T26" s="10"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="43"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="16">
         <v>12</v>
       </c>
@@ -2135,7 +2163,9 @@
       <c r="F27" s="2">
         <v>100</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>4</v>
+      </c>
       <c r="H27" s="2">
         <v>4</v>
       </c>
@@ -2161,7 +2191,7 @@
         <v>51</v>
       </c>
       <c r="P27" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>21</v>
@@ -2173,7 +2203,7 @@
       <c r="T27" s="10"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="43"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="16">
         <v>13</v>
       </c>
@@ -2187,7 +2217,9 @@
       <c r="F28" s="2">
         <v>100</v>
       </c>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2">
+        <v>4</v>
+      </c>
       <c r="H28" s="2">
         <v>4</v>
       </c>
@@ -2206,14 +2238,14 @@
       <c r="M28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>47</v>
+      <c r="N28" s="29" t="s">
+        <v>62</v>
       </c>
       <c r="O28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P28" s="31" t="s">
-        <v>61</v>
+      <c r="P28" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="Q28" s="2" t="s">
         <v>21</v>
@@ -2222,11 +2254,13 @@
         <v>21</v>
       </c>
       <c r="S28" s="2"/>
-      <c r="T28" s="10"/>
+      <c r="T28" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="43"/>
-      <c r="B29" s="16">
+      <c r="A29" s="41"/>
+      <c r="B29" s="45">
         <v>14</v>
       </c>
       <c r="C29" s="9"/>
@@ -2241,10 +2275,10 @@
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>32</v>
+        <v>4</v>
+      </c>
+      <c r="I29" s="25">
+        <v>48</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>45</v>
@@ -2258,8 +2292,8 @@
       <c r="M29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N29" s="29" t="s">
-        <v>62</v>
+      <c r="N29" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="O29" s="2" t="s">
         <v>51</v>
@@ -2277,8 +2311,8 @@
       <c r="T29" s="10"/>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="43"/>
-      <c r="B30" s="16">
+      <c r="A30" s="41"/>
+      <c r="B30" s="45">
         <v>15</v>
       </c>
       <c r="C30" s="9"/>
@@ -2298,8 +2332,8 @@
       <c r="I30" s="2">
         <v>32</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>45</v>
+      <c r="J30" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>21</v>
@@ -2319,8 +2353,8 @@
       <c r="P30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q30" s="32" t="b">
-        <v>1</v>
+      <c r="Q30" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="R30" s="2" t="s">
         <v>21</v>
@@ -2329,8 +2363,8 @@
       <c r="T30" s="10"/>
     </row>
     <row r="31" spans="1:20">
-      <c r="A31" s="43"/>
-      <c r="B31" s="16">
+      <c r="A31" s="41"/>
+      <c r="B31" s="45">
         <v>16</v>
       </c>
       <c r="C31" s="9"/>
@@ -2344,8 +2378,8 @@
         <v>100</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="2">
-        <v>4</v>
+      <c r="H31" s="24">
+        <v>6</v>
       </c>
       <c r="I31" s="2">
         <v>32</v>
@@ -2374,15 +2408,15 @@
       <c r="Q31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R31" s="33" t="b">
-        <v>1</v>
+      <c r="R31" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="S31" s="2"/>
       <c r="T31" s="10"/>
     </row>
     <row r="32" spans="1:20">
-      <c r="A32" s="43"/>
-      <c r="B32" s="16">
+      <c r="A32" s="41"/>
+      <c r="B32" s="45">
         <v>17</v>
       </c>
       <c r="C32" s="9"/>
@@ -2399,8 +2433,8 @@
       <c r="H32" s="2">
         <v>4</v>
       </c>
-      <c r="I32" s="25">
-        <v>48</v>
+      <c r="I32" s="2">
+        <v>32</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>45</v>
@@ -2426,15 +2460,15 @@
       <c r="Q32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="2" t="s">
-        <v>21</v>
+      <c r="R32" s="33" t="b">
+        <v>1</v>
       </c>
       <c r="S32" s="2"/>
       <c r="T32" s="10"/>
     </row>
-    <row r="33" spans="1:20">
-      <c r="A33" s="43"/>
-      <c r="B33" s="16">
+    <row r="33" spans="1:20" s="1" customFormat="1">
+      <c r="A33" s="41"/>
+      <c r="B33" s="45">
         <v>18</v>
       </c>
       <c r="C33" s="9"/>
@@ -2454,8 +2488,8 @@
       <c r="I33" s="2">
         <v>32</v>
       </c>
-      <c r="J33" s="26" t="s">
-        <v>22</v>
+      <c r="J33" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>21</v>
@@ -2475,18 +2509,18 @@
       <c r="P33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" s="2" t="s">
-        <v>21</v>
+      <c r="Q33" s="32" t="b">
+        <v>1</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="S33" s="2"/>
-      <c r="T33" s="10"/>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="43"/>
-      <c r="B34" s="16">
+      <c r="T33" s="35"/>
+    </row>
+    <row r="34" spans="1:20" s="1" customFormat="1">
+      <c r="A34" s="41"/>
+      <c r="B34" s="45">
         <v>19</v>
       </c>
       <c r="C34" s="9"/>
@@ -2500,8 +2534,8 @@
         <v>100</v>
       </c>
       <c r="G34" s="2"/>
-      <c r="H34" s="24">
-        <v>6</v>
+      <c r="H34" s="2">
+        <v>4</v>
       </c>
       <c r="I34" s="2">
         <v>32</v>
@@ -2509,8 +2543,8 @@
       <c r="J34" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>21</v>
+      <c r="K34" s="27" t="b">
+        <v>1</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>50</v>
@@ -2534,10 +2568,10 @@
         <v>21</v>
       </c>
       <c r="S34" s="2"/>
-      <c r="T34" s="10"/>
-    </row>
-    <row r="35" spans="1:20">
-      <c r="A35" s="43"/>
+      <c r="T34" s="35"/>
+    </row>
+    <row r="35" spans="1:20" s="1" customFormat="1">
+      <c r="A35" s="41"/>
       <c r="B35" s="16"/>
       <c r="C35" s="9"/>
       <c r="D35" s="2"/>
@@ -2556,10 +2590,10 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-      <c r="T35" s="10"/>
+      <c r="T35" s="35"/>
     </row>
     <row r="36" spans="1:20">
-      <c r="A36" s="43"/>
+      <c r="A36" s="41"/>
       <c r="B36" s="16"/>
       <c r="C36" s="9"/>
       <c r="D36" s="2"/>
@@ -2581,7 +2615,7 @@
       <c r="T36" s="10"/>
     </row>
     <row r="37" spans="1:20">
-      <c r="A37" s="43"/>
+      <c r="A37" s="41"/>
       <c r="B37" s="37" t="s">
         <v>63</v>
       </c>
@@ -2638,7 +2672,7 @@
       </c>
     </row>
     <row r="38" spans="1:20">
-      <c r="A38" s="44"/>
+      <c r="A38" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Commit before changing lastengen.py
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Network</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">0.01 LR, 0.99 Momentum</t>
+  </si>
+  <si>
+    <t>7_euclidean</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -226,6 +229,9 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -311,11 +317,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
   </fills>
-  <borders count="26">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -562,6 +565,77 @@
     </border>
     <border>
       <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color theme="1"/>
       </left>
       <right/>
@@ -614,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -686,11 +760,83 @@
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="16" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="16" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,58 +844,23 @@
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="15" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="16" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="29" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="30" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="31" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="32" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1839,70 +1950,70 @@
       <c r="T15" s="16"/>
     </row>
     <row r="16">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="29">
         <v>1</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="29">
         <v>250</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="29">
         <v>1</v>
       </c>
-      <c r="H16" s="20">
-        <v>4</v>
-      </c>
-      <c r="I16" s="20">
+      <c r="H16" s="29">
+        <v>4</v>
+      </c>
+      <c r="I16" s="29">
         <v>32</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="20" t="s">
+      <c r="K16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="O16" s="28" t="s">
+      <c r="O16" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="P16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="20"/>
-      <c r="T16" s="22" t="s">
+      <c r="P16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="29"/>
+      <c r="T16" s="31" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="23"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="18">
         <v>2</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E17" s="2">
@@ -1935,7 +2046,7 @@
       <c r="N17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="30" t="s">
+      <c r="O17" s="33" t="s">
         <v>50</v>
       </c>
       <c r="P17" s="2" t="s">
@@ -1948,12 +2059,12 @@
         <v>21</v>
       </c>
       <c r="S17" s="2"/>
-      <c r="T17" s="11" t="s">
+      <c r="T17" s="34" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="23"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="18">
         <v>3</v>
       </c>
@@ -1961,7 +2072,7 @@
       <c r="D18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="35">
         <v>168</v>
       </c>
       <c r="F18" s="2">
@@ -2006,18 +2117,18 @@
       <c r="S18" s="2">
         <v>51.599499999999999</v>
       </c>
-      <c r="T18" s="11"/>
+      <c r="T18" s="34"/>
     </row>
     <row r="19">
-      <c r="A19" s="23"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="18">
         <v>4</v>
       </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="35">
         <v>3360</v>
       </c>
       <c r="F19" s="2">
@@ -2060,15 +2171,15 @@
         <v>21</v>
       </c>
       <c r="S19" s="2"/>
-      <c r="T19" s="11"/>
+      <c r="T19" s="34"/>
     </row>
     <row r="20">
-      <c r="A20" s="23"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="18">
         <v>5</v>
       </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="36" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="2">
@@ -2114,15 +2225,15 @@
         <v>21</v>
       </c>
       <c r="S20" s="2"/>
-      <c r="T20" s="11"/>
+      <c r="T20" s="34"/>
     </row>
     <row r="21">
-      <c r="A21" s="23"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="18">
         <v>6</v>
       </c>
       <c r="C21" s="10"/>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="36" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="2">
@@ -2134,44 +2245,44 @@
       <c r="G21" s="2">
         <v>4</v>
       </c>
-      <c r="H21" s="33">
-        <v>4</v>
-      </c>
-      <c r="I21" s="34">
+      <c r="H21" s="37">
+        <v>4</v>
+      </c>
+      <c r="I21" s="38">
         <v>32</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="M21" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="N21" s="38" t="s">
+      <c r="K21" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="P21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="R21" s="42" t="s">
+      <c r="P21" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="46" t="s">
         <v>21</v>
       </c>
       <c r="S21" s="2"/>
-      <c r="T21" s="11"/>
+      <c r="T21" s="34"/>
     </row>
     <row r="22">
-      <c r="A22" s="23"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="18">
         <v>7</v>
       </c>
@@ -2200,10 +2311,10 @@
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="37" t="s">
+      <c r="L22" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="37" t="s">
+      <c r="M22" s="41" t="s">
         <v>45</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -2222,10 +2333,10 @@
         <v>21</v>
       </c>
       <c r="S22" s="2"/>
-      <c r="T22" s="11"/>
+      <c r="T22" s="34"/>
     </row>
     <row r="23">
-      <c r="A23" s="23"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="18">
         <v>8</v>
       </c>
@@ -2263,7 +2374,7 @@
       <c r="N23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="O23" s="43" t="s">
         <v>54</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2276,10 +2387,10 @@
         <v>21</v>
       </c>
       <c r="S23" s="2"/>
-      <c r="T23" s="11"/>
+      <c r="T23" s="34"/>
     </row>
     <row r="24">
-      <c r="A24" s="23"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="18">
         <v>9</v>
       </c>
@@ -2317,17 +2428,17 @@
       <c r="N24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O24" s="39" t="s">
+      <c r="O24" s="43" t="s">
         <v>55</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
-      <c r="T24" s="11"/>
+      <c r="T24" s="34"/>
     </row>
     <row r="25">
-      <c r="A25" s="23"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="18">
         <v>10</v>
       </c>
@@ -2365,19 +2476,19 @@
       <c r="N25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="39" t="s">
+      <c r="O25" s="43" t="s">
         <v>56</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-      <c r="T25" s="11" t="s">
+      <c r="T25" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="23"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="18">
         <v>11</v>
       </c>
@@ -2418,7 +2529,7 @@
       <c r="O26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P26" s="40" t="s">
+      <c r="P26" s="44" t="s">
         <v>58</v>
       </c>
       <c r="Q26" s="2" t="s">
@@ -2428,10 +2539,10 @@
         <v>21</v>
       </c>
       <c r="S26" s="2"/>
-      <c r="T26" s="11"/>
+      <c r="T26" s="34"/>
     </row>
     <row r="27">
-      <c r="A27" s="23"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="18">
         <v>12</v>
       </c>
@@ -2472,7 +2583,7 @@
       <c r="O27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P27" s="40" t="s">
+      <c r="P27" s="44" t="s">
         <v>59</v>
       </c>
       <c r="Q27" s="2" t="s">
@@ -2482,10 +2593,10 @@
         <v>21</v>
       </c>
       <c r="S27" s="2"/>
-      <c r="T27" s="11"/>
+      <c r="T27" s="34"/>
     </row>
     <row r="28">
-      <c r="A28" s="23"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="18">
         <v>13</v>
       </c>
@@ -2520,7 +2631,7 @@
       <c r="M28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="38" t="s">
+      <c r="N28" s="42" t="s">
         <v>60</v>
       </c>
       <c r="O28" s="2" t="s">
@@ -2536,13 +2647,13 @@
         <v>21</v>
       </c>
       <c r="S28" s="2"/>
-      <c r="T28" s="11" t="s">
+      <c r="T28" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="23"/>
-      <c r="B29" s="43">
+      <c r="A29" s="32"/>
+      <c r="B29" s="47">
         <v>14</v>
       </c>
       <c r="C29" s="10"/>
@@ -2559,7 +2670,7 @@
       <c r="H29" s="2">
         <v>4</v>
       </c>
-      <c r="I29" s="34">
+      <c r="I29" s="38">
         <v>48</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -2590,11 +2701,11 @@
         <v>21</v>
       </c>
       <c r="S29" s="2"/>
-      <c r="T29" s="11"/>
+      <c r="T29" s="34"/>
     </row>
     <row r="30">
-      <c r="A30" s="23"/>
-      <c r="B30" s="43">
+      <c r="A30" s="32"/>
+      <c r="B30" s="47">
         <v>15</v>
       </c>
       <c r="C30" s="10"/>
@@ -2614,7 +2725,7 @@
       <c r="I30" s="2">
         <v>32</v>
       </c>
-      <c r="J30" s="35" t="s">
+      <c r="J30" s="39" t="s">
         <v>22</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -2642,11 +2753,11 @@
         <v>21</v>
       </c>
       <c r="S30" s="2"/>
-      <c r="T30" s="11"/>
+      <c r="T30" s="34"/>
     </row>
     <row r="31">
-      <c r="A31" s="23"/>
-      <c r="B31" s="43">
+      <c r="A31" s="32"/>
+      <c r="B31" s="47">
         <v>16</v>
       </c>
       <c r="C31" s="10"/>
@@ -2660,7 +2771,7 @@
         <v>100</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="33">
+      <c r="H31" s="37">
         <v>6</v>
       </c>
       <c r="I31" s="2">
@@ -2694,11 +2805,11 @@
         <v>21</v>
       </c>
       <c r="S31" s="2"/>
-      <c r="T31" s="11"/>
+      <c r="T31" s="34"/>
     </row>
     <row r="32">
-      <c r="A32" s="23"/>
-      <c r="B32" s="43">
+      <c r="A32" s="32"/>
+      <c r="B32" s="47">
         <v>17</v>
       </c>
       <c r="C32" s="10"/>
@@ -2742,15 +2853,15 @@
       <c r="Q32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="42" t="b">
+      <c r="R32" s="46" t="b">
         <v>1</v>
       </c>
       <c r="S32" s="2"/>
-      <c r="T32" s="11"/>
+      <c r="T32" s="34"/>
     </row>
     <row r="33" s="1" customFormat="1">
-      <c r="A33" s="23"/>
-      <c r="B33" s="43">
+      <c r="A33" s="32"/>
+      <c r="B33" s="47">
         <v>18</v>
       </c>
       <c r="C33" s="10"/>
@@ -2791,179 +2902,351 @@
       <c r="P33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" s="41" t="b">
+      <c r="Q33" s="45" t="b">
         <v>1</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="S33" s="2"/>
-      <c r="T33" s="11"/>
+      <c r="T33" s="34"/>
     </row>
     <row r="34" s="1" customFormat="1">
-      <c r="A34" s="23"/>
-      <c r="B34" s="43">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49">
         <v>19</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="50"/>
+      <c r="D34" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="51">
         <v>3360</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="51">
         <v>100</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2">
-        <v>4</v>
-      </c>
-      <c r="I34" s="2">
+      <c r="G34" s="51"/>
+      <c r="H34" s="51">
+        <v>4</v>
+      </c>
+      <c r="I34" s="51">
         <v>32</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="K34" s="36" t="b">
+      <c r="K34" s="52" t="b">
         <v>1</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N34" s="2" t="s">
+      <c r="L34" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="N34" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="O34" s="2" t="s">
+      <c r="O34" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S34" s="2"/>
-      <c r="T34" s="11"/>
+      <c r="P34" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="51" t="s">
+        <v>21</v>
+      </c>
+      <c r="S34" s="51"/>
+      <c r="T34" s="53"/>
     </row>
     <row r="35" s="1" customFormat="1">
-      <c r="A35" s="23"/>
-      <c r="B35" s="18"/>
+      <c r="A35" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="18">
+        <v>1</v>
+      </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
+      <c r="D35" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="2">
+        <v>168</v>
+      </c>
+      <c r="F35" s="2">
+        <v>100</v>
+      </c>
+      <c r="G35" s="2">
+        <v>4</v>
+      </c>
+      <c r="H35" s="56">
+        <v>4</v>
+      </c>
+      <c r="I35" s="2">
+        <v>32</v>
+      </c>
+      <c r="J35" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="K35" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="M35" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="N35" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="O35" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="P35" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q35" s="55" t="s">
+        <v>21</v>
+      </c>
+      <c r="R35" s="55" t="s">
+        <v>21</v>
+      </c>
       <c r="S35" s="2"/>
       <c r="T35" s="11"/>
     </row>
-    <row r="36">
-      <c r="A36" s="23"/>
-      <c r="B36" s="18"/>
+    <row r="36" s="1" customFormat="1">
+      <c r="A36" s="32"/>
+      <c r="B36" s="18">
+        <v>2</v>
+      </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="44"/>
+      <c r="H36" s="56"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
+      <c r="O36" s="55"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
       <c r="T36" s="11"/>
     </row>
-    <row r="37">
-      <c r="A37" s="23"/>
-      <c r="B37" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47">
+    <row r="37" s="1" customFormat="1">
+      <c r="A37" s="32"/>
+      <c r="B37" s="18">
         <v>3</v>
       </c>
-      <c r="E37" s="47">
+      <c r="C37" s="10"/>
+      <c r="D37" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="11"/>
+    </row>
+    <row r="38" s="1" customFormat="1">
+      <c r="A38" s="32"/>
+      <c r="B38" s="18">
+        <v>4</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="11"/>
+    </row>
+    <row r="39" s="1" customFormat="1">
+      <c r="A39" s="32"/>
+      <c r="B39" s="18">
+        <v>5</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="11"/>
+    </row>
+    <row r="40" s="1" customFormat="1">
+      <c r="A40" s="32"/>
+      <c r="B40" s="18">
+        <v>6</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="11"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="32"/>
+      <c r="B41" s="18">
+        <v>7</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="11"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="57"/>
+      <c r="B42" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="59"/>
+      <c r="D42" s="60">
+        <v>3</v>
+      </c>
+      <c r="E42" s="60">
         <v>1</v>
       </c>
-      <c r="F37" s="47">
+      <c r="F42" s="60">
         <v>1</v>
       </c>
-      <c r="G37" s="47">
+      <c r="G42" s="60">
         <v>1</v>
       </c>
-      <c r="H37" s="47">
+      <c r="H42" s="60">
         <v>2</v>
       </c>
-      <c r="I37" s="47">
+      <c r="I42" s="60">
         <v>2</v>
       </c>
-      <c r="J37" s="47">
+      <c r="J42" s="60">
         <v>2</v>
       </c>
-      <c r="K37" s="47">
+      <c r="K42" s="60">
         <v>2</v>
       </c>
-      <c r="L37" s="47">
+      <c r="L42" s="60">
         <v>2</v>
       </c>
-      <c r="M37" s="47">
+      <c r="M42" s="60">
         <v>1</v>
       </c>
-      <c r="N37" s="47">
+      <c r="N42" s="60">
         <v>2</v>
       </c>
-      <c r="O37" s="47">
+      <c r="O42" s="60">
         <v>3</v>
       </c>
-      <c r="P37" s="47">
+      <c r="P42" s="60">
         <v>2</v>
       </c>
-      <c r="Q37" s="47">
+      <c r="Q42" s="60">
         <v>2</v>
       </c>
-      <c r="R37" s="47">
+      <c r="R42" s="60">
         <v>2</v>
       </c>
-      <c r="S37" s="47"/>
-      <c r="T37" s="48">
-        <f>PRODUCT(D37:R37)</f>
+      <c r="S42" s="60"/>
+      <c r="T42" s="61">
+        <f>PRODUCT(D42:R42)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="25"/>
+    <row r="43">
+      <c r="A43" s="62"/>
+    </row>
+    <row r="44" ht="14.25">
+      <c r="A44" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A38"/>
+    <mergeCell ref="A16:A34"/>
+    <mergeCell ref="A35:A41"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Notebooks for creating new data sets
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Network</t>
   </si>
@@ -202,6 +202,27 @@
   </si>
   <si>
     <t>7_euclidean</t>
+  </si>
+  <si>
+    <t>LASTENS</t>
+  </si>
+  <si>
+    <t>LASTENA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10% original data</t>
+  </si>
+  <si>
+    <t>LASTENAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5% original data</t>
+  </si>
+  <si>
+    <t>LASTENS+LASTEN</t>
+  </si>
+  <si>
+    <t>LASTENS+LASTENA</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -688,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -835,15 +856,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -860,7 +879,6 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1371,7 +1389,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="1" width="22"/>
     <col customWidth="1" min="2" max="2" style="1" width="11.28515625"/>
-    <col customWidth="1" min="3" max="4" style="1" width="10.5703125"/>
+    <col customWidth="1" min="3" max="3" style="1" width="10.5703125"/>
+    <col customWidth="1" min="4" max="4" style="1" width="17.3984375"/>
     <col customWidth="1" min="5" max="5" style="1" width="10.7109375"/>
     <col customWidth="1" min="6" max="6" style="1" width="9.140625"/>
     <col customWidth="1" min="7" max="8" style="1" width="12.28515625"/>
@@ -2964,14 +2983,14 @@
       <c r="T34" s="53"/>
     </row>
     <row r="35" s="1" customFormat="1">
-      <c r="A35" s="54" t="s">
+      <c r="A35" s="27" t="s">
         <v>62</v>
       </c>
       <c r="B35" s="18">
         <v>1</v>
       </c>
       <c r="C35" s="10"/>
-      <c r="D35" s="55" t="s">
+      <c r="D35" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="2">
@@ -2981,39 +3000,39 @@
         <v>100</v>
       </c>
       <c r="G35" s="2">
-        <v>4</v>
-      </c>
-      <c r="H35" s="56">
+        <v>2</v>
+      </c>
+      <c r="H35" s="54">
         <v>4</v>
       </c>
       <c r="I35" s="2">
         <v>32</v>
       </c>
-      <c r="J35" s="55" t="s">
+      <c r="J35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K35" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="M35" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="N35" s="55" t="s">
+      <c r="K35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O35" s="55" t="s">
+      <c r="O35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P35" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q35" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="R35" s="55" t="s">
+      <c r="P35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="S35" s="2"/>
@@ -3028,20 +3047,48 @@
       <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
-      <c r="R36" s="2"/>
+      <c r="E36" s="2">
+        <v>168</v>
+      </c>
+      <c r="F36" s="2">
+        <v>100</v>
+      </c>
+      <c r="G36" s="2">
+        <v>4</v>
+      </c>
+      <c r="H36" s="54">
+        <v>4</v>
+      </c>
+      <c r="I36" s="2">
+        <v>32</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S36" s="2"/>
       <c r="T36" s="11"/>
     </row>
@@ -3052,22 +3099,50 @@
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="E37" s="54">
+        <v>3360</v>
+      </c>
+      <c r="F37" s="2">
+        <v>100</v>
+      </c>
+      <c r="G37" s="2">
+        <v>4</v>
+      </c>
+      <c r="H37" s="54">
+        <v>4</v>
+      </c>
+      <c r="I37" s="2">
+        <v>32</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S37" s="2"/>
       <c r="T37" s="11"/>
     </row>
@@ -3077,25 +3152,55 @@
         <v>4</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="R38" s="2"/>
+      <c r="D38" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="54">
+        <v>3360</v>
+      </c>
+      <c r="F38" s="2">
+        <v>100</v>
+      </c>
+      <c r="G38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38" s="54">
+        <v>4</v>
+      </c>
+      <c r="I38" s="2">
+        <v>32</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S38" s="2"/>
-      <c r="T38" s="11"/>
+      <c r="T38" s="56" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="39" s="1" customFormat="1">
       <c r="A39" s="32"/>
@@ -3103,25 +3208,55 @@
         <v>5</v>
       </c>
       <c r="C39" s="10"/>
-      <c r="D39" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="56"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
+      <c r="D39" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1680</v>
+      </c>
+      <c r="F39" s="2">
+        <v>100</v>
+      </c>
+      <c r="G39" s="2">
+        <v>4</v>
+      </c>
+      <c r="H39" s="54">
+        <v>4</v>
+      </c>
+      <c r="I39" s="2">
+        <v>32</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R39" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S39" s="2"/>
-      <c r="T39" s="11"/>
+      <c r="T39" s="56" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="40" s="1" customFormat="1">
       <c r="A40" s="32"/>
@@ -3130,12 +3265,16 @@
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3528</v>
+      </c>
+      <c r="F40" s="2">
+        <v>100</v>
+      </c>
       <c r="G40" s="2"/>
-      <c r="H40" s="56"/>
+      <c r="H40" s="54"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
@@ -3149,94 +3288,166 @@
       <c r="S40" s="2"/>
       <c r="T40" s="11"/>
     </row>
-    <row r="41">
+    <row r="41" s="1" customFormat="1">
       <c r="A41" s="32"/>
       <c r="B41" s="18">
         <v>7</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="2"/>
+        <v>69</v>
+      </c>
+      <c r="E41" s="2">
+        <v>6720</v>
+      </c>
+      <c r="F41" s="2">
+        <v>100</v>
+      </c>
+      <c r="G41" s="2">
+        <v>4</v>
+      </c>
+      <c r="H41" s="54">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2">
+        <v>32</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R41" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="S41" s="2"/>
       <c r="T41" s="11"/>
     </row>
-    <row r="42">
-      <c r="A42" s="57"/>
-      <c r="B42" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="59"/>
-      <c r="D42" s="60">
+    <row r="42" s="1" customFormat="1">
+      <c r="A42" s="32"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="11"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="32"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="11"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="57"/>
+      <c r="B44" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="59"/>
+      <c r="D44" s="60">
         <v>3</v>
       </c>
-      <c r="E42" s="60">
+      <c r="E44" s="60">
         <v>1</v>
       </c>
-      <c r="F42" s="60">
+      <c r="F44" s="60">
         <v>1</v>
       </c>
-      <c r="G42" s="60">
+      <c r="G44" s="60">
         <v>1</v>
       </c>
-      <c r="H42" s="60">
+      <c r="H44" s="60">
         <v>2</v>
       </c>
-      <c r="I42" s="60">
+      <c r="I44" s="60">
         <v>2</v>
       </c>
-      <c r="J42" s="60">
+      <c r="J44" s="60">
         <v>2</v>
       </c>
-      <c r="K42" s="60">
+      <c r="K44" s="60">
         <v>2</v>
       </c>
-      <c r="L42" s="60">
+      <c r="L44" s="60">
         <v>2</v>
       </c>
-      <c r="M42" s="60">
+      <c r="M44" s="60">
         <v>1</v>
       </c>
-      <c r="N42" s="60">
+      <c r="N44" s="60">
         <v>2</v>
       </c>
-      <c r="O42" s="60">
+      <c r="O44" s="60">
         <v>3</v>
       </c>
-      <c r="P42" s="60">
+      <c r="P44" s="60">
         <v>2</v>
       </c>
-      <c r="Q42" s="60">
+      <c r="Q44" s="60">
         <v>2</v>
       </c>
-      <c r="R42" s="60">
+      <c r="R44" s="60">
         <v>2</v>
       </c>
-      <c r="S42" s="60"/>
-      <c r="T42" s="61">
-        <f>PRODUCT(D42:R42)</f>
+      <c r="S44" s="60"/>
+      <c r="T44" s="61">
+        <f>PRODUCT(D44:R44)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="62"/>
-    </row>
-    <row r="44" ht="14.25">
-      <c r="A44" s="63"/>
+    <row r="45">
+      <c r="A45" s="62"/>
+    </row>
+    <row r="46" ht="14.25">
+      <c r="A46" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3246,7 +3457,7 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A16:A34"/>
-    <mergeCell ref="A35:A41"/>
+    <mergeCell ref="A35:A43"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Trainings 7_1_2_3 and 7_4_5_6 set up
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Julian\workspace\endolas\experiments\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="72">
   <si>
     <t>Network</t>
   </si>
@@ -21,25 +27,25 @@
     <t>Training</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Train Size</t>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Train Size</t>
   </si>
   <si>
     <t>Epochs</t>
   </si>
   <si>
-    <t xml:space="preserve">Batch Size</t>
+    <t>Batch Size</t>
   </si>
   <si>
     <t>Depth</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature Maps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Size</t>
+    <t>Feature Maps</t>
+  </si>
+  <si>
+    <t>Image Size</t>
   </si>
   <si>
     <t>Augment</t>
@@ -63,10 +69,10 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t xml:space="preserve">Gap Filling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Score Value</t>
+    <t>Gap Filling</t>
+  </si>
+  <si>
+    <t>Score Value</t>
   </si>
   <si>
     <t>Note</t>
@@ -90,13 +96,13 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Dropout</t>
+    <t>No Dropout</t>
   </si>
   <si>
     <t>MAE</t>
   </si>
   <si>
-    <t xml:space="preserve">No Preprocessing</t>
+    <t>No Preprocessing</t>
   </si>
   <si>
     <t>2_segmentation</t>
@@ -108,7 +114,7 @@
     <t>LASTEN</t>
   </si>
   <si>
-    <t xml:space="preserve">384 x 384</t>
+    <t>384 x 384</t>
   </si>
   <si>
     <t>Dice</t>
@@ -159,7 +165,7 @@
     <t>Fixed+Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed and Moving Input</t>
+    <t>Fixed and Moving Input</t>
   </si>
   <si>
     <t>msed</t>
@@ -168,7 +174,7 @@
     <t>Moving</t>
   </si>
   <si>
-    <t xml:space="preserve">Moving Input</t>
+    <t>Moving Input</t>
   </si>
   <si>
     <t>SIMPLEA</t>
@@ -186,7 +192,7 @@
     <t>Moving+Diff+Gradient</t>
   </si>
   <si>
-    <t xml:space="preserve">Gradient of Image</t>
+    <t>Gradient of Image</t>
   </si>
   <si>
     <t>L1</t>
@@ -198,7 +204,7 @@
     <t>SGD</t>
   </si>
   <si>
-    <t xml:space="preserve">0.01 LR, 0.99 Momentum</t>
+    <t>0.01 LR, 0.99 Momentum</t>
   </si>
   <si>
     <t>7_euclidean</t>
@@ -210,41 +216,44 @@
     <t>LASTENA</t>
   </si>
   <si>
-    <t xml:space="preserve">10% original data</t>
+    <t>10% original data</t>
   </si>
   <si>
     <t>LASTENAS</t>
   </si>
   <si>
-    <t xml:space="preserve">5% original data</t>
+    <t>5% original data</t>
   </si>
   <si>
     <t>LASTENS+LASTEN</t>
   </si>
   <si>
-    <t>LASTENS+LASTENA</t>
-  </si>
-  <si>
     <t>Possibilities</t>
+  </si>
+  <si>
+    <t>Pretrained</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color indexed="64"/>
       <name val="Arial Unicode MS"/>
-      <color indexed="64"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,14 +337,38 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE0EB4C"/>
-        <bgColor rgb="FFE0EB4C"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor rgb="FFE0EB4C"/>
       </patternFill>
     </fill>
   </fills>
@@ -707,177 +740,192 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+  <cellXfs count="68">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="13" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="14" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="15" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="16" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="16" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="29" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="30" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="31" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="32" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -885,294 +933,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF996633"/>
+      <color rgb="FFCCFF33"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1375,46 +1154,47 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMX45"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="R31" activeCellId="0" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" style="1" width="22"/>
-    <col customWidth="1" min="2" max="2" style="1" width="11.28515625"/>
-    <col customWidth="1" min="3" max="3" style="1" width="10.5703125"/>
-    <col customWidth="1" min="4" max="4" style="1" width="17.3984375"/>
-    <col customWidth="1" min="5" max="5" style="1" width="10.7109375"/>
-    <col customWidth="1" min="6" max="6" style="1" width="9.140625"/>
-    <col customWidth="1" min="7" max="8" style="1" width="12.28515625"/>
-    <col customWidth="1" min="9" max="9" style="1" width="13.140625"/>
-    <col customWidth="1" min="10" max="11" style="1" width="12.28515625"/>
-    <col customWidth="1" min="12" max="12" style="1" width="8.85546875"/>
-    <col customWidth="1" min="13" max="13" style="1" width="8"/>
-    <col customWidth="1" min="14" max="14" style="1" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" min="15" max="15" style="1" width="19.42578125"/>
-    <col customWidth="1" min="16" max="16" style="1" width="13.7109375"/>
-    <col customWidth="1" min="17" max="18" style="1" width="15.7109375"/>
-    <col bestFit="1" customWidth="1" min="19" max="19" style="1" width="14.5703125"/>
-    <col customWidth="1" min="20" max="20" style="1" width="26.85546875"/>
-    <col customWidth="1" min="21" max="21" style="1" width="15.42578125"/>
-    <col customWidth="1" min="22" max="22" style="1" width="14.5703125"/>
-    <col customWidth="1" min="23" max="24" style="1" width="8.5703125"/>
-    <col customWidth="1" min="25" max="25" style="1" width="14.42578125"/>
-    <col customWidth="1" min="26" max="26" style="1" width="15.42578125"/>
-    <col customWidth="1" min="27" max="1034" style="1" width="8.5703125"/>
-    <col customWidth="1" min="1035" max="1037" style="1" width="9.140625"/>
-    <col min="1038" max="16384" width="9.140625"/>
+    <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="1" customWidth="1"/>
+    <col min="17" max="19" width="15.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.85546875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" style="1" customWidth="1"/>
+    <col min="24" max="25" width="8.5703125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" style="1" customWidth="1"/>
+    <col min="28" max="1035" width="8.5703125" style="1" customWidth="1"/>
+    <col min="1036" max="1038" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1">
+    <row r="1" spans="1:21" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1467,23 +1247,26 @@
         <v>15</v>
       </c>
       <c r="R1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:21">
+      <c r="A2" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="2"/>
@@ -1516,16 +1299,17 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="47"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" s="1" customFormat="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12">
+      <c r="T2" s="2"/>
+      <c r="U2" s="10"/>
+    </row>
+    <row r="3" spans="1:21" s="1" customFormat="1">
+      <c r="A3" s="61"/>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="2"/>
@@ -1558,18 +1342,19 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="R3" s="47"/>
       <c r="S3" s="2"/>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="2"/>
+      <c r="U3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12">
+    <row r="4" spans="1:21" s="1" customFormat="1">
+      <c r="A4" s="61"/>
+      <c r="B4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="2"/>
@@ -1602,90 +1387,93 @@
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="R4" s="47"/>
       <c r="S4" s="2"/>
-      <c r="T4" s="11" t="s">
+      <c r="T4" s="2"/>
+      <c r="U4" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="16"/>
-    </row>
-    <row r="6" ht="15.75">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:21">
+      <c r="A5" s="61"/>
+      <c r="B5" s="12">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="15"/>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="18">
         <v>168</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="18">
         <v>300</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <v>8</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18">
         <v>32</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="20" t="b">
+      <c r="K6" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="L6" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="21" t="s">
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" ht="15.75">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18">
+      <c r="U6" s="20"/>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="63"/>
+      <c r="B7" s="16">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1720,18 +1508,19 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="24" t="s">
+      <c r="R7" s="47"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="T7" s="11"/>
-    </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18">
+      <c r="U7" s="10"/>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="63"/>
+      <c r="B8" s="16">
         <v>3</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1766,272 +1555,283 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="24" t="s">
+      <c r="R8" s="47"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="T8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26">
-        <v>4</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="U8" s="10"/>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="64"/>
+      <c r="B9" s="22">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>168</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>300</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>2</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14">
         <v>48</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="15" t="b">
+      <c r="K9" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="16"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
+      <c r="U9" s="15"/>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="16">
         <v>1</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="22"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26">
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="20"/>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="64"/>
+      <c r="B11" s="22">
         <v>2</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="16"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="15"/>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="62" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="T12" s="22"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26">
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="20"/>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="64"/>
+      <c r="B13" s="22">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="15"/>
-      <c r="S13" s="15"/>
-      <c r="T13" s="16"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="15"/>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="62" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="22"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26">
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+      <c r="T14" s="18"/>
+      <c r="U14" s="20"/>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="64"/>
+      <c r="B15" s="22">
         <v>2</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="16"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="27" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="15"/>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="58" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="24">
         <v>1</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="24">
         <v>250</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="24">
         <v>1</v>
       </c>
-      <c r="H16" s="29">
-        <v>4</v>
-      </c>
-      <c r="I16" s="29">
+      <c r="H16" s="24">
+        <v>4</v>
+      </c>
+      <c r="I16" s="24">
         <v>32</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="29" t="s">
+      <c r="K16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="29" t="s">
+      <c r="M16" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="29" t="s">
+      <c r="N16" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O16" s="30" t="s">
+      <c r="O16" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="P16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="R16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="S16" s="29"/>
-      <c r="T16" s="31" t="s">
+      <c r="P16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="S16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" s="24"/>
+      <c r="U16" s="26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="32"/>
-      <c r="B17" s="18">
+    <row r="17" spans="1:21">
+      <c r="A17" s="59"/>
+      <c r="B17" s="16">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
@@ -2065,7 +1865,7 @@
       <c r="N17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="33" t="s">
+      <c r="O17" s="27" t="s">
         <v>50</v>
       </c>
       <c r="P17" s="2" t="s">
@@ -2074,24 +1874,27 @@
       <c r="Q17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S17" s="2"/>
-      <c r="T17" s="34" t="s">
+      <c r="R17" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="2"/>
+      <c r="U17" s="28" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="32"/>
-      <c r="B18" s="18">
+    <row r="18" spans="1:21">
+      <c r="A18" s="59"/>
+      <c r="B18" s="16">
         <v>3</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="29">
         <v>168</v>
       </c>
       <c r="F18" s="2">
@@ -2130,24 +1933,27 @@
       <c r="Q18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S18" s="2">
+      <c r="R18" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T18" s="2">
         <v>51.599499999999999</v>
       </c>
-      <c r="T18" s="34"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="32"/>
-      <c r="B19" s="18">
-        <v>4</v>
-      </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="36" t="s">
+      <c r="U18" s="28"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="59"/>
+      <c r="B19" s="16">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="29">
         <v>3360</v>
       </c>
       <c r="F19" s="2">
@@ -2186,19 +1992,22 @@
       <c r="Q19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="34"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="32"/>
-      <c r="B20" s="18">
+      <c r="R19" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="28"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="59"/>
+      <c r="B20" s="16">
         <v>5</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="36" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="2">
@@ -2240,19 +2049,22 @@
       <c r="Q20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="34"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="32"/>
-      <c r="B21" s="18">
+      <c r="R20" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="28"/>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="59"/>
+      <c r="B21" s="16">
         <v>6</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="36" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="30" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="2">
@@ -2264,48 +2076,51 @@
       <c r="G21" s="2">
         <v>4</v>
       </c>
-      <c r="H21" s="37">
-        <v>4</v>
-      </c>
-      <c r="I21" s="38">
+      <c r="H21" s="31">
+        <v>4</v>
+      </c>
+      <c r="I21" s="32">
         <v>32</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="M21" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="N21" s="42" t="s">
+      <c r="K21" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="O21" s="43" t="s">
+      <c r="O21" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="P21" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q21" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="R21" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="34"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="32"/>
-      <c r="B22" s="18">
+      <c r="P21" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="S21" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="28"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="59"/>
+      <c r="B22" s="16">
         <v>7</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
@@ -2330,10 +2145,10 @@
       <c r="K22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="41" t="s">
+      <c r="L22" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="41" t="s">
+      <c r="M22" s="35" t="s">
         <v>45</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -2348,18 +2163,21 @@
       <c r="Q22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="34"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="32"/>
-      <c r="B23" s="18">
+      <c r="R22" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="28"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="59"/>
+      <c r="B23" s="16">
         <v>8</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2393,7 +2211,7 @@
       <c r="N23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O23" s="43" t="s">
+      <c r="O23" s="37" t="s">
         <v>54</v>
       </c>
       <c r="P23" s="2" t="s">
@@ -2402,18 +2220,21 @@
       <c r="Q23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S23" s="2"/>
-      <c r="T23" s="34"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="32"/>
-      <c r="B24" s="18">
+      <c r="R23" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" s="2"/>
+      <c r="U23" s="28"/>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="59"/>
+      <c r="B24" s="16">
         <v>9</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="2" t="s">
         <v>53</v>
       </c>
@@ -2447,21 +2268,24 @@
       <c r="N24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O24" s="43" t="s">
+      <c r="O24" s="37" t="s">
         <v>55</v>
       </c>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
+      <c r="R24" s="47" t="s">
+        <v>21</v>
+      </c>
       <c r="S24" s="2"/>
-      <c r="T24" s="34"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="18">
+      <c r="T24" s="2"/>
+      <c r="U24" s="28"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="59"/>
+      <c r="B25" s="16">
         <v>10</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="2" t="s">
         <v>53</v>
       </c>
@@ -2495,23 +2319,26 @@
       <c r="N25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="43" t="s">
+      <c r="O25" s="37" t="s">
         <v>56</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
+      <c r="R25" s="47" t="s">
+        <v>21</v>
+      </c>
       <c r="S25" s="2"/>
-      <c r="T25" s="34" t="s">
+      <c r="T25" s="2"/>
+      <c r="U25" s="28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="32"/>
-      <c r="B26" s="18">
+    <row r="26" spans="1:21">
+      <c r="A26" s="59"/>
+      <c r="B26" s="16">
         <v>11</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="2" t="s">
         <v>53</v>
       </c>
@@ -2548,24 +2375,27 @@
       <c r="O26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P26" s="44" t="s">
+      <c r="P26" s="38" t="s">
         <v>58</v>
       </c>
       <c r="Q26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S26" s="2"/>
-      <c r="T26" s="34"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="32"/>
-      <c r="B27" s="18">
+      <c r="R26" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="28"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="59"/>
+      <c r="B27" s="16">
         <v>12</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="2" t="s">
         <v>53</v>
       </c>
@@ -2602,24 +2432,27 @@
       <c r="O27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="P27" s="44" t="s">
+      <c r="P27" s="38" t="s">
         <v>59</v>
       </c>
       <c r="Q27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S27" s="2"/>
-      <c r="T27" s="34"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="32"/>
-      <c r="B28" s="18">
+      <c r="R27" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="28"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="59"/>
+      <c r="B28" s="16">
         <v>13</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="2" t="s">
         <v>53</v>
       </c>
@@ -2650,7 +2483,7 @@
       <c r="M28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="42" t="s">
+      <c r="N28" s="36" t="s">
         <v>60</v>
       </c>
       <c r="O28" s="2" t="s">
@@ -2662,20 +2495,23 @@
       <c r="Q28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S28" s="2"/>
-      <c r="T28" s="34" t="s">
+      <c r="R28" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="32"/>
-      <c r="B29" s="47">
+    <row r="29" spans="1:21">
+      <c r="A29" s="59"/>
+      <c r="B29" s="40">
         <v>14</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="2" t="s">
         <v>53</v>
       </c>
@@ -2689,7 +2525,7 @@
       <c r="H29" s="2">
         <v>4</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I29" s="32">
         <v>48</v>
       </c>
       <c r="J29" s="2" t="s">
@@ -2716,18 +2552,21 @@
       <c r="Q29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="34"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="32"/>
-      <c r="B30" s="47">
+      <c r="R29" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="28"/>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="59"/>
+      <c r="B30" s="40">
         <v>15</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="2" t="s">
         <v>53</v>
       </c>
@@ -2744,7 +2583,7 @@
       <c r="I30" s="2">
         <v>32</v>
       </c>
-      <c r="J30" s="39" t="s">
+      <c r="J30" s="33" t="s">
         <v>22</v>
       </c>
       <c r="K30" s="2" t="s">
@@ -2768,18 +2607,21 @@
       <c r="Q30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R30" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="34"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="32"/>
-      <c r="B31" s="47">
+      <c r="R30" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T30" s="2"/>
+      <c r="U30" s="28"/>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="59"/>
+      <c r="B31" s="40">
         <v>16</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="2" t="s">
         <v>53</v>
       </c>
@@ -2790,7 +2632,7 @@
         <v>100</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="37">
+      <c r="H31" s="31">
         <v>6</v>
       </c>
       <c r="I31" s="2">
@@ -2820,18 +2662,21 @@
       <c r="Q31" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R31" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S31" s="2"/>
-      <c r="T31" s="34"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="32"/>
-      <c r="B32" s="47">
+      <c r="R31" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" s="2"/>
+      <c r="U31" s="28"/>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="59"/>
+      <c r="B32" s="40">
         <v>17</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="2" t="s">
         <v>53</v>
       </c>
@@ -2872,18 +2717,21 @@
       <c r="Q32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R32" s="46" t="b">
+      <c r="R32" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" s="67" t="b">
         <v>1</v>
       </c>
-      <c r="S32" s="2"/>
-      <c r="T32" s="34"/>
-    </row>
-    <row r="33" s="1" customFormat="1">
-      <c r="A33" s="32"/>
-      <c r="B33" s="47">
+      <c r="T32" s="2"/>
+      <c r="U32" s="28"/>
+    </row>
+    <row r="33" spans="1:21" s="1" customFormat="1">
+      <c r="A33" s="59"/>
+      <c r="B33" s="40">
         <v>18</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="2" t="s">
         <v>53</v>
       </c>
@@ -2921,76 +2769,82 @@
       <c r="P33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q33" s="45" t="b">
+      <c r="Q33" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="R33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S33" s="2"/>
-      <c r="T33" s="34"/>
-    </row>
-    <row r="34" s="1" customFormat="1">
-      <c r="A34" s="48"/>
-      <c r="B34" s="49">
+      <c r="R33" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T33" s="2"/>
+      <c r="U33" s="28"/>
+    </row>
+    <row r="34" spans="1:21" s="1" customFormat="1">
+      <c r="A34" s="60"/>
+      <c r="B34" s="41">
         <v>19</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="51" t="s">
+      <c r="C34" s="42"/>
+      <c r="D34" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="51">
+      <c r="E34" s="43">
         <v>3360</v>
       </c>
-      <c r="F34" s="51">
+      <c r="F34" s="43">
         <v>100</v>
       </c>
-      <c r="G34" s="51"/>
-      <c r="H34" s="51">
-        <v>4</v>
-      </c>
-      <c r="I34" s="51">
+      <c r="G34" s="43"/>
+      <c r="H34" s="43">
+        <v>4</v>
+      </c>
+      <c r="I34" s="43">
         <v>32</v>
       </c>
-      <c r="J34" s="51" t="s">
+      <c r="J34" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="K34" s="52" t="b">
+      <c r="K34" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="L34" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="M34" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="N34" s="51" t="s">
+      <c r="L34" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="M34" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="N34" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="O34" s="51" t="s">
+      <c r="O34" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="P34" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q34" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="R34" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="S34" s="51"/>
-      <c r="T34" s="53"/>
-    </row>
-    <row r="35" s="1" customFormat="1">
-      <c r="A35" s="27" t="s">
+      <c r="P34" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q34" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="S34" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="T34" s="43"/>
+      <c r="U34" s="45"/>
+    </row>
+    <row r="35" spans="1:21" s="1" customFormat="1">
+      <c r="A35" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="16">
         <v>1</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="2" t="s">
+      <c r="C35" s="9"/>
+      <c r="D35" s="56" t="s">
         <v>30</v>
       </c>
       <c r="E35" s="2">
@@ -2999,10 +2853,10 @@
       <c r="F35" s="2">
         <v>100</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="55">
         <v>2</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="46">
         <v>4</v>
       </c>
       <c r="I35" s="2">
@@ -3032,19 +2886,22 @@
       <c r="Q35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S35" s="2"/>
-      <c r="T35" s="11"/>
-    </row>
-    <row r="36" s="1" customFormat="1">
-      <c r="A36" s="32"/>
-      <c r="B36" s="18">
+      <c r="R35" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T35" s="2"/>
+      <c r="U35" s="10"/>
+    </row>
+    <row r="36" spans="1:21" s="1" customFormat="1">
+      <c r="A36" s="59"/>
+      <c r="B36" s="16">
         <v>2</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="9"/>
+      <c r="D36" s="56" t="s">
         <v>30</v>
       </c>
       <c r="E36" s="2">
@@ -3056,7 +2913,7 @@
       <c r="G36" s="2">
         <v>4</v>
       </c>
-      <c r="H36" s="54">
+      <c r="H36" s="46">
         <v>4</v>
       </c>
       <c r="I36" s="2">
@@ -3086,31 +2943,34 @@
       <c r="Q36" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S36" s="2"/>
-      <c r="T36" s="11"/>
-    </row>
-    <row r="37" s="1" customFormat="1">
-      <c r="A37" s="32"/>
-      <c r="B37" s="18">
+      <c r="R36" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T36" s="2"/>
+      <c r="U36" s="10"/>
+    </row>
+    <row r="37" spans="1:21" s="1" customFormat="1">
+      <c r="A37" s="59"/>
+      <c r="B37" s="16">
         <v>3</v>
       </c>
-      <c r="C37" s="10"/>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="54">
+      <c r="E37" s="46">
         <v>3360</v>
       </c>
       <c r="F37" s="2">
         <v>100</v>
       </c>
-      <c r="G37" s="2">
-        <v>4</v>
-      </c>
-      <c r="H37" s="54">
+      <c r="G37" s="57">
+        <v>4</v>
+      </c>
+      <c r="H37" s="46">
         <v>4</v>
       </c>
       <c r="I37" s="2">
@@ -3140,131 +3000,140 @@
       <c r="Q37" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R37" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S37" s="2"/>
-      <c r="T37" s="11"/>
-    </row>
-    <row r="38" s="1" customFormat="1">
-      <c r="A38" s="32"/>
-      <c r="B38" s="18">
-        <v>4</v>
-      </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="55" t="s">
+      <c r="R37" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T37" s="2"/>
+      <c r="U37" s="10"/>
+    </row>
+    <row r="38" spans="1:21" s="1" customFormat="1">
+      <c r="A38" s="59"/>
+      <c r="B38" s="16">
+        <v>4</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="54">
+      <c r="E38" s="46">
         <v>3360</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="47">
         <v>100</v>
       </c>
-      <c r="G38" s="2">
-        <v>4</v>
-      </c>
-      <c r="H38" s="54">
-        <v>4</v>
-      </c>
-      <c r="I38" s="2">
+      <c r="G38" s="47">
+        <v>4</v>
+      </c>
+      <c r="H38" s="46">
+        <v>4</v>
+      </c>
+      <c r="I38" s="47">
         <v>32</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J38" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N38" s="2" t="s">
+      <c r="K38" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M38" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N38" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="O38" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="P38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S38" s="2"/>
-      <c r="T38" s="56" t="s">
+      <c r="P38" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q38" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="R38" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S38" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="T38" s="47"/>
+      <c r="U38" s="48" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="39" s="1" customFormat="1">
-      <c r="A39" s="32"/>
-      <c r="B39" s="18">
+    <row r="39" spans="1:21" s="1" customFormat="1">
+      <c r="A39" s="59"/>
+      <c r="B39" s="16">
         <v>5</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="55" t="s">
+      <c r="C39" s="9"/>
+      <c r="D39" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="47">
         <v>1680</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="47">
         <v>100</v>
       </c>
-      <c r="G39" s="2">
-        <v>4</v>
-      </c>
-      <c r="H39" s="54">
-        <v>4</v>
-      </c>
-      <c r="I39" s="2">
+      <c r="G39" s="47">
+        <v>4</v>
+      </c>
+      <c r="H39" s="46">
+        <v>4</v>
+      </c>
+      <c r="I39" s="47">
         <v>32</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="J39" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="K39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N39" s="2" t="s">
+      <c r="K39" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M39" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N39" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="O39" s="2" t="s">
+      <c r="O39" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="P39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S39" s="2"/>
-      <c r="T39" s="56" t="s">
+      <c r="P39" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q39" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="R39" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S39" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="T39" s="47"/>
+      <c r="U39" s="48" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" s="1" customFormat="1">
-      <c r="A40" s="32"/>
-      <c r="B40" s="18">
+    <row r="40" spans="1:21" s="1" customFormat="1">
+      <c r="A40" s="59"/>
+      <c r="B40" s="16">
         <v>6</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="9"/>
+      <c r="D40" s="56" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="2">
@@ -3273,32 +3142,59 @@
       <c r="F40" s="2">
         <v>100</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2"/>
-      <c r="T40" s="11"/>
-    </row>
-    <row r="41" s="1" customFormat="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="18">
+      <c r="G40" s="2">
+        <v>4</v>
+      </c>
+      <c r="H40" s="46">
+        <v>4</v>
+      </c>
+      <c r="I40" s="47">
+        <v>32</v>
+      </c>
+      <c r="J40" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M40" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N40" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="O40" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R40" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T40" s="2"/>
+      <c r="U40" s="10"/>
+    </row>
+    <row r="41" spans="1:21" s="1" customFormat="1">
+      <c r="A41" s="59"/>
+      <c r="B41" s="16">
         <v>7</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="2" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="E41" s="2">
-        <v>6720</v>
+        <v>168</v>
       </c>
       <c r="F41" s="2">
         <v>100</v>
@@ -3306,28 +3202,28 @@
       <c r="G41" s="2">
         <v>4</v>
       </c>
-      <c r="H41" s="54">
-        <v>4</v>
-      </c>
-      <c r="I41" s="2">
+      <c r="H41" s="46">
+        <v>4</v>
+      </c>
+      <c r="I41" s="47">
         <v>32</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="K41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N41" s="2" t="s">
+      <c r="K41" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M41" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N41" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="O41" s="2" t="s">
+      <c r="O41" s="47" t="s">
         <v>54</v>
       </c>
       <c r="P41" s="2" t="s">
@@ -3336,43 +3232,81 @@
       <c r="Q41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R41" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S41" s="2"/>
-      <c r="T41" s="11"/>
-    </row>
-    <row r="42" s="1" customFormat="1">
-      <c r="A42" s="32"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="11"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="32"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="10"/>
+      <c r="R41" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="S41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T41" s="2"/>
+      <c r="U41" s="10"/>
+    </row>
+    <row r="42" spans="1:21" s="1" customFormat="1">
+      <c r="A42" s="59"/>
+      <c r="B42" s="16">
+        <v>8</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="47">
+        <v>168</v>
+      </c>
+      <c r="F42" s="47">
+        <v>100</v>
+      </c>
+      <c r="G42" s="47">
+        <v>4</v>
+      </c>
+      <c r="H42" s="46">
+        <v>4</v>
+      </c>
+      <c r="I42" s="47">
+        <v>32</v>
+      </c>
+      <c r="J42" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="M42" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="N42" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="O42" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R42" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="S42" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="T42" s="2"/>
+      <c r="U42" s="10"/>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="59"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="54"/>
+      <c r="H43" s="46"/>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
@@ -3382,86 +3316,84 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
-      <c r="R43" s="2"/>
+      <c r="R43" s="47"/>
       <c r="S43" s="2"/>
-      <c r="T43" s="11"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="57"/>
-      <c r="B44" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="60">
+      <c r="T43" s="2"/>
+      <c r="U43" s="10"/>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="49"/>
+      <c r="B44" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="51"/>
+      <c r="D44" s="52">
         <v>3</v>
       </c>
-      <c r="E44" s="60">
+      <c r="E44" s="52">
         <v>1</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="52">
         <v>1</v>
       </c>
-      <c r="G44" s="60">
+      <c r="G44" s="52">
         <v>1</v>
       </c>
-      <c r="H44" s="60">
+      <c r="H44" s="52">
         <v>2</v>
       </c>
-      <c r="I44" s="60">
+      <c r="I44" s="52">
         <v>2</v>
       </c>
-      <c r="J44" s="60">
+      <c r="J44" s="52">
         <v>2</v>
       </c>
-      <c r="K44" s="60">
+      <c r="K44" s="52">
         <v>2</v>
       </c>
-      <c r="L44" s="60">
+      <c r="L44" s="52">
         <v>2</v>
       </c>
-      <c r="M44" s="60">
+      <c r="M44" s="52">
         <v>1</v>
       </c>
-      <c r="N44" s="60">
+      <c r="N44" s="52">
         <v>2</v>
       </c>
-      <c r="O44" s="60">
+      <c r="O44" s="52">
         <v>3</v>
       </c>
-      <c r="P44" s="60">
+      <c r="P44" s="52">
         <v>2</v>
       </c>
-      <c r="Q44" s="60">
+      <c r="Q44" s="52">
         <v>2</v>
       </c>
-      <c r="R44" s="60">
+      <c r="R44" s="52"/>
+      <c r="S44" s="52">
         <v>2</v>
       </c>
-      <c r="S44" s="60"/>
-      <c r="T44" s="61">
-        <f>PRODUCT(D44:R44)</f>
+      <c r="T44" s="52"/>
+      <c r="U44" s="53">
+        <f>PRODUCT(D44:S44)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="62"/>
-    </row>
-    <row r="46" ht="14.25">
-      <c r="A46" s="1"/>
+    <row r="45" spans="1:21">
+      <c r="A45" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A16:A34"/>
+    <mergeCell ref="A35:A43"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A34"/>
-    <mergeCell ref="A35:A43"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="1"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="300"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Further trainings set up
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Network</t>
   </si>
@@ -285,7 +285,10 @@
     <t xml:space="preserve">From LASTEN a percentage X is randomly drawn and the other 1-X is randomly drawn from LASTENS for Train. Val and Test stay the same</t>
   </si>
   <si>
-    <t xml:space="preserve">X % LASTEN2 + 100 – X % LASTENS</t>
+    <t xml:space="preserve">LASTEN2_0: 336 synthetic, 0 real
+LASTEN2_10: 302 synthetic, 34 real
+LASTEN2_25: 252 synthetic, 84 real
+LASTEN2_50: 168 synthetic, 168real</t>
   </si>
   <si>
     <t xml:space="preserve">2x20 Frames</t>
@@ -309,7 +312,13 @@
     <t>LASTEN2_X</t>
   </si>
   <si>
-    <t xml:space="preserve">From LASTEN2 a percentage X is randomly drawn and the other 1-X is randomly drawn from LASTENS for Train. Val and Test stay the same</t>
+    <t xml:space="preserve">From LASTEN2 a percentage X is randomly drawn and the other 1-X is drawn from LASTENS for Train. Val and Test stay the same</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTEN2_0: 320 synthetic, 0 real
+LASTEN2_10: 288 synthetic, 32 real
+LASTEN2_25: 240 synthetic, 80 real
+LASTEN2_50: 160 synthetic, 160 real</t>
   </si>
   <si>
     <t xml:space="preserve">3200 images</t>
@@ -318,10 +327,12 @@
     <t>LASTEN2A_X</t>
   </si>
   <si>
-    <t xml:space="preserve">From LASTEN2_X only the ground truth data is taken and augmented in such a way that that a total of 320 training images are present</t>
-  </si>
-  <si>
-    <t xml:space="preserve">320 images</t>
+    <t xml:space="preserve">From LASTEN2 only the ground truth data is taken and each image is augmented 19 times and stored in a seperate folder. Afterwards for LASTEN2_10 the first 9 augmentations for LASTEN2_25 the first 3 augmentations and for LASTEN2_50 the first augmentation is copied. Like that randomness is reduced since the same augmentation appears in multiple data sets.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LASTEN2_10: 288 augmented, 32 real
+LASTEN2_25: 240 augmented, 80 real
+LASTEN2_50: 160 augmented, 160 real</t>
   </si>
 </sst>
 </file>
@@ -472,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -650,13 +661,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="hair">
         <color theme="1"/>
       </right>
-      <top style="hair">
+      <top style="thin">
         <color theme="1"/>
       </top>
       <bottom style="hair">
@@ -666,6 +677,36 @@
     </border>
     <border>
       <left style="hair">
+        <color theme="1"/>
+      </left>
+      <right style="hair">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="hair">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="hair">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="hair">
@@ -677,7 +718,7 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top/>
@@ -685,7 +726,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
+      <left style="thin">
         <color theme="1"/>
       </left>
       <right style="hair">
@@ -708,11 +749,53 @@
     </border>
     <border>
       <left/>
-      <right style="hair">
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top/>
       <bottom style="hair">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="hair">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color theme="1"/>
       </bottom>
       <diagonal/>
@@ -726,7 +809,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,24 +928,18 @@
     <xf fontId="0" fillId="18" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="20" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="19" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="20" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="20" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="21" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -871,7 +948,9 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -880,7 +959,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -892,35 +971,38 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1363,7 +1445,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" style="0" width="22"/>
     <col customWidth="1" min="2" max="2" style="0" width="18.629999999999999"/>
-    <col customWidth="1" min="3" max="3" style="0" width="14.220000000000001"/>
+    <col customWidth="1" min="3" max="3" style="0" width="31.9296875"/>
     <col customWidth="1" min="4" max="4" style="0" width="17.399999999999999"/>
     <col customWidth="1" min="5" max="5" style="0" width="11.68"/>
     <col customWidth="1" min="6" max="6" style="0" width="9.1400000000000006"/>
@@ -3337,10 +3419,10 @@
       <c r="B41" s="9">
         <v>7</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D41" s="42" t="s">
         <v>69</v>
       </c>
       <c r="E41" s="1">
@@ -3393,10 +3475,10 @@
       <c r="B42" s="9">
         <v>8</v>
       </c>
-      <c r="C42" s="42" t="s">
+      <c r="C42" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="42" t="s">
         <v>70</v>
       </c>
       <c r="E42" s="1">
@@ -3449,10 +3531,10 @@
       <c r="B43" s="9">
         <v>9</v>
       </c>
-      <c r="C43" s="42" t="s">
+      <c r="C43" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="43" t="s">
+      <c r="D43" s="42" t="s">
         <v>71</v>
       </c>
       <c r="E43" s="1">
@@ -3505,10 +3587,10 @@
       <c r="B44" s="9">
         <v>10</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="42" t="s">
         <v>72</v>
       </c>
       <c r="E44" s="1">
@@ -3564,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="43" t="s">
         <v>40</v>
       </c>
       <c r="E45" s="17">
@@ -3617,10 +3699,10 @@
       <c r="B46" s="9">
         <v>2</v>
       </c>
-      <c r="C46" s="42" t="s">
+      <c r="C46" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="46" t="s">
+      <c r="D46" s="44" t="s">
         <v>74</v>
       </c>
       <c r="E46" s="1">
@@ -3674,7 +3756,7 @@
         <v>3</v>
       </c>
       <c r="C47" s="9"/>
-      <c r="D47" s="46" t="s">
+      <c r="D47" s="44" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="1">
@@ -3728,7 +3810,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="9"/>
-      <c r="D48" s="46" t="s">
+      <c r="D48" s="44" t="s">
         <v>76</v>
       </c>
       <c r="E48" s="1">
@@ -3781,8 +3863,10 @@
       <c r="B49" s="9">
         <v>5</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="47" t="s">
+      <c r="C49" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="44" t="s">
         <v>77</v>
       </c>
       <c r="E49" s="1">
@@ -3835,8 +3919,10 @@
       <c r="B50" s="9">
         <v>6</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="48" t="s">
+      <c r="C50" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" s="46" t="s">
         <v>78</v>
       </c>
       <c r="E50" s="1">
@@ -3889,8 +3975,10 @@
       <c r="B51" s="9">
         <v>7</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="48" t="s">
+      <c r="C51" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="46" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="1">
@@ -3943,8 +4031,10 @@
       <c r="B52" s="9">
         <v>8</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="48" t="s">
+      <c r="C52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="46" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="1">
@@ -3997,8 +4087,10 @@
       <c r="B53" s="9">
         <v>9</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="48" t="s">
+      <c r="C53" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="46" t="s">
         <v>81</v>
       </c>
       <c r="E53" s="1">
@@ -4069,7 +4161,7 @@
       <c r="T54" s="15"/>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="49"/>
+      <c r="A55" s="47"/>
       <c r="B55" s="4" t="s">
         <v>82</v>
       </c>
@@ -4120,22 +4212,22 @@
         <v>2</v>
       </c>
       <c r="S55" s="5"/>
-      <c r="T55" s="50">
+      <c r="T55" s="48">
         <f>PRODUCT(D55:R55)</f>
         <v>4608</v>
       </c>
     </row>
     <row r="59" ht="13.800000000000001">
-      <c r="A59" s="51" t="s">
+      <c r="A59" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="51" t="s">
+      <c r="C59" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="51" t="s">
+      <c r="D59" s="50" t="s">
         <v>85</v>
       </c>
       <c r="E59" s="51" t="s">
@@ -4251,27 +4343,27 @@
       <c r="B66" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="C66" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="D66" s="64" t="s">
+      <c r="C66" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="E66" s="65" t="s">
+      <c r="E66" s="64" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="67" ht="14.25">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="65" t="s">
         <v>81</v>
       </c>
       <c r="B67" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D67" s="64" t="s">
+      <c r="C67" s="58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D67" s="63" t="s">
         <v>91</v>
       </c>
       <c r="E67" s="64" t="s">
@@ -4279,19 +4371,19 @@
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68" s="68" t="s">
+      <c r="A68" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="66" t="s">
+      <c r="B68" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="D68" s="64" t="s">
+      <c r="C68" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="D68" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="E68" s="64" t="s">
+      <c r="E68" s="69" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pipeline started with segmentation and went on with peaking
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -827,7 +827,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="71">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -844,9 +844,6 @@
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -885,15 +882,6 @@
     <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1516,66 +1504,66 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" ht="14.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="1"/>
@@ -1612,14 +1600,14 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
-      <c r="U2" s="11"/>
+      <c r="U2" s="10"/>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="12">
+      <c r="A3" s="7"/>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="1"/>
@@ -1656,16 +1644,16 @@
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="12">
+      <c r="A4" s="7"/>
+      <c r="B4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="1"/>
@@ -1702,91 +1690,91 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="11" t="s">
+      <c r="U4" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="13">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="16"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="12">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="15"/>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="17"/>
+      <c r="E6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <v>168</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>300</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="17">
         <v>8</v>
       </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18">
+      <c r="I6" s="17"/>
+      <c r="J6" s="17">
         <v>32</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="18" t="b">
-        <f t="shared" ref="L6:L10" si="1">TRUE()</f>
+      <c r="L6" s="17" t="b">
+        <f t="shared" ref="L6:L35" si="1">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="M6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="18" t="s">
+      <c r="N6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="19" t="s">
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="U6" s="20"/>
+      <c r="U6" s="19"/>
     </row>
     <row r="7" ht="15.75">
-      <c r="A7" s="17"/>
-      <c r="B7" s="10">
+      <c r="A7" s="16"/>
+      <c r="B7" s="9">
         <v>2</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="1"/>
@@ -1824,17 +1812,17 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="U7" s="11"/>
+      <c r="U7" s="10"/>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="17"/>
-      <c r="B8" s="10">
+      <c r="A8" s="16"/>
+      <c r="B8" s="9">
         <v>3</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="1"/>
@@ -1872,67 +1860,67 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="U8" s="11"/>
+      <c r="U8" s="10"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14">
-        <v>4</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="13">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="14">
         <v>168</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>300</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="14">
         <v>2</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15">
+      <c r="I9" s="14"/>
+      <c r="J9" s="14">
         <v>48</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="15" t="b">
+      <c r="L9" s="14" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15" t="s">
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="U9" s="16"/>
+      <c r="U9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <v>1</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1"/>
@@ -1952,7 +1940,7 @@
       <c r="J10" s="1">
         <v>32</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L10" s="1" t="b">
@@ -1965,24 +1953,24 @@
       <c r="N10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="20"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="19"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="10">
+      <c r="A11" s="16"/>
+      <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="9" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="1">
@@ -1998,16 +1986,16 @@
       <c r="J11" s="1">
         <v>32</v>
       </c>
-      <c r="K11" s="22" t="s">
-        <v>23</v>
+      <c r="K11" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="L11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="22" t="s">
+      <c r="N11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="O11" s="1"/>
@@ -2016,218 +2004,218 @@
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
-      <c r="U11" s="11"/>
+      <c r="U11" s="10"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14">
+      <c r="A12" s="16"/>
+      <c r="B12" s="13">
         <v>3</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="15" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <v>168</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="14">
         <v>100</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="14">
         <v>1</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15">
+      <c r="I12" s="14"/>
+      <c r="J12" s="14">
         <v>32</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="25" t="b">
+      <c r="K12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="21" t="b">
         <v>0</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="16"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="15"/>
     </row>
     <row r="13" ht="13.800000000000001">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3">
         <v>1</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="19"/>
     </row>
     <row r="14" ht="13.800000000000001">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14">
+      <c r="A14" s="16"/>
+      <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="16"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="15"/>
     </row>
     <row r="15" ht="13.800000000000001">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="3">
         <v>1</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
-      <c r="T15" s="18"/>
-      <c r="U15" s="20"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="19"/>
     </row>
     <row r="16" ht="13.800000000000001">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14">
+      <c r="A16" s="16"/>
+      <c r="B16" s="13">
         <v>2</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="15"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="17"/>
+      <c r="E17" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <v>1</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G17" s="17">
         <v>250</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="17">
         <v>1</v>
       </c>
-      <c r="I17" s="18">
-        <v>4</v>
-      </c>
-      <c r="J17" s="18">
+      <c r="I17" s="17">
+        <v>4</v>
+      </c>
+      <c r="J17" s="17">
         <v>32</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="18" t="s">
+      <c r="L17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="18" t="s">
+      <c r="N17" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="18" t="s">
+      <c r="O17" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="26" t="s">
+      <c r="P17" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="Q17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="S17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="T17" s="18"/>
-      <c r="U17" s="20" t="s">
+      <c r="Q17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" s="17"/>
+      <c r="U17" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="10">
+      <c r="A18" s="16"/>
+      <c r="B18" s="9">
         <v>2</v>
       </c>
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>43</v>
@@ -2262,7 +2250,7 @@
       <c r="O18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="27" t="s">
+      <c r="P18" s="23" t="s">
         <v>50</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -2275,21 +2263,21 @@
         <v>22</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="11" t="s">
+      <c r="U18" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="17"/>
-      <c r="B19" s="10">
+      <c r="A19" s="16"/>
+      <c r="B19" s="9">
         <v>3</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="24">
         <v>168</v>
       </c>
       <c r="G19" s="1">
@@ -2334,19 +2322,19 @@
       <c r="T19" s="1">
         <v>51.599499999999999</v>
       </c>
-      <c r="U19" s="11"/>
+      <c r="U19" s="10"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="10">
-        <v>4</v>
-      </c>
-      <c r="C20" s="10"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="9">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="24">
         <v>3360</v>
       </c>
       <c r="G20" s="1">
@@ -2389,16 +2377,16 @@
         <v>22</v>
       </c>
       <c r="T20" s="1"/>
-      <c r="U20" s="11"/>
+      <c r="U20" s="10"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="10">
+      <c r="A21" s="16"/>
+      <c r="B21" s="9">
         <v>5</v>
       </c>
-      <c r="C21" s="10"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="25" t="s">
         <v>43</v>
       </c>
       <c r="F21" s="1">
@@ -2444,16 +2432,16 @@
         <v>22</v>
       </c>
       <c r="T21" s="1"/>
-      <c r="U21" s="11"/>
+      <c r="U21" s="10"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="10">
+      <c r="A22" s="16"/>
+      <c r="B22" s="9">
         <v>6</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="29" t="s">
+      <c r="E22" s="25" t="s">
         <v>53</v>
       </c>
       <c r="F22" s="1">
@@ -2465,48 +2453,48 @@
       <c r="H22" s="1">
         <v>4</v>
       </c>
-      <c r="I22" s="30">
-        <v>4</v>
-      </c>
-      <c r="J22" s="31">
+      <c r="I22" s="26">
+        <v>4</v>
+      </c>
+      <c r="J22" s="27">
         <v>32</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="N22" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="O22" s="35" t="s">
+      <c r="L22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="P22" s="36" t="s">
+      <c r="P22" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="Q22" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="R22" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="39" t="s">
+      <c r="Q22" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="R22" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="35" t="s">
         <v>22</v>
       </c>
       <c r="T22" s="1"/>
-      <c r="U22" s="11"/>
+      <c r="U22" s="10"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="10">
+      <c r="A23" s="16"/>
+      <c r="B23" s="9">
         <v>7</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
         <v>53</v>
@@ -2532,10 +2520,10 @@
       <c r="L23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="34" t="s">
+      <c r="M23" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="N23" s="34" t="s">
+      <c r="N23" s="30" t="s">
         <v>45</v>
       </c>
       <c r="O23" s="1" t="s">
@@ -2554,14 +2542,14 @@
         <v>22</v>
       </c>
       <c r="T23" s="1"/>
-      <c r="U23" s="11"/>
+      <c r="U23" s="10"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="10">
+      <c r="A24" s="16"/>
+      <c r="B24" s="9">
         <v>8</v>
       </c>
-      <c r="C24" s="10"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>53</v>
@@ -2596,7 +2584,7 @@
       <c r="O24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P24" s="36" t="s">
+      <c r="P24" s="32" t="s">
         <v>54</v>
       </c>
       <c r="Q24" s="1" t="s">
@@ -2609,14 +2597,14 @@
         <v>22</v>
       </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="11"/>
+      <c r="U24" s="10"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="10">
+      <c r="A25" s="16"/>
+      <c r="B25" s="9">
         <v>9</v>
       </c>
-      <c r="C25" s="10"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
         <v>53</v>
@@ -2651,21 +2639,21 @@
       <c r="O25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P25" s="36" t="s">
+      <c r="P25" s="32" t="s">
         <v>55</v>
       </c>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="11"/>
+      <c r="U25" s="10"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="10">
+      <c r="A26" s="16"/>
+      <c r="B26" s="9">
         <v>10</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
         <v>53</v>
@@ -2700,23 +2688,23 @@
       <c r="O26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P26" s="36" t="s">
+      <c r="P26" s="32" t="s">
         <v>56</v>
       </c>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="11" t="s">
+      <c r="U26" s="10" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="10">
+      <c r="A27" s="16"/>
+      <c r="B27" s="9">
         <v>11</v>
       </c>
-      <c r="C27" s="10"/>
+      <c r="C27" s="9"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
         <v>53</v>
@@ -2754,7 +2742,7 @@
       <c r="P27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q27" s="37" t="s">
+      <c r="Q27" s="33" t="s">
         <v>58</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -2764,14 +2752,14 @@
         <v>22</v>
       </c>
       <c r="T27" s="1"/>
-      <c r="U27" s="11"/>
+      <c r="U27" s="10"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="10">
+      <c r="A28" s="16"/>
+      <c r="B28" s="9">
         <v>12</v>
       </c>
-      <c r="C28" s="10"/>
+      <c r="C28" s="9"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
         <v>53</v>
@@ -2809,7 +2797,7 @@
       <c r="P28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q28" s="37" t="s">
+      <c r="Q28" s="33" t="s">
         <v>59</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -2819,14 +2807,14 @@
         <v>22</v>
       </c>
       <c r="T28" s="1"/>
-      <c r="U28" s="11"/>
+      <c r="U28" s="10"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="40">
+      <c r="A29" s="16"/>
+      <c r="B29" s="36">
         <v>13</v>
       </c>
-      <c r="C29" s="10"/>
+      <c r="C29" s="9"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
         <v>53</v>
@@ -2858,7 +2846,7 @@
       <c r="N29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O29" s="35" t="s">
+      <c r="O29" s="31" t="s">
         <v>60</v>
       </c>
       <c r="P29" s="1" t="s">
@@ -2874,16 +2862,16 @@
         <v>22</v>
       </c>
       <c r="T29" s="1"/>
-      <c r="U29" s="11" t="s">
+      <c r="U29" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="41">
+      <c r="A30" s="16"/>
+      <c r="B30" s="37">
         <v>14</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
         <v>53</v>
@@ -2898,7 +2886,7 @@
       <c r="I30" s="1">
         <v>4</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="27">
         <v>48</v>
       </c>
       <c r="K30" s="1" t="s">
@@ -2929,14 +2917,14 @@
         <v>22</v>
       </c>
       <c r="T30" s="1"/>
-      <c r="U30" s="11"/>
+      <c r="U30" s="10"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="41">
+      <c r="A31" s="16"/>
+      <c r="B31" s="37">
         <v>15</v>
       </c>
-      <c r="C31" s="10"/>
+      <c r="C31" s="9"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
         <v>53</v>
@@ -2954,7 +2942,7 @@
       <c r="J31" s="1">
         <v>32</v>
       </c>
-      <c r="K31" s="32" t="s">
+      <c r="K31" s="28" t="s">
         <v>23</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -2982,14 +2970,14 @@
         <v>22</v>
       </c>
       <c r="T31" s="1"/>
-      <c r="U31" s="11"/>
+      <c r="U31" s="10"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="17"/>
-      <c r="B32" s="41">
+      <c r="A32" s="16"/>
+      <c r="B32" s="37">
         <v>16</v>
       </c>
-      <c r="C32" s="10"/>
+      <c r="C32" s="9"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
         <v>53</v>
@@ -3001,7 +2989,7 @@
         <v>100</v>
       </c>
       <c r="H32" s="1"/>
-      <c r="I32" s="30">
+      <c r="I32" s="26">
         <v>6</v>
       </c>
       <c r="J32" s="1">
@@ -3035,14 +3023,14 @@
         <v>22</v>
       </c>
       <c r="T32" s="1"/>
-      <c r="U32" s="11"/>
+      <c r="U32" s="10"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="17"/>
-      <c r="B33" s="41">
+      <c r="A33" s="16"/>
+      <c r="B33" s="37">
         <v>17</v>
       </c>
-      <c r="C33" s="10"/>
+      <c r="C33" s="9"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
         <v>53</v>
@@ -3084,19 +3072,19 @@
       <c r="R33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S33" s="39" t="b">
+      <c r="S33" s="35" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
       <c r="T33" s="1"/>
-      <c r="U33" s="11"/>
+      <c r="U33" s="10"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="17"/>
-      <c r="B34" s="41">
+      <c r="A34" s="16"/>
+      <c r="B34" s="37">
         <v>18</v>
       </c>
-      <c r="C34" s="10"/>
+      <c r="C34" s="9"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
         <v>53</v>
@@ -3135,7 +3123,7 @@
       <c r="Q34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="38" t="b">
+      <c r="R34" s="34" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
@@ -3143,70 +3131,70 @@
         <v>22</v>
       </c>
       <c r="T34" s="1"/>
-      <c r="U34" s="11"/>
+      <c r="U34" s="10"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="42">
+      <c r="A35" s="16"/>
+      <c r="B35" s="38">
         <v>19</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="15">
+      <c r="F35" s="14">
         <v>3360</v>
       </c>
-      <c r="G35" s="15">
+      <c r="G35" s="14">
         <v>100</v>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15">
-        <v>4</v>
-      </c>
-      <c r="J35" s="15">
+      <c r="H35" s="14"/>
+      <c r="I35" s="14">
+        <v>4</v>
+      </c>
+      <c r="J35" s="14">
         <v>32</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="K35" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="L35" s="43" t="b">
-        <f>TRUE()</f>
+      <c r="L35" s="39" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="N35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="O35" s="15" t="s">
+      <c r="M35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O35" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P35" s="15" t="s">
+      <c r="P35" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Q35" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="R35" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="S35" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="T35" s="15"/>
-      <c r="U35" s="16"/>
+      <c r="Q35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="T35" s="14"/>
+      <c r="U35" s="15"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="C36" s="10"/>
+      <c r="C36" s="9"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
         <v>31</v>
@@ -3217,7 +3205,7 @@
       <c r="G36" s="1">
         <v>100</v>
       </c>
-      <c r="H36" s="45">
+      <c r="H36" s="41">
         <v>2</v>
       </c>
       <c r="I36" s="1">
@@ -3254,16 +3242,16 @@
         <v>22</v>
       </c>
       <c r="T36" s="1"/>
-      <c r="U36" s="11"/>
+      <c r="U36" s="10"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="10">
+      <c r="A37" s="40"/>
+      <c r="B37" s="9">
         <v>2</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="9"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="46" t="s">
+      <c r="E37" s="42" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="1">
@@ -3272,7 +3260,7 @@
       <c r="G37" s="1">
         <v>100</v>
       </c>
-      <c r="H37" s="45">
+      <c r="H37" s="41">
         <v>4</v>
       </c>
       <c r="I37" s="1">
@@ -3309,18 +3297,18 @@
         <v>22</v>
       </c>
       <c r="T37" s="1"/>
-      <c r="U37" s="11"/>
+      <c r="U37" s="10"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="10">
+      <c r="A38" s="40"/>
+      <c r="B38" s="9">
         <v>3</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="9"/>
       <c r="D38" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="46" t="s">
+      <c r="E38" s="42" t="s">
         <v>64</v>
       </c>
       <c r="F38" s="1">
@@ -3366,18 +3354,18 @@
         <v>22</v>
       </c>
       <c r="T38" s="1"/>
-      <c r="U38" s="11"/>
+      <c r="U38" s="10"/>
     </row>
     <row r="39" ht="14.25">
-      <c r="A39" s="44"/>
-      <c r="B39" s="10">
-        <v>4</v>
-      </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="22" t="s">
+      <c r="A39" s="40"/>
+      <c r="B39" s="9">
+        <v>4</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="46" t="s">
+      <c r="E39" s="42" t="s">
         <v>65</v>
       </c>
       <c r="F39" s="1">
@@ -3419,22 +3407,22 @@
       <c r="R39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S39" s="47" t="s">
+      <c r="S39" s="43" t="s">
         <v>22</v>
       </c>
       <c r="T39" s="1"/>
-      <c r="U39" s="11" t="s">
+      <c r="U39" s="10" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="44"/>
-      <c r="B40" s="40">
+      <c r="A40" s="40"/>
+      <c r="B40" s="36">
         <v>5</v>
       </c>
-      <c r="C40" s="10"/>
+      <c r="C40" s="9"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="46" t="s">
+      <c r="E40" s="42" t="s">
         <v>67</v>
       </c>
       <c r="F40" s="1">
@@ -3480,18 +3468,18 @@
         <v>22</v>
       </c>
       <c r="T40" s="1"/>
-      <c r="U40" s="11" t="s">
+      <c r="U40" s="10" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="41" ht="14.25">
-      <c r="A41" s="44"/>
-      <c r="B41" s="40">
+      <c r="A41" s="40"/>
+      <c r="B41" s="36">
         <v>6</v>
       </c>
-      <c r="C41" s="10"/>
+      <c r="C41" s="9"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="46" t="s">
+      <c r="E41" s="42" t="s">
         <v>69</v>
       </c>
       <c r="F41" s="1">
@@ -3537,18 +3525,18 @@
         <v>22</v>
       </c>
       <c r="T41" s="1"/>
-      <c r="U41" s="11"/>
+      <c r="U41" s="10"/>
     </row>
     <row r="42" ht="13.800000000000001">
-      <c r="A42" s="44"/>
-      <c r="B42" s="10">
+      <c r="A42" s="40"/>
+      <c r="B42" s="9">
         <v>7</v>
       </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="22" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="48" t="s">
+      <c r="E42" s="44" t="s">
         <v>71</v>
       </c>
       <c r="F42" s="1">
@@ -3594,18 +3582,18 @@
         <v>22</v>
       </c>
       <c r="T42" s="1"/>
-      <c r="U42" s="11"/>
+      <c r="U42" s="10"/>
     </row>
     <row r="43" ht="13.800000000000001">
-      <c r="A43" s="44"/>
-      <c r="B43" s="10">
+      <c r="A43" s="40"/>
+      <c r="B43" s="9">
         <v>8</v>
       </c>
-      <c r="C43" s="10"/>
+      <c r="C43" s="9"/>
       <c r="D43" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E43" s="48" t="s">
+      <c r="E43" s="44" t="s">
         <v>72</v>
       </c>
       <c r="F43" s="1">
@@ -3651,18 +3639,18 @@
         <v>22</v>
       </c>
       <c r="T43" s="1"/>
-      <c r="U43" s="11"/>
+      <c r="U43" s="10"/>
     </row>
     <row r="44" ht="13.800000000000001">
-      <c r="A44" s="44"/>
-      <c r="B44" s="10">
+      <c r="A44" s="40"/>
+      <c r="B44" s="9">
         <v>9</v>
       </c>
-      <c r="C44" s="10"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="48" t="s">
+      <c r="E44" s="44" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="1">
@@ -3708,18 +3696,18 @@
         <v>22</v>
       </c>
       <c r="T44" s="1"/>
-      <c r="U44" s="11"/>
+      <c r="U44" s="10"/>
     </row>
     <row r="45" ht="14.25">
-      <c r="A45" s="44"/>
-      <c r="B45" s="10">
+      <c r="A45" s="40"/>
+      <c r="B45" s="9">
         <v>10</v>
       </c>
-      <c r="C45" s="10"/>
+      <c r="C45" s="9"/>
       <c r="D45" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="48" t="s">
+      <c r="E45" s="44" t="s">
         <v>74</v>
       </c>
       <c r="F45" s="1">
@@ -3765,73 +3753,73 @@
         <v>22</v>
       </c>
       <c r="T45" s="1"/>
-      <c r="U45" s="11"/>
+      <c r="U45" s="10"/>
     </row>
     <row r="46" ht="13.800000000000001">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>75</v>
       </c>
       <c r="B46" s="3">
         <v>1</v>
       </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="49" t="s">
+      <c r="D46" s="17"/>
+      <c r="E46" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F46" s="18">
+      <c r="F46" s="17">
         <v>160</v>
       </c>
-      <c r="G46" s="18">
+      <c r="G46" s="17">
         <v>100</v>
       </c>
-      <c r="H46" s="18">
-        <v>4</v>
-      </c>
-      <c r="I46" s="18">
-        <v>4</v>
-      </c>
-      <c r="J46" s="18">
+      <c r="H46" s="17">
+        <v>4</v>
+      </c>
+      <c r="I46" s="17">
+        <v>4</v>
+      </c>
+      <c r="J46" s="17">
         <v>32</v>
       </c>
-      <c r="K46" s="18" t="s">
+      <c r="K46" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L46" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M46" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="N46" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="O46" s="18" t="s">
+      <c r="L46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M46" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N46" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="O46" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="P46" s="18" t="s">
+      <c r="P46" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="Q46" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="R46" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="S46" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="T46" s="18"/>
-      <c r="U46" s="20"/>
+      <c r="Q46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="R46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="S46" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T46" s="17"/>
+      <c r="U46" s="19"/>
     </row>
     <row r="47" ht="13.800000000000001">
-      <c r="A47" s="17"/>
-      <c r="B47" s="10">
+      <c r="A47" s="16"/>
+      <c r="B47" s="9">
         <v>2</v>
       </c>
-      <c r="C47" s="10"/>
+      <c r="C47" s="9"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="46" t="s">
         <v>76</v>
       </c>
       <c r="F47" s="1">
@@ -3877,16 +3865,16 @@
         <v>22</v>
       </c>
       <c r="T47" s="1"/>
-      <c r="U47" s="11"/>
+      <c r="U47" s="10"/>
     </row>
     <row r="48" ht="13.800000000000001">
-      <c r="A48" s="17"/>
-      <c r="B48" s="10">
+      <c r="A48" s="16"/>
+      <c r="B48" s="9">
         <v>3</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="9"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="50" t="s">
+      <c r="E48" s="46" t="s">
         <v>77</v>
       </c>
       <c r="F48" s="1">
@@ -3932,16 +3920,16 @@
         <v>22</v>
       </c>
       <c r="T48" s="1"/>
-      <c r="U48" s="11"/>
+      <c r="U48" s="10"/>
     </row>
     <row r="49" ht="13.800000000000001">
-      <c r="A49" s="17"/>
-      <c r="B49" s="10">
-        <v>4</v>
-      </c>
-      <c r="C49" s="10"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="9">
+        <v>4</v>
+      </c>
+      <c r="C49" s="9"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="50" t="s">
+      <c r="E49" s="46" t="s">
         <v>78</v>
       </c>
       <c r="F49" s="1">
@@ -3987,16 +3975,16 @@
         <v>22</v>
       </c>
       <c r="T49" s="1"/>
-      <c r="U49" s="11"/>
+      <c r="U49" s="10"/>
     </row>
     <row r="50" ht="13.800000000000001">
-      <c r="A50" s="17"/>
-      <c r="B50" s="10">
+      <c r="A50" s="16"/>
+      <c r="B50" s="9">
         <v>5</v>
       </c>
-      <c r="C50" s="10"/>
+      <c r="C50" s="9"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="46" t="s">
         <v>79</v>
       </c>
       <c r="F50" s="1">
@@ -4042,16 +4030,16 @@
         <v>22</v>
       </c>
       <c r="T50" s="1"/>
-      <c r="U50" s="11"/>
+      <c r="U50" s="10"/>
     </row>
     <row r="51" ht="13.800000000000001">
-      <c r="A51" s="17"/>
-      <c r="B51" s="10">
+      <c r="A51" s="16"/>
+      <c r="B51" s="9">
         <v>6</v>
       </c>
-      <c r="C51" s="10"/>
+      <c r="C51" s="9"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="51" t="s">
+      <c r="E51" s="47" t="s">
         <v>80</v>
       </c>
       <c r="F51" s="1">
@@ -4097,16 +4085,16 @@
         <v>22</v>
       </c>
       <c r="T51" s="1"/>
-      <c r="U51" s="11"/>
+      <c r="U51" s="10"/>
     </row>
     <row r="52" ht="13.800000000000001">
-      <c r="A52" s="17"/>
-      <c r="B52" s="10">
+      <c r="A52" s="16"/>
+      <c r="B52" s="9">
         <v>7</v>
       </c>
-      <c r="C52" s="10"/>
+      <c r="C52" s="9"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="51" t="s">
+      <c r="E52" s="47" t="s">
         <v>81</v>
       </c>
       <c r="F52" s="1">
@@ -4152,16 +4140,16 @@
         <v>22</v>
       </c>
       <c r="T52" s="1"/>
-      <c r="U52" s="11"/>
+      <c r="U52" s="10"/>
     </row>
     <row r="53" ht="13.800000000000001">
-      <c r="A53" s="17"/>
-      <c r="B53" s="10">
+      <c r="A53" s="16"/>
+      <c r="B53" s="9">
         <v>8</v>
       </c>
-      <c r="C53" s="10"/>
+      <c r="C53" s="9"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="51" t="s">
+      <c r="E53" s="47" t="s">
         <v>82</v>
       </c>
       <c r="F53" s="1">
@@ -4207,16 +4195,16 @@
         <v>22</v>
       </c>
       <c r="T53" s="1"/>
-      <c r="U53" s="11"/>
+      <c r="U53" s="10"/>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="10">
+      <c r="A54" s="16"/>
+      <c r="B54" s="9">
         <v>9</v>
       </c>
-      <c r="C54" s="10"/>
+      <c r="C54" s="9"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="51" t="s">
+      <c r="E54" s="47" t="s">
         <v>83</v>
       </c>
       <c r="F54" s="1">
@@ -4262,266 +4250,266 @@
         <v>22</v>
       </c>
       <c r="T54" s="1"/>
-      <c r="U54" s="11"/>
+      <c r="U54" s="10"/>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="15"/>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55" s="15"/>
-      <c r="U55" s="16"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="14"/>
+      <c r="O55" s="14"/>
+      <c r="P55" s="14"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="15"/>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="52"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6">
+      <c r="D56" s="5"/>
+      <c r="E56" s="5">
         <v>3</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="5">
         <v>1</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G56" s="5">
         <v>1</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H56" s="5">
         <v>1</v>
       </c>
-      <c r="I56" s="6">
+      <c r="I56" s="5">
         <v>2</v>
       </c>
-      <c r="J56" s="6">
+      <c r="J56" s="5">
         <v>2</v>
       </c>
-      <c r="K56" s="6">
+      <c r="K56" s="5">
         <v>2</v>
       </c>
-      <c r="L56" s="6">
+      <c r="L56" s="5">
         <v>2</v>
       </c>
-      <c r="M56" s="6">
+      <c r="M56" s="5">
         <v>2</v>
       </c>
-      <c r="N56" s="6">
+      <c r="N56" s="5">
         <v>1</v>
       </c>
-      <c r="O56" s="6">
+      <c r="O56" s="5">
         <v>2</v>
       </c>
-      <c r="P56" s="6">
+      <c r="P56" s="5">
         <v>3</v>
       </c>
-      <c r="Q56" s="6">
+      <c r="Q56" s="5">
         <v>2</v>
       </c>
-      <c r="R56" s="6">
+      <c r="R56" s="5">
         <v>2</v>
       </c>
-      <c r="S56" s="6">
+      <c r="S56" s="5">
         <v>2</v>
       </c>
-      <c r="T56" s="6"/>
-      <c r="U56" s="53">
+      <c r="T56" s="5"/>
+      <c r="U56" s="49">
         <f>PRODUCT(E56:S56)</f>
         <v>4608</v>
       </c>
     </row>
     <row r="60" ht="13.800000000000001">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="B60" s="55" t="s">
+      <c r="B60" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="C60" s="55" t="s">
+      <c r="C60" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55" t="s">
+      <c r="D60" s="51"/>
+      <c r="E60" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="F60" s="56" t="s">
+      <c r="F60" s="52" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="61" ht="47.25" customHeight="1">
-      <c r="A61" s="57" t="s">
+      <c r="A61" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B61" s="58" t="s">
+      <c r="B61" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="59">
+      <c r="C61" s="55">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D61" s="59"/>
-      <c r="E61" s="59">
+      <c r="D61" s="55"/>
+      <c r="E61" s="55">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F61" s="60">
+      <c r="F61" s="56">
         <v>0.14999999999999999</v>
       </c>
     </row>
     <row r="62" ht="112.5" customHeight="1">
-      <c r="A62" s="57" t="s">
+      <c r="A62" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="61" t="s">
+      <c r="B62" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="62" t="s">
+      <c r="C62" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="D62" s="62"/>
-      <c r="E62" s="63" t="s">
+      <c r="D62" s="58"/>
+      <c r="E62" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="64" t="s">
+      <c r="F62" s="60" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="63" ht="71.25">
-      <c r="A63" s="57" t="s">
+      <c r="A63" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="58" t="s">
+      <c r="B63" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="C63" s="59">
+      <c r="C63" s="55">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D63" s="59"/>
-      <c r="E63" s="59">
+      <c r="D63" s="55"/>
+      <c r="E63" s="55">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F63" s="60">
+      <c r="F63" s="56">
         <v>0.14999999999999999</v>
       </c>
     </row>
     <row r="64" ht="57">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="61" t="s">
+      <c r="B64" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="59">
+      <c r="C64" s="55">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59">
+      <c r="D64" s="55"/>
+      <c r="E64" s="55">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F64" s="60">
+      <c r="F64" s="56">
         <v>0.14999999999999999</v>
       </c>
     </row>
     <row r="65" ht="57">
-      <c r="A65" s="65" t="s">
+      <c r="A65" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="61" t="s">
+      <c r="B65" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="C65" s="59">
+      <c r="C65" s="55">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D65" s="59"/>
-      <c r="E65" s="59">
+      <c r="D65" s="55"/>
+      <c r="E65" s="55">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F65" s="60">
+      <c r="F65" s="56">
         <v>0.14999999999999999</v>
       </c>
     </row>
     <row r="66" ht="42.75">
-      <c r="A66" s="57" t="s">
+      <c r="A66" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="61" t="s">
+      <c r="B66" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="63" t="s">
+      <c r="C66" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63" t="s">
+      <c r="D66" s="59"/>
+      <c r="E66" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="F66" s="64" t="s">
+      <c r="F66" s="60" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="67" ht="114">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="67" t="s">
+      <c r="B67" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="C67" s="62" t="s">
+      <c r="C67" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="D67" s="62"/>
-      <c r="E67" s="68" t="s">
+      <c r="D67" s="58"/>
+      <c r="E67" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F67" s="69" t="s">
+      <c r="F67" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="68" ht="14.25">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="B68" s="62" t="s">
+      <c r="B68" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="63" t="s">
+      <c r="C68" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="D68" s="63"/>
-      <c r="E68" s="68" t="s">
+      <c r="D68" s="59"/>
+      <c r="E68" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="F68" s="69" t="s">
+      <c r="F68" s="65" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="69" ht="14.25">
-      <c r="A69" s="71" t="s">
+      <c r="A69" s="67" t="s">
         <v>103</v>
       </c>
-      <c r="B69" s="72" t="s">
+      <c r="B69" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="C69" s="72" t="s">
+      <c r="C69" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="D69" s="72"/>
-      <c r="E69" s="73" t="s">
+      <c r="D69" s="68"/>
+      <c r="E69" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F69" s="74" t="s">
+      <c r="F69" s="70" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created latest trainings for VAE
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Network</t>
   </si>
@@ -265,6 +265,24 @@
   </si>
   <si>
     <t>LASTEN2A</t>
+  </si>
+  <si>
+    <t>9_euclidean</t>
+  </si>
+  <si>
+    <t>LASTEN2V</t>
+  </si>
+  <si>
+    <t>LASTEN2VL</t>
+  </si>
+  <si>
+    <t>LASTEN2VS</t>
+  </si>
+  <si>
+    <t>LASTEN2VSL</t>
+  </si>
+  <si>
+    <t>LASTENVA</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -367,7 +385,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,8 +524,21 @@
         <bgColor theme="5" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill/>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor theme="3" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -621,6 +652,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="1"/>
       </left>
@@ -666,22 +717,15 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top style="medium">
         <color theme="1"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -833,7 +877,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="85">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -866,33 +910,33 @@
     <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="2" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="3" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -940,10 +984,10 @@
     <xf fontId="0" fillId="17" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="17" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="9" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="17" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="9" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -961,7 +1005,7 @@
     <xf fontId="0" fillId="21" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="22" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="22" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="22" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -970,14 +1014,56 @@
     <xf fontId="0" fillId="23" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="24" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="25" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="26" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="24" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="26" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="24" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="26" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -986,7 +1072,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="21" numFmtId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
@@ -998,28 +1084,19 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1029,12 +1106,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1706,85 +1786,108 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" ht="14.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="12">
-        <v>4</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
+    <row r="5" ht="15.75">
+      <c r="A5" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="13">
+        <v>168</v>
+      </c>
+      <c r="G5" s="13">
+        <v>300</v>
+      </c>
+      <c r="H5" s="13">
+        <v>8</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13">
+        <v>32</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="13" t="b">
+        <f t="shared" ref="L5:L9" si="1">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="U5" s="15"/>
     </row>
     <row r="6" ht="15.75">
-      <c r="A6" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="12"/>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1">
+        <v>168</v>
+      </c>
+      <c r="G6" s="1">
+        <v>300</v>
+      </c>
+      <c r="H6" s="1">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="17">
-        <v>168</v>
-      </c>
-      <c r="G6" s="17">
-        <v>300</v>
-      </c>
-      <c r="H6" s="17">
-        <v>8</v>
-      </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17">
-        <v>32</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6" s="17" t="b">
-        <f t="shared" ref="L6:L35" si="1">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="17" t="s">
+      <c r="M6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" s="19"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" s="10"/>
     </row>
     <row r="7" ht="15.75">
-      <c r="A7" s="16"/>
-      <c r="B7" s="9">
-        <v>2</v>
+      <c r="A7" s="12"/>
+      <c r="B7" s="11">
+        <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>30</v>
@@ -1800,14 +1903,14 @@
         <v>300</v>
       </c>
       <c r="H7" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="L7" s="1" t="b">
         <f t="shared" si="1"/>
@@ -1824,113 +1927,111 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="20" t="s">
-        <v>36</v>
+      <c r="T7" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" ht="15.75">
-      <c r="A8" s="16"/>
-      <c r="B8" s="9">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9" t="s">
+    <row r="8" ht="14.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="17">
+        <v>4</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="19">
         <v>168</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="19">
         <v>300</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="19">
         <v>2</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1">
-        <v>32</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="I8" s="19"/>
+      <c r="J8" s="19">
+        <v>48</v>
+      </c>
+      <c r="K8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="L8" s="1" t="b">
+      <c r="L8" s="19" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="U8" s="10"/>
-    </row>
-    <row r="9" ht="14.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="13">
-        <v>4</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="U8" s="20"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="14">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1">
         <v>168</v>
       </c>
-      <c r="G9" s="14">
-        <v>300</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="G9" s="1">
+        <v>100</v>
+      </c>
+      <c r="H9" s="1">
         <v>2</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14">
-        <v>48</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="14" t="b">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>32</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="14" t="s">
+      <c r="N9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14" t="s">
-        <v>39</v>
-      </c>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
       <c r="U9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="A10" s="12"/>
       <c r="B10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>30</v>
@@ -1952,11 +2053,10 @@
       <c r="J10" s="1">
         <v>32</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>23</v>
+      <c r="K10" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="L10" s="1" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M10" s="1" t="s">
@@ -1965,281 +2065,415 @@
       <c r="N10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="19"/>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="9">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="10"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="19">
+        <v>168</v>
+      </c>
+      <c r="G11" s="19">
+        <v>100</v>
+      </c>
+      <c r="H11" s="19">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19">
+        <v>32</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="20"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13">
+        <v>250</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
+      <c r="I12" s="13">
+        <v>4</v>
+      </c>
+      <c r="J12" s="13">
+        <v>32</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="13"/>
+      <c r="U12" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="C13" s="9"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>250</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4</v>
+      </c>
+      <c r="J13" s="1">
+        <v>32</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P13" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T13" s="1"/>
+      <c r="U13" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="24">
         <v>168</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G14" s="1">
+        <v>300</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4</v>
+      </c>
+      <c r="I14" s="1">
+        <v>4</v>
+      </c>
+      <c r="J14" s="1">
+        <v>32</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="1">
+        <v>51.599499999999999</v>
+      </c>
+      <c r="U14" s="10"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="24">
+        <v>3360</v>
+      </c>
+      <c r="G15" s="1">
         <v>100</v>
       </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1">
-        <v>32</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="10"/>
-    </row>
-    <row r="12" ht="14.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="13">
-        <v>3</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="14">
-        <v>168</v>
-      </c>
-      <c r="G12" s="14">
+      <c r="H15" s="1">
+        <v>4</v>
+      </c>
+      <c r="I15" s="1">
+        <v>4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>32</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T15" s="1"/>
+      <c r="U15" s="10"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9">
+        <v>5</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1">
+        <v>3360</v>
+      </c>
+      <c r="G16" s="1">
         <v>100</v>
       </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14">
-        <v>32</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="15"/>
-    </row>
-    <row r="13" ht="13.800000000000001">
-      <c r="A13" s="16"/>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="19"/>
-    </row>
-    <row r="14" ht="13.800000000000001">
-      <c r="A14" s="16"/>
-      <c r="B14" s="13">
-        <v>2</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="15"/>
-    </row>
-    <row r="15" ht="13.800000000000001">
-      <c r="A15" s="16"/>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="19"/>
-    </row>
-    <row r="16" ht="13.800000000000001">
-      <c r="A16" s="16"/>
-      <c r="B16" s="13">
-        <v>2</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="15"/>
+      <c r="H16" s="1">
+        <v>4</v>
+      </c>
+      <c r="I16" s="1">
+        <v>4</v>
+      </c>
+      <c r="J16" s="1">
+        <v>32</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="1"/>
+      <c r="U16" s="10"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="3">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="17">
-        <v>1</v>
-      </c>
-      <c r="G17" s="17">
-        <v>250</v>
-      </c>
-      <c r="H17" s="17">
-        <v>1</v>
-      </c>
-      <c r="I17" s="17">
-        <v>4</v>
-      </c>
-      <c r="J17" s="17">
-        <v>32</v>
-      </c>
-      <c r="K17" s="17" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="9">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3360</v>
+      </c>
+      <c r="G17" s="1">
+        <v>100</v>
+      </c>
+      <c r="H17" s="1">
+        <v>4</v>
+      </c>
+      <c r="I17" s="26">
+        <v>4</v>
+      </c>
+      <c r="J17" s="27">
+        <v>32</v>
+      </c>
+      <c r="K17" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" s="17" t="s">
+      <c r="L17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="P17" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="S17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T17" s="17"/>
-      <c r="U17" s="19" t="s">
-        <v>48</v>
-      </c>
+      <c r="P17" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q17" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="S17" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="10"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>3360</v>
       </c>
       <c r="G18" s="1">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I18" s="1">
         <v>4</v>
@@ -2253,16 +2487,16 @@
       <c r="L18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>49</v>
+      <c r="M18" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="N18" s="30" t="s">
+        <v>45</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="23" t="s">
+      <c r="P18" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Q18" s="1" t="s">
@@ -2275,25 +2509,23 @@
         <v>22</v>
       </c>
       <c r="T18" s="1"/>
-      <c r="U18" s="10" t="s">
-        <v>51</v>
-      </c>
+      <c r="U18" s="10"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="24">
-        <v>168</v>
+        <v>53</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3360</v>
       </c>
       <c r="G19" s="1">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1">
         <v>4</v>
@@ -2319,8 +2551,8 @@
       <c r="O19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>50</v>
+      <c r="P19" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>22</v>
@@ -2331,22 +2563,20 @@
       <c r="S19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T19" s="1">
-        <v>51.599499999999999</v>
-      </c>
+      <c r="T19" s="1"/>
       <c r="U19" s="10"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="24">
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="1">
         <v>3360</v>
       </c>
       <c r="G20" s="1">
@@ -2376,30 +2606,24 @@
       <c r="O20" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="P20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="10"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="25" t="s">
-        <v>43</v>
+      <c r="E21" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="F21" s="1">
         <v>3360</v>
@@ -2431,29 +2655,25 @@
       <c r="O21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="P21" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
       <c r="T21" s="1"/>
-      <c r="U21" s="10"/>
+      <c r="U21" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F22" s="1">
@@ -2465,46 +2685,46 @@
       <c r="H22" s="1">
         <v>4</v>
       </c>
-      <c r="I22" s="26">
-        <v>4</v>
-      </c>
-      <c r="J22" s="27">
-        <v>32</v>
-      </c>
-      <c r="K22" s="28" t="s">
+      <c r="I22" s="1">
+        <v>4</v>
+      </c>
+      <c r="J22" s="1">
+        <v>32</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="N22" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="O22" s="31" t="s">
+      <c r="L22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P22" s="32" t="s">
+      <c r="P22" s="1" t="s">
         <v>50</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="R22" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="S22" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>22</v>
       </c>
       <c r="T22" s="1"/>
       <c r="U22" s="10"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="9">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="1"/>
@@ -2532,11 +2752,11 @@
       <c r="L23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="N23" s="30" t="s">
-        <v>45</v>
+      <c r="M23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>46</v>
@@ -2544,8 +2764,8 @@
       <c r="P23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>22</v>
+      <c r="Q23" s="33" t="s">
+        <v>59</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>22</v>
@@ -2557,9 +2777,9 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="9">
-        <v>8</v>
+      <c r="A24" s="12"/>
+      <c r="B24" s="36">
+        <v>13</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="1"/>
@@ -2593,11 +2813,11 @@
       <c r="N24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P24" s="32" t="s">
-        <v>54</v>
+      <c r="O24" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>22</v>
@@ -2609,12 +2829,14 @@
         <v>22</v>
       </c>
       <c r="T24" s="1"/>
-      <c r="U24" s="10"/>
+      <c r="U24" s="10" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="9">
-        <v>9</v>
+      <c r="A25" s="12"/>
+      <c r="B25" s="37">
+        <v>14</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="1"/>
@@ -2627,14 +2849,12 @@
       <c r="G25" s="1">
         <v>100</v>
       </c>
-      <c r="H25" s="1">
-        <v>4</v>
-      </c>
+      <c r="H25" s="1"/>
       <c r="I25" s="1">
         <v>4</v>
       </c>
-      <c r="J25" s="1">
-        <v>32</v>
+      <c r="J25" s="27">
+        <v>48</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>44</v>
@@ -2651,19 +2871,25 @@
       <c r="O25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P25" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
+      <c r="P25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="T25" s="1"/>
       <c r="U25" s="10"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="9">
-        <v>10</v>
+      <c r="A26" s="12"/>
+      <c r="B26" s="37">
+        <v>15</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="1"/>
@@ -2676,17 +2902,15 @@
       <c r="G26" s="1">
         <v>100</v>
       </c>
-      <c r="H26" s="1">
-        <v>4</v>
-      </c>
+      <c r="H26" s="1"/>
       <c r="I26" s="1">
         <v>4</v>
       </c>
       <c r="J26" s="1">
         <v>32</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>44</v>
+      <c r="K26" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>22</v>
@@ -2700,21 +2924,25 @@
       <c r="O26" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P26" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
+      <c r="P26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="T26" s="1"/>
-      <c r="U26" s="10" t="s">
-        <v>57</v>
-      </c>
+      <c r="U26" s="10"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="9">
-        <v>11</v>
+      <c r="A27" s="12"/>
+      <c r="B27" s="37">
+        <v>16</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="1"/>
@@ -2727,11 +2955,9 @@
       <c r="G27" s="1">
         <v>100</v>
       </c>
-      <c r="H27" s="1">
-        <v>4</v>
-      </c>
-      <c r="I27" s="1">
-        <v>4</v>
+      <c r="H27" s="1"/>
+      <c r="I27" s="26">
+        <v>6</v>
       </c>
       <c r="J27" s="1">
         <v>32</v>
@@ -2754,8 +2980,8 @@
       <c r="P27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q27" s="33" t="s">
-        <v>58</v>
+      <c r="Q27" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>22</v>
@@ -2767,9 +2993,9 @@
       <c r="U27" s="10"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="9">
-        <v>12</v>
+      <c r="A28" s="12"/>
+      <c r="B28" s="37">
+        <v>17</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="1"/>
@@ -2782,9 +3008,7 @@
       <c r="G28" s="1">
         <v>100</v>
       </c>
-      <c r="H28" s="1">
-        <v>4</v>
-      </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="1">
         <v>4</v>
       </c>
@@ -2809,22 +3033,23 @@
       <c r="P28" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q28" s="33" t="s">
-        <v>59</v>
+      <c r="Q28" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="R28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S28" s="1" t="s">
-        <v>22</v>
+      <c r="S28" s="35" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="T28" s="1"/>
       <c r="U28" s="10"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="36">
-        <v>13</v>
+      <c r="A29" s="12"/>
+      <c r="B29" s="37">
+        <v>18</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="1"/>
@@ -2837,9 +3062,7 @@
       <c r="G29" s="1">
         <v>100</v>
       </c>
-      <c r="H29" s="1">
-        <v>4</v>
-      </c>
+      <c r="H29" s="1"/>
       <c r="I29" s="1">
         <v>4</v>
       </c>
@@ -2858,8 +3081,8 @@
       <c r="N29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O29" s="31" t="s">
-        <v>60</v>
+      <c r="O29" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>50</v>
@@ -2867,94 +3090,98 @@
       <c r="Q29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R29" s="1" t="s">
-        <v>22</v>
+      <c r="R29" s="34" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="T29" s="1"/>
-      <c r="U29" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="U29" s="10"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="37">
-        <v>14</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="38">
+        <v>19</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="19">
         <v>3360</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="19">
         <v>100</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1">
-        <v>4</v>
-      </c>
-      <c r="J30" s="27">
-        <v>48</v>
-      </c>
-      <c r="K30" s="1" t="s">
+      <c r="H30" s="19"/>
+      <c r="I30" s="19">
+        <v>4</v>
+      </c>
+      <c r="J30" s="19">
+        <v>32</v>
+      </c>
+      <c r="K30" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="L30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O30" s="1" t="s">
+      <c r="L30" s="39" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="P30" s="1" t="s">
+      <c r="P30" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T30" s="1"/>
-      <c r="U30" s="10"/>
+      <c r="Q30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="S30" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="T30" s="19"/>
+      <c r="U30" s="20"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="37">
-        <v>15</v>
+      <c r="A31" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="F31" s="1">
-        <v>3360</v>
+        <v>168</v>
       </c>
       <c r="G31" s="1">
         <v>100</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="41">
+        <v>2</v>
+      </c>
       <c r="I31" s="1">
         <v>4</v>
       </c>
       <c r="J31" s="1">
         <v>32</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="L31" s="1" t="s">
@@ -2970,7 +3197,7 @@
         <v>46</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>22</v>
@@ -2985,30 +3212,32 @@
       <c r="U31" s="10"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="37">
-        <v>16</v>
+      <c r="A32" s="40"/>
+      <c r="B32" s="9">
+        <v>2</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>53</v>
+      <c r="E32" s="42" t="s">
+        <v>31</v>
       </c>
       <c r="F32" s="1">
-        <v>3360</v>
+        <v>168</v>
       </c>
       <c r="G32" s="1">
         <v>100</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="26">
-        <v>6</v>
+      <c r="H32" s="41">
+        <v>4</v>
+      </c>
+      <c r="I32" s="1">
+        <v>4</v>
       </c>
       <c r="J32" s="1">
         <v>32</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>22</v>
@@ -3023,7 +3252,7 @@
         <v>46</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>22</v>
@@ -3038,14 +3267,16 @@
       <c r="U32" s="10"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="37">
-        <v>17</v>
+      <c r="A33" s="40"/>
+      <c r="B33" s="9">
+        <v>3</v>
       </c>
       <c r="C33" s="9"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>53</v>
+      <c r="D33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="42" t="s">
+        <v>64</v>
       </c>
       <c r="F33" s="1">
         <v>3360</v>
@@ -3053,7 +3284,9 @@
       <c r="G33" s="1">
         <v>100</v>
       </c>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1">
+        <v>4</v>
+      </c>
       <c r="I33" s="1">
         <v>4</v>
       </c>
@@ -3061,7 +3294,7 @@
         <v>32</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>22</v>
@@ -3076,7 +3309,7 @@
         <v>46</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>22</v>
@@ -3084,22 +3317,23 @@
       <c r="R33" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S33" s="35" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+      <c r="S33" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="10"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="37">
-        <v>18</v>
+      <c r="A34" s="40"/>
+      <c r="B34" s="9">
+        <v>4</v>
       </c>
       <c r="C34" s="9"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>53</v>
+      <c r="D34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>65</v>
       </c>
       <c r="F34" s="1">
         <v>3360</v>
@@ -3107,7 +3341,9 @@
       <c r="G34" s="1">
         <v>100</v>
       </c>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1">
+        <v>4</v>
+      </c>
       <c r="I34" s="1">
         <v>4</v>
       </c>
@@ -3115,7 +3351,7 @@
         <v>32</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>22</v>
@@ -3130,95 +3366,97 @@
         <v>46</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R34" s="34" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="S34" s="1" t="s">
+      <c r="R34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S34" s="43" t="s">
         <v>22</v>
       </c>
       <c r="T34" s="1"/>
-      <c r="U34" s="10"/>
+      <c r="U34" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="35" ht="14.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="38">
-        <v>19</v>
-      </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F35" s="14">
-        <v>3360</v>
-      </c>
-      <c r="G35" s="14">
+      <c r="A35" s="40"/>
+      <c r="B35" s="36">
+        <v>5</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1680</v>
+      </c>
+      <c r="G35" s="1">
         <v>100</v>
       </c>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14">
-        <v>4</v>
-      </c>
-      <c r="J35" s="14">
-        <v>32</v>
-      </c>
-      <c r="K35" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="L35" s="39" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="M35" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N35" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="O35" s="14" t="s">
+      <c r="H35" s="1">
+        <v>4</v>
+      </c>
+      <c r="I35" s="1">
+        <v>4</v>
+      </c>
+      <c r="J35" s="1">
+        <v>32</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P35" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="R35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="S35" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="T35" s="14"/>
-      <c r="U35" s="15"/>
+      <c r="P35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T35" s="1"/>
+      <c r="U35" s="10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="9">
-        <v>1</v>
+      <c r="A36" s="40"/>
+      <c r="B36" s="36">
+        <v>6</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>31</v>
+      <c r="E36" s="42" t="s">
+        <v>69</v>
       </c>
       <c r="F36" s="1">
-        <v>168</v>
+        <v>3528</v>
       </c>
       <c r="G36" s="1">
         <v>100</v>
       </c>
-      <c r="H36" s="41">
-        <v>2</v>
+      <c r="H36" s="1">
+        <v>4</v>
       </c>
       <c r="I36" s="1">
         <v>4</v>
@@ -3256,23 +3494,25 @@
       <c r="T36" s="1"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" ht="14.25">
+    <row r="37" ht="13.800000000000001">
       <c r="A37" s="40"/>
       <c r="B37" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C37" s="9"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="42" t="s">
-        <v>31</v>
+      <c r="D37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="44" t="s">
+        <v>71</v>
       </c>
       <c r="F37" s="1">
-        <v>168</v>
+        <v>336</v>
       </c>
       <c r="G37" s="1">
         <v>100</v>
       </c>
-      <c r="H37" s="41">
+      <c r="H37" s="1">
         <v>4</v>
       </c>
       <c r="I37" s="1">
@@ -3311,20 +3551,20 @@
       <c r="T37" s="1"/>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" ht="14.25">
+    <row r="38" ht="13.800000000000001">
       <c r="A38" s="40"/>
       <c r="B38" s="9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>72</v>
       </c>
       <c r="F38" s="1">
-        <v>3360</v>
+        <v>336</v>
       </c>
       <c r="G38" s="1">
         <v>100</v>
@@ -3368,20 +3608,20 @@
       <c r="T38" s="1"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" ht="14.25">
+    <row r="39" ht="13.800000000000001">
       <c r="A39" s="40"/>
       <c r="B39" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>73</v>
       </c>
       <c r="F39" s="1">
-        <v>3360</v>
+        <v>336</v>
       </c>
       <c r="G39" s="1">
         <v>100</v>
@@ -3419,26 +3659,26 @@
       <c r="R39" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S39" s="43" t="s">
+      <c r="S39" s="1" t="s">
         <v>22</v>
       </c>
       <c r="T39" s="1"/>
-      <c r="U39" s="10" t="s">
-        <v>66</v>
-      </c>
+      <c r="U39" s="10"/>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="40"/>
-      <c r="B40" s="36">
-        <v>5</v>
+      <c r="B40" s="9">
+        <v>10</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="42" t="s">
-        <v>67</v>
+      <c r="D40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>74</v>
       </c>
       <c r="F40" s="1">
-        <v>1680</v>
+        <v>336</v>
       </c>
       <c r="G40" s="1">
         <v>100</v>
@@ -3480,79 +3720,77 @@
         <v>22</v>
       </c>
       <c r="T40" s="1"/>
-      <c r="U40" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="36">
-        <v>6</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="1">
-        <v>3528</v>
-      </c>
-      <c r="G41" s="1">
+      <c r="U40" s="10"/>
+    </row>
+    <row r="41" ht="13.800000000000001">
+      <c r="A41" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="13">
+        <v>160</v>
+      </c>
+      <c r="G41" s="13">
         <v>100</v>
       </c>
-      <c r="H41" s="1">
-        <v>4</v>
-      </c>
-      <c r="I41" s="1">
-        <v>4</v>
-      </c>
-      <c r="J41" s="1">
-        <v>32</v>
-      </c>
-      <c r="K41" s="1" t="s">
+      <c r="H41" s="13">
+        <v>4</v>
+      </c>
+      <c r="I41" s="13">
+        <v>4</v>
+      </c>
+      <c r="J41" s="13">
+        <v>32</v>
+      </c>
+      <c r="K41" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O41" s="1" t="s">
+      <c r="L41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N41" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O41" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="P41" s="1" t="s">
+      <c r="P41" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="Q41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S41" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T41" s="1"/>
-      <c r="U41" s="10"/>
+      <c r="Q41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S41" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="T41" s="13"/>
+      <c r="U41" s="15"/>
     </row>
     <row r="42" ht="13.800000000000001">
-      <c r="A42" s="40"/>
+      <c r="A42" s="12"/>
       <c r="B42" s="9">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42" s="9"/>
-      <c r="D42" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E42" s="44" t="s">
-        <v>71</v>
+      <c r="D42" s="1"/>
+      <c r="E42" s="46" t="s">
+        <v>76</v>
       </c>
       <c r="F42" s="1">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="G42" s="1">
         <v>100</v>
@@ -3597,19 +3835,17 @@
       <c r="U42" s="10"/>
     </row>
     <row r="43" ht="13.800000000000001">
-      <c r="A43" s="40"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="9">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43" s="9"/>
-      <c r="D43" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="44" t="s">
-        <v>72</v>
+      <c r="D43" s="1"/>
+      <c r="E43" s="46" t="s">
+        <v>77</v>
       </c>
       <c r="F43" s="1">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="G43" s="1">
         <v>100</v>
@@ -3654,19 +3890,17 @@
       <c r="U43" s="10"/>
     </row>
     <row r="44" ht="13.800000000000001">
-      <c r="A44" s="40"/>
+      <c r="A44" s="12"/>
       <c r="B44" s="9">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44" s="9"/>
-      <c r="D44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="44" t="s">
-        <v>73</v>
+      <c r="D44" s="1"/>
+      <c r="E44" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="F44" s="1">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="G44" s="1">
         <v>100</v>
@@ -3710,20 +3944,18 @@
       <c r="T44" s="1"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" ht="14.25">
-      <c r="A45" s="40"/>
+    <row r="45" ht="13.800000000000001">
+      <c r="A45" s="12"/>
       <c r="B45" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" s="9"/>
-      <c r="D45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E45" s="44" t="s">
-        <v>74</v>
+      <c r="D45" s="1"/>
+      <c r="E45" s="46" t="s">
+        <v>79</v>
       </c>
       <c r="F45" s="1">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="G45" s="1">
         <v>100</v>
@@ -3768,71 +4000,69 @@
       <c r="U45" s="10"/>
     </row>
     <row r="46" ht="13.800000000000001">
-      <c r="A46" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="F46" s="17">
-        <v>160</v>
-      </c>
-      <c r="G46" s="17">
+      <c r="A46" s="12"/>
+      <c r="B46" s="9">
+        <v>6</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="F46" s="1">
+        <v>320</v>
+      </c>
+      <c r="G46" s="1">
         <v>100</v>
       </c>
-      <c r="H46" s="17">
-        <v>4</v>
-      </c>
-      <c r="I46" s="17">
-        <v>4</v>
-      </c>
-      <c r="J46" s="17">
-        <v>32</v>
-      </c>
-      <c r="K46" s="17" t="s">
+      <c r="H46" s="1">
+        <v>4</v>
+      </c>
+      <c r="I46" s="1">
+        <v>4</v>
+      </c>
+      <c r="J46" s="1">
+        <v>32</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L46" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="M46" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="O46" s="17" t="s">
+      <c r="L46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O46" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P46" s="17" t="s">
+      <c r="P46" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q46" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="R46" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="S46" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="T46" s="17"/>
-      <c r="U46" s="19"/>
+      <c r="Q46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T46" s="1"/>
+      <c r="U46" s="10"/>
     </row>
     <row r="47" ht="13.800000000000001">
-      <c r="A47" s="16"/>
+      <c r="A47" s="12"/>
       <c r="B47" s="9">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="46" t="s">
-        <v>76</v>
+      <c r="E47" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="F47" s="1">
         <v>320</v>
@@ -3880,14 +4110,14 @@
       <c r="U47" s="10"/>
     </row>
     <row r="48" ht="13.800000000000001">
-      <c r="A48" s="16"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="9">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="46" t="s">
-        <v>77</v>
+      <c r="E48" s="47" t="s">
+        <v>82</v>
       </c>
       <c r="F48" s="1">
         <v>320</v>
@@ -3934,18 +4164,18 @@
       <c r="T48" s="1"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" ht="13.800000000000001">
-      <c r="A49" s="16"/>
+    <row r="49" ht="14.25">
+      <c r="A49" s="12"/>
       <c r="B49" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="46" t="s">
-        <v>78</v>
+      <c r="E49" s="47" t="s">
+        <v>83</v>
       </c>
       <c r="F49" s="1">
-        <v>320</v>
+        <v>3200</v>
       </c>
       <c r="G49" s="1">
         <v>100</v>
@@ -3989,18 +4219,18 @@
       <c r="T49" s="1"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" ht="13.800000000000001">
-      <c r="A50" s="16"/>
+    <row r="50" ht="14.25">
+      <c r="A50" s="12"/>
       <c r="B50" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="46" t="s">
-        <v>79</v>
+      <c r="E50" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="F50" s="1">
-        <v>320</v>
+        <v>3200</v>
       </c>
       <c r="G50" s="1">
         <v>100</v>
@@ -4014,8 +4244,8 @@
       <c r="J50" s="1">
         <v>32</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>23</v>
+      <c r="K50" s="49" t="s">
+        <v>37</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>22</v>
@@ -4044,18 +4274,18 @@
       <c r="T50" s="1"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" ht="13.800000000000001">
-      <c r="A51" s="16"/>
+    <row r="51" ht="14.25">
+      <c r="A51" s="40"/>
       <c r="B51" s="9">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="47" t="s">
-        <v>80</v>
+      <c r="E51" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="F51" s="1">
-        <v>320</v>
+        <v>3200</v>
       </c>
       <c r="G51" s="1">
         <v>100</v>
@@ -4093,79 +4323,81 @@
       <c r="R51" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S51" s="1" t="s">
-        <v>22</v>
+      <c r="S51" s="50" t="b">
+        <v>1</v>
       </c>
       <c r="T51" s="1"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" ht="13.800000000000001">
-      <c r="A52" s="16"/>
-      <c r="B52" s="9">
-        <v>7</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="F52" s="1">
-        <v>320</v>
-      </c>
-      <c r="G52" s="1">
+    <row r="52" ht="14.25">
+      <c r="A52" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="8">
+        <v>1</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52" s="13">
+        <v>3200</v>
+      </c>
+      <c r="G52" s="13">
         <v>100</v>
       </c>
-      <c r="H52" s="1">
-        <v>4</v>
-      </c>
-      <c r="I52" s="1">
-        <v>4</v>
-      </c>
-      <c r="J52" s="1">
-        <v>32</v>
-      </c>
-      <c r="K52" s="1" t="s">
+      <c r="H52" s="13">
+        <v>4</v>
+      </c>
+      <c r="I52" s="13">
+        <v>4</v>
+      </c>
+      <c r="J52" s="13">
+        <v>32</v>
+      </c>
+      <c r="K52" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N52" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O52" s="1" t="s">
+      <c r="L52" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="M52" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="N52" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="O52" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="P52" s="1" t="s">
+      <c r="P52" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="Q52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T52" s="1"/>
-      <c r="U52" s="10"/>
-    </row>
-    <row r="53" ht="13.800000000000001">
-      <c r="A53" s="16"/>
-      <c r="B53" s="9">
-        <v>8</v>
-      </c>
-      <c r="C53" s="9"/>
+      <c r="Q52" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="R52" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="S52" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="T52" s="13"/>
+      <c r="U52" s="15"/>
+    </row>
+    <row r="53" ht="14.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="11">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="47" t="s">
-        <v>82</v>
+      <c r="E53" s="55" t="s">
+        <v>86</v>
       </c>
       <c r="F53" s="1">
-        <v>320</v>
+        <v>3200</v>
       </c>
       <c r="G53" s="1">
         <v>100</v>
@@ -4179,48 +4411,48 @@
       <c r="J53" s="1">
         <v>32</v>
       </c>
-      <c r="K53" s="1" t="s">
+      <c r="K53" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O53" s="1" t="s">
+      <c r="L53" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="M53" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="N53" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="O53" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="P53" s="1" t="s">
+      <c r="P53" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="Q53" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R53" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S53" s="1" t="s">
+      <c r="Q53" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="R53" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="S53" s="57" t="s">
         <v>22</v>
       </c>
       <c r="T53" s="1"/>
       <c r="U53" s="10"/>
     </row>
     <row r="54" ht="14.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="9">
-        <v>9</v>
-      </c>
-      <c r="C54" s="9"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="11">
+        <v>3</v>
+      </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="47" t="s">
-        <v>83</v>
+      <c r="E54" s="55" t="s">
+        <v>87</v>
       </c>
       <c r="F54" s="1">
-        <v>3200</v>
+        <v>1600</v>
       </c>
       <c r="G54" s="1">
         <v>100</v>
@@ -4237,7 +4469,7 @@
       <c r="K54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="1" t="s">
+      <c r="L54" s="56" t="s">
         <v>22</v>
       </c>
       <c r="M54" s="1" t="s">
@@ -4258,283 +4490,458 @@
       <c r="R54" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="S54" s="48" t="s">
         <v>22</v>
       </c>
       <c r="T54" s="1"/>
       <c r="U54" s="10"/>
     </row>
     <row r="55" ht="14.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
-      <c r="T55" s="14"/>
-      <c r="U55" s="15"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="11">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="1">
+        <v>1600</v>
+      </c>
+      <c r="G55" s="1">
+        <v>100</v>
+      </c>
+      <c r="H55" s="1">
+        <v>4</v>
+      </c>
+      <c r="I55" s="1">
+        <v>4</v>
+      </c>
+      <c r="J55" s="1">
+        <v>32</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L55" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R55" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S55" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T55" s="1"/>
+      <c r="U55" s="10"/>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="48"/>
-      <c r="B56" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="4"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5">
+      <c r="A56" s="58"/>
+      <c r="B56" s="17">
+        <v>5</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" s="19">
+        <v>6240</v>
+      </c>
+      <c r="G56" s="1">
+        <v>100</v>
+      </c>
+      <c r="H56" s="19">
+        <v>4</v>
+      </c>
+      <c r="I56" s="19">
+        <v>4</v>
+      </c>
+      <c r="J56" s="1">
+        <v>32</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S56" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T56" s="19"/>
+      <c r="U56" s="20"/>
+    </row>
+    <row r="57" ht="14.25">
+      <c r="A57" s="61"/>
+      <c r="B57" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="5">
         <v>3</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F57" s="5">
         <v>1</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G57" s="5">
         <v>1</v>
       </c>
-      <c r="H56" s="5">
+      <c r="H57" s="5">
         <v>1</v>
       </c>
-      <c r="I56" s="5">
+      <c r="I57" s="5">
         <v>2</v>
       </c>
-      <c r="J56" s="5">
+      <c r="J57" s="5">
         <v>2</v>
       </c>
-      <c r="K56" s="5">
+      <c r="K57" s="5">
         <v>2</v>
       </c>
-      <c r="L56" s="5">
+      <c r="L57" s="5">
         <v>2</v>
       </c>
-      <c r="M56" s="5">
+      <c r="M57" s="5">
         <v>2</v>
       </c>
-      <c r="N56" s="5">
+      <c r="N57" s="5">
         <v>1</v>
       </c>
-      <c r="O56" s="5">
+      <c r="O57" s="5">
         <v>2</v>
       </c>
-      <c r="P56" s="5">
+      <c r="P57" s="5">
         <v>3</v>
       </c>
-      <c r="Q56" s="5">
+      <c r="Q57" s="5">
         <v>2</v>
       </c>
-      <c r="R56" s="5">
+      <c r="R57" s="5">
         <v>2</v>
       </c>
-      <c r="S56" s="5">
+      <c r="S57" s="5">
         <v>2</v>
       </c>
-      <c r="T56" s="5"/>
-      <c r="U56" s="49">
-        <f>PRODUCT(E56:S56)</f>
+      <c r="T57" s="5"/>
+      <c r="U57" s="63">
+        <f>PRODUCT(E57:S57)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="60" ht="13.800000000000001">
-      <c r="A60" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B60" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="C60" s="51" t="s">
+    <row r="58" ht="14.25">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+      <c r="H58"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+      <c r="O58"/>
+      <c r="P58"/>
+      <c r="Q58"/>
+      <c r="R58"/>
+      <c r="S58"/>
+      <c r="U58"/>
+    </row>
+    <row r="59" ht="14.25">
+      <c r="A59"/>
+      <c r="B59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+      <c r="H59"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="U59"/>
+    </row>
+    <row r="60" ht="14.25">
+      <c r="A60"/>
+      <c r="B60"/>
+      <c r="E60"/>
+      <c r="F60"/>
+      <c r="G60"/>
+      <c r="H60"/>
+      <c r="I60"/>
+      <c r="J60"/>
+      <c r="K60"/>
+      <c r="L60"/>
+      <c r="M60"/>
+      <c r="N60"/>
+      <c r="O60"/>
+      <c r="P60"/>
+      <c r="Q60"/>
+      <c r="R60"/>
+      <c r="S60"/>
+      <c r="U60"/>
+    </row>
+    <row r="61" ht="13.800000000000001">
+      <c r="A61" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="65" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="F60" s="52" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" ht="47.25" customHeight="1">
-      <c r="A61" s="53" t="s">
+      <c r="D61" s="65"/>
+      <c r="E61" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61"/>
+      <c r="H61"/>
+      <c r="I61"/>
+      <c r="J61"/>
+      <c r="K61"/>
+      <c r="L61"/>
+      <c r="M61"/>
+      <c r="N61"/>
+      <c r="O61"/>
+      <c r="P61"/>
+      <c r="Q61"/>
+      <c r="R61"/>
+      <c r="S61"/>
+      <c r="U61"/>
+    </row>
+    <row r="62" ht="47.25" customHeight="1">
+      <c r="A62" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="B61" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="55">
+      <c r="B62" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="69">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55">
+      <c r="D62" s="69"/>
+      <c r="E62" s="69">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F61" s="56">
+      <c r="F62" s="70">
         <v>0.14999999999999999</v>
       </c>
-    </row>
-    <row r="62" ht="112.5" customHeight="1">
-      <c r="A62" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="D62" s="58"/>
-      <c r="E62" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" s="60" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="63" ht="71.25">
-      <c r="A63" s="53" t="s">
+      <c r="G62"/>
+      <c r="H62"/>
+      <c r="I62"/>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62"/>
+      <c r="M62"/>
+      <c r="N62"/>
+      <c r="O62"/>
+      <c r="P62"/>
+      <c r="Q62"/>
+      <c r="R62"/>
+      <c r="S62"/>
+      <c r="U62"/>
+    </row>
+    <row r="63" ht="112.5" customHeight="1">
+      <c r="A63" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="72" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="72"/>
+      <c r="E63" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="U63"/>
+    </row>
+    <row r="64" ht="71.25">
+      <c r="A64" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C63" s="55">
+      <c r="B64" s="68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C64" s="69">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55">
+      <c r="D64" s="69"/>
+      <c r="E64" s="69">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F63" s="56">
+      <c r="F64" s="70">
         <v>0.14999999999999999</v>
       </c>
     </row>
-    <row r="64" ht="57">
-      <c r="A64" s="53" t="s">
+    <row r="65" ht="57">
+      <c r="A65" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="55">
+      <c r="B65" s="71" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="69">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D64" s="55"/>
-      <c r="E64" s="55">
+      <c r="D65" s="69"/>
+      <c r="E65" s="69">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F64" s="56">
+      <c r="F65" s="70">
         <v>0.14999999999999999</v>
       </c>
     </row>
-    <row r="65" ht="57">
-      <c r="A65" s="61" t="s">
+    <row r="66" ht="57">
+      <c r="A66" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="57" t="s">
-        <v>96</v>
-      </c>
-      <c r="C65" s="55">
+      <c r="B66" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" s="69">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55">
+      <c r="D66" s="69"/>
+      <c r="E66" s="69">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F65" s="56">
+      <c r="F66" s="70">
         <v>0.14999999999999999</v>
       </c>
     </row>
-    <row r="66" ht="42.75">
-      <c r="A66" s="53" t="s">
+    <row r="67" ht="42.75">
+      <c r="A67" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="57" t="s">
-        <v>97</v>
-      </c>
-      <c r="C66" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="D66" s="59"/>
-      <c r="E66" s="62" t="s">
+      <c r="B67" s="71" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="F67" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" ht="114">
+      <c r="A68" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="77" t="s">
+        <v>108</v>
+      </c>
+      <c r="C68" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="D68" s="72"/>
+      <c r="E68" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="F66" s="63" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="67" ht="114">
-      <c r="A67" s="64" t="s">
+      <c r="F68" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" ht="14.25">
+      <c r="A69" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="B67" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" s="58" t="s">
-        <v>103</v>
-      </c>
-      <c r="D67" s="58"/>
-      <c r="E67" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" ht="14.25">
-      <c r="A68" s="68" t="s">
-        <v>83</v>
-      </c>
-      <c r="B68" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="D68" s="59"/>
-      <c r="E68" s="66" t="s">
-        <v>93</v>
-      </c>
-      <c r="F68" s="67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25">
-      <c r="A69" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="C69" s="70" t="s">
-        <v>107</v>
-      </c>
-      <c r="D69" s="70"/>
-      <c r="E69" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="F69" s="72" t="s">
-        <v>93</v>
+      <c r="C69" s="73" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" s="73"/>
+      <c r="E69" s="78" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25">
+      <c r="A70" s="81" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" s="82" t="s">
+        <v>112</v>
+      </c>
+      <c r="C70" s="82" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" s="82"/>
+      <c r="E70" s="83" t="s">
+        <v>99</v>
+      </c>
+      <c r="F70" s="84" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A35"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="A46:A55"/>
+  <mergeCells count="7">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A30"/>
+    <mergeCell ref="A31:A40"/>
+    <mergeCell ref="A41:A51"/>
+    <mergeCell ref="A52:A56"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Created latest trainings for VAE from ground truth
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>Network</t>
   </si>
@@ -283,6 +283,15 @@
   </si>
   <si>
     <t>LASTENVA</t>
+  </si>
+  <si>
+    <t>10_euclidean</t>
+  </si>
+  <si>
+    <t>LASTEN2VG</t>
+  </si>
+  <si>
+    <t>LASTEN2VGS</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -385,7 +394,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -537,6 +546,12 @@
         <bgColor theme="3" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="29">
     <border>
@@ -720,9 +735,7 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color theme="1"/>
       </bottom>
@@ -877,7 +890,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1029,28 +1042,34 @@
     <xf fontId="0" fillId="26" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="24" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="26" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="27" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="24" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="26" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="24" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="26" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="27" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="24" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1059,7 +1078,6 @@
     <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1"/>
@@ -1767,7 +1785,7 @@
         <v>23</v>
       </c>
       <c r="L4" s="1" t="b">
-        <f>TRUE()</f>
+        <f t="shared" ref="L4:L30" si="1">TRUE()</f>
         <v>1</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -1817,7 +1835,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="13" t="b">
-        <f t="shared" ref="L5:L9" si="1">TRUE()</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M5" s="13" t="s">
@@ -3127,7 +3145,7 @@
         <v>44</v>
       </c>
       <c r="L30" s="39" t="b">
-        <f>TRUE()</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M30" s="19" t="s">
@@ -4356,31 +4374,31 @@
       <c r="J52" s="13">
         <v>32</v>
       </c>
-      <c r="K52" s="53" t="s">
+      <c r="K52" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="L52" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="M52" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="N52" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="O52" s="53" t="s">
+      <c r="L52" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M52" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N52" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O52" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="P52" s="53" t="s">
+      <c r="P52" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="Q52" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="R52" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="S52" s="54" t="s">
+      <c r="Q52" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R52" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="S52" s="53" t="s">
         <v>22</v>
       </c>
       <c r="T52" s="13"/>
@@ -4393,7 +4411,7 @@
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="55" t="s">
+      <c r="E53" s="54" t="s">
         <v>86</v>
       </c>
       <c r="F53" s="1">
@@ -4411,31 +4429,31 @@
       <c r="J53" s="1">
         <v>32</v>
       </c>
-      <c r="K53" s="56" t="s">
+      <c r="K53" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L53" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="M53" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="N53" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="O53" s="56" t="s">
+      <c r="L53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O53" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P53" s="56" t="s">
+      <c r="P53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q53" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="R53" s="56" t="s">
-        <v>22</v>
-      </c>
-      <c r="S53" s="57" t="s">
+      <c r="Q53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S53" s="48" t="s">
         <v>22</v>
       </c>
       <c r="T53" s="1"/>
@@ -4448,7 +4466,7 @@
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="55" t="s">
+      <c r="E54" s="54" t="s">
         <v>87</v>
       </c>
       <c r="F54" s="1">
@@ -4469,7 +4487,7 @@
       <c r="K54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="56" t="s">
+      <c r="L54" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M54" s="1" t="s">
@@ -4503,7 +4521,7 @@
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="55" t="s">
+      <c r="E55" s="54" t="s">
         <v>88</v>
       </c>
       <c r="F55" s="1">
@@ -4524,7 +4542,7 @@
       <c r="K55" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L55" s="56" t="s">
+      <c r="L55" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M55" s="1" t="s">
@@ -4552,25 +4570,25 @@
       <c r="U55" s="10"/>
     </row>
     <row r="56" ht="14.25">
-      <c r="A56" s="58"/>
-      <c r="B56" s="17">
+      <c r="A56" s="7"/>
+      <c r="B56" s="11">
         <v>5</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="59" t="s">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="F56" s="19">
+      <c r="F56" s="1">
         <v>6240</v>
       </c>
       <c r="G56" s="1">
         <v>100</v>
       </c>
-      <c r="H56" s="19">
-        <v>4</v>
-      </c>
-      <c r="I56" s="19">
+      <c r="H56" s="1">
+        <v>4</v>
+      </c>
+      <c r="I56" s="1">
         <v>4</v>
       </c>
       <c r="J56" s="1">
@@ -4579,7 +4597,7 @@
       <c r="K56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L56" s="60" t="s">
+      <c r="L56" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M56" s="1" t="s">
@@ -4603,338 +4621,364 @@
       <c r="S56" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="T56" s="19"/>
-      <c r="U56" s="20"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="10"/>
     </row>
     <row r="57" ht="14.25">
-      <c r="A57" s="61"/>
-      <c r="B57" s="18" t="s">
+      <c r="A57" s="55" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="62"/>
-      <c r="E57" s="5">
+      <c r="B57" s="8">
+        <v>1</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="F57" s="13">
+        <v>3200</v>
+      </c>
+      <c r="G57" s="13">
+        <v>100</v>
+      </c>
+      <c r="H57" s="13">
+        <v>4</v>
+      </c>
+      <c r="I57" s="13">
+        <v>4</v>
+      </c>
+      <c r="J57" s="13">
+        <v>32</v>
+      </c>
+      <c r="K57" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M57" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N57" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O57" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="P57" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q57" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="R57" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="S57" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="T57" s="13"/>
+      <c r="U57" s="15"/>
+    </row>
+    <row r="58" ht="14.25">
+      <c r="A58" s="59"/>
+      <c r="B58" s="17">
+        <v>2</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="19">
+        <v>1600</v>
+      </c>
+      <c r="G58" s="19">
+        <v>100</v>
+      </c>
+      <c r="H58" s="19">
+        <v>4</v>
+      </c>
+      <c r="I58" s="19">
+        <v>4</v>
+      </c>
+      <c r="J58" s="19">
+        <v>32</v>
+      </c>
+      <c r="K58" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L58" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M58" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N58" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O58" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P58" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q58" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="R58" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="S58" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="T58" s="19"/>
+      <c r="U58" s="20"/>
+    </row>
+    <row r="59" ht="14.25">
+      <c r="A59" s="63"/>
+      <c r="B59" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="64"/>
+      <c r="E59" s="19">
         <v>3</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F59" s="19">
         <v>1</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G59" s="19">
         <v>1</v>
       </c>
-      <c r="H57" s="5">
+      <c r="H59" s="19">
         <v>1</v>
       </c>
-      <c r="I57" s="5">
+      <c r="I59" s="19">
         <v>2</v>
       </c>
-      <c r="J57" s="5">
+      <c r="J59" s="19">
         <v>2</v>
       </c>
-      <c r="K57" s="5">
+      <c r="K59" s="19">
         <v>2</v>
       </c>
-      <c r="L57" s="5">
+      <c r="L59" s="19">
         <v>2</v>
       </c>
-      <c r="M57" s="5">
+      <c r="M59" s="19">
         <v>2</v>
       </c>
-      <c r="N57" s="5">
+      <c r="N59" s="19">
         <v>1</v>
       </c>
-      <c r="O57" s="5">
+      <c r="O59" s="19">
         <v>2</v>
       </c>
-      <c r="P57" s="5">
+      <c r="P59" s="19">
         <v>3</v>
       </c>
-      <c r="Q57" s="5">
+      <c r="Q59" s="19">
         <v>2</v>
       </c>
-      <c r="R57" s="5">
+      <c r="R59" s="19">
         <v>2</v>
       </c>
-      <c r="S57" s="5">
+      <c r="S59" s="19">
         <v>2</v>
       </c>
-      <c r="T57" s="5"/>
-      <c r="U57" s="63">
-        <f>PRODUCT(E57:S57)</f>
+      <c r="T59" s="19"/>
+      <c r="U59" s="20">
+        <f>PRODUCT(E59:S59)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="58" ht="14.25">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="E58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
-      <c r="L58"/>
-      <c r="M58"/>
-      <c r="N58"/>
-      <c r="O58"/>
-      <c r="P58"/>
-      <c r="Q58"/>
-      <c r="R58"/>
-      <c r="S58"/>
-      <c r="U58"/>
-    </row>
-    <row r="59" ht="14.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-      <c r="N59"/>
-      <c r="O59"/>
-      <c r="P59"/>
-      <c r="Q59"/>
-      <c r="R59"/>
-      <c r="S59"/>
-      <c r="U59"/>
-    </row>
-    <row r="60" ht="14.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60"/>
-      <c r="L60"/>
-      <c r="M60"/>
-      <c r="N60"/>
-      <c r="O60"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60"/>
-      <c r="U60"/>
-    </row>
-    <row r="61" ht="13.800000000000001">
-      <c r="A61" s="64" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="65" t="s">
-        <v>92</v>
-      </c>
-      <c r="C61" s="65" t="s">
+    <row r="60" ht="14.25"/>
+    <row r="61" ht="14.25"/>
+    <row r="62" ht="14.25"/>
+    <row r="63" ht="13.800000000000001">
+      <c r="A63" s="65" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="65"/>
-      <c r="E61" s="65" t="s">
-        <v>93</v>
-      </c>
-      <c r="F61" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="G61"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61"/>
-      <c r="L61"/>
-      <c r="M61"/>
-      <c r="N61"/>
-      <c r="O61"/>
-      <c r="P61"/>
-      <c r="Q61"/>
-      <c r="R61"/>
-      <c r="S61"/>
-      <c r="U61"/>
-    </row>
-    <row r="62" ht="47.25" customHeight="1">
-      <c r="A62" s="67" t="s">
+      <c r="D63" s="66"/>
+      <c r="E63" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" ht="47.25" customHeight="1">
+      <c r="A64" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="B62" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="C62" s="69">
+      <c r="B64" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="70">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D62" s="69"/>
-      <c r="E62" s="69">
+      <c r="D64" s="70"/>
+      <c r="E64" s="70">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F62" s="70">
+      <c r="F64" s="71">
         <v>0.14999999999999999</v>
       </c>
-      <c r="G62"/>
-      <c r="H62"/>
-      <c r="I62"/>
-      <c r="J62"/>
-      <c r="K62"/>
-      <c r="L62"/>
-      <c r="M62"/>
-      <c r="N62"/>
-      <c r="O62"/>
-      <c r="P62"/>
-      <c r="Q62"/>
-      <c r="R62"/>
-      <c r="S62"/>
-      <c r="U62"/>
-    </row>
-    <row r="63" ht="112.5" customHeight="1">
-      <c r="A63" s="67" t="s">
-        <v>96</v>
-      </c>
-      <c r="B63" s="71" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="D63" s="72"/>
-      <c r="E63" s="73" t="s">
+    </row>
+    <row r="65" ht="112.5" customHeight="1">
+      <c r="A65" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="74" t="s">
-        <v>99</v>
-      </c>
-      <c r="U63"/>
-    </row>
-    <row r="64" ht="71.25">
-      <c r="A64" s="67" t="s">
+      <c r="B65" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="D65" s="73"/>
+      <c r="E65" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="F65" s="75" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" ht="71.25">
+      <c r="A66" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="B64" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="69">
+      <c r="B66" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="70">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D64" s="69"/>
-      <c r="E64" s="69">
+      <c r="D66" s="70"/>
+      <c r="E66" s="70">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F64" s="70">
+      <c r="F66" s="71">
         <v>0.14999999999999999</v>
       </c>
     </row>
-    <row r="65" ht="57">
-      <c r="A65" s="67" t="s">
+    <row r="67" ht="57">
+      <c r="A67" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="B65" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="C65" s="69">
+      <c r="B67" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="C67" s="70">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D65" s="69"/>
-      <c r="E65" s="69">
+      <c r="D67" s="70"/>
+      <c r="E67" s="70">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F65" s="70">
+      <c r="F67" s="71">
         <v>0.14999999999999999</v>
       </c>
     </row>
-    <row r="66" ht="57">
-      <c r="A66" s="75" t="s">
+    <row r="68" ht="57">
+      <c r="A68" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="71" t="s">
+      <c r="B68" s="72" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" s="70">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F68" s="71">
+        <v>0.14999999999999999</v>
+      </c>
+    </row>
+    <row r="69" ht="42.75">
+      <c r="A69" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" s="75" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" ht="114">
+      <c r="A70" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="B70" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="73" t="s">
+        <v>112</v>
+      </c>
+      <c r="D70" s="73"/>
+      <c r="E70" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="69">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D66" s="69"/>
-      <c r="E66" s="69">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F66" s="70">
-        <v>0.14999999999999999</v>
-      </c>
-    </row>
-    <row r="67" ht="42.75">
-      <c r="A67" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="B67" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="C67" s="73" t="s">
+      <c r="F70" s="80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" ht="14.25">
+      <c r="A71" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="F67" s="74" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" ht="114">
-      <c r="A68" s="76" t="s">
-        <v>107</v>
-      </c>
-      <c r="B68" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="C68" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="D68" s="72"/>
-      <c r="E68" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="F68" s="79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="69" ht="14.25">
-      <c r="A69" s="80" t="s">
-        <v>83</v>
-      </c>
-      <c r="B69" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="73" t="s">
-        <v>110</v>
-      </c>
-      <c r="D69" s="73"/>
-      <c r="E69" s="78" t="s">
-        <v>99</v>
-      </c>
-      <c r="F69" s="79" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="70" ht="14.25">
-      <c r="A70" s="81" t="s">
-        <v>111</v>
-      </c>
-      <c r="B70" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="C70" s="82" t="s">
+      <c r="C71" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="D70" s="82"/>
-      <c r="E70" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="F70" s="84" t="s">
-        <v>99</v>
+      <c r="D71" s="74"/>
+      <c r="E71" s="79" t="s">
+        <v>102</v>
+      </c>
+      <c r="F71" s="80" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" ht="14.25">
+      <c r="A72" s="82" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="C72" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="D72" s="83"/>
+      <c r="E72" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="F72" s="85" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A11"/>
@@ -4942,6 +4986,7 @@
     <mergeCell ref="A31:A40"/>
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A57:A58"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Extrapolation and Interpolation for VAE
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <si>
     <t>Network</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>LASTEN2VGI</t>
+  </si>
+  <si>
+    <t>LASTEN2VGIE</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -441,6 +444,15 @@
   </si>
   <si>
     <t xml:space="preserve">Like LASTEN2VGL but interpolated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like LASTEN2VGL but interpolated and extrapolated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1840 images</t>
   </si>
 </sst>
 </file>
@@ -827,7 +839,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="100">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -998,6 +1010,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="28" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="28" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="24" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="28" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1077,11 +1098,14 @@
     <xf fontId="0" fillId="24" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="24" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="24" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
@@ -1534,7 +1558,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="0" width="22"/>
-    <col customWidth="1" min="2" max="2" style="0" width="29.12890625"/>
+    <col customWidth="1" min="2" max="2" style="0" width="45.9296875"/>
     <col customWidth="1" min="3" max="3" style="0" width="10.8515625"/>
     <col customWidth="1" min="4" max="4" style="0" width="31.9296875"/>
     <col customWidth="1" min="5" max="5" style="0" width="24.00390625"/>
@@ -4872,831 +4896,928 @@
       <c r="E62" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="48"/>
+      <c r="F62" s="1">
+        <v>800</v>
+      </c>
+      <c r="G62" s="1">
+        <v>100</v>
+      </c>
+      <c r="H62" s="1">
+        <v>4</v>
+      </c>
+      <c r="I62" s="1">
+        <v>4</v>
+      </c>
+      <c r="J62" s="1">
+        <v>32</v>
+      </c>
+      <c r="K62" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="L62" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="M62" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="N62" s="61" t="s">
+        <v>49</v>
+      </c>
+      <c r="O62" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="P62" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q62" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="R62" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="S62" s="62" t="s">
+        <v>22</v>
+      </c>
       <c r="T62" s="1"/>
       <c r="U62" s="10"/>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="61"/>
-      <c r="B63" s="17">
+      <c r="A63" s="7"/>
+      <c r="B63" s="11">
         <v>3</v>
       </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="62" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="F63" s="19">
-        <v>800</v>
-      </c>
-      <c r="G63" s="19">
+      <c r="F63" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G63" s="1">
         <v>100</v>
       </c>
-      <c r="H63" s="19">
-        <v>4</v>
-      </c>
-      <c r="I63" s="19">
-        <v>4</v>
-      </c>
-      <c r="J63" s="19">
+      <c r="H63" s="1">
+        <v>4</v>
+      </c>
+      <c r="I63" s="1">
+        <v>4</v>
+      </c>
+      <c r="J63" s="1">
         <v>32</v>
       </c>
-      <c r="K63" s="19" t="s">
+      <c r="K63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L63" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M63" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="N63" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O63" s="19" t="s">
+      <c r="L63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O63" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P63" s="19" t="s">
+      <c r="P63" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q63" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="R63" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="S63" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="T63" s="19"/>
-      <c r="U63" s="20"/>
+      <c r="Q63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S63" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T63" s="1"/>
+      <c r="U63" s="10"/>
     </row>
     <row r="64" ht="14.25">
       <c r="A64" s="64"/>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="17">
+        <v>4</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="C64" s="4"/>
-      <c r="D64" s="65"/>
-      <c r="E64" s="19">
+      <c r="F64" s="19">
+        <v>840</v>
+      </c>
+      <c r="G64" s="19">
+        <v>100</v>
+      </c>
+      <c r="H64" s="19">
+        <v>4</v>
+      </c>
+      <c r="I64" s="19">
+        <v>4</v>
+      </c>
+      <c r="J64" s="19">
+        <v>32</v>
+      </c>
+      <c r="K64" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L64" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M64" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N64" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O64" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P64" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q64" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R64" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="S64" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="T64" s="19"/>
+      <c r="U64" s="20"/>
+    </row>
+    <row r="65" ht="14.25">
+      <c r="A65" s="67"/>
+      <c r="B65" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="19">
         <v>3</v>
       </c>
-      <c r="F64" s="5">
+      <c r="F65" s="5">
         <v>1</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G65" s="5">
         <v>1</v>
       </c>
-      <c r="H64" s="5">
+      <c r="H65" s="5">
         <v>1</v>
       </c>
-      <c r="I64" s="5">
+      <c r="I65" s="5">
         <v>2</v>
       </c>
-      <c r="J64" s="5">
+      <c r="J65" s="5">
         <v>2</v>
       </c>
-      <c r="K64" s="5">
+      <c r="K65" s="5">
         <v>2</v>
       </c>
-      <c r="L64" s="5">
+      <c r="L65" s="5">
         <v>2</v>
       </c>
-      <c r="M64" s="5">
+      <c r="M65" s="5">
         <v>2</v>
       </c>
-      <c r="N64" s="5">
+      <c r="N65" s="5">
         <v>1</v>
       </c>
-      <c r="O64" s="5">
+      <c r="O65" s="5">
         <v>2</v>
       </c>
-      <c r="P64" s="5">
+      <c r="P65" s="5">
         <v>3</v>
       </c>
-      <c r="Q64" s="5">
+      <c r="Q65" s="5">
         <v>2</v>
       </c>
-      <c r="R64" s="5">
+      <c r="R65" s="5">
         <v>2</v>
       </c>
-      <c r="S64" s="5">
+      <c r="S65" s="5">
         <v>2</v>
       </c>
-      <c r="T64" s="5"/>
-      <c r="U64" s="66">
-        <f>PRODUCT(E64:S64)</f>
+      <c r="T65" s="5"/>
+      <c r="U65" s="69">
+        <f>PRODUCT(E65:S65)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="65" ht="14.25">
-      <c r="U65" s="67"/>
-    </row>
-    <row r="66" ht="14.25"/>
-    <row r="67" ht="14.25">
-      <c r="A67" s="67"/>
-      <c r="B67" s="67"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="67"/>
-      <c r="F67" s="67"/>
-    </row>
-    <row r="68" ht="13.800000000000001">
-      <c r="A68" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="B68" s="69" t="s">
+    <row r="66" ht="14.25">
+      <c r="U66" s="70"/>
+    </row>
+    <row r="67" ht="14.25"/>
+    <row r="68" ht="14.25">
+      <c r="A68" s="70"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="70"/>
+      <c r="F68" s="70"/>
+    </row>
+    <row r="69" ht="13.800000000000001">
+      <c r="A69" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="70" t="s">
+      <c r="B69" s="72" t="s">
+        <v>102</v>
+      </c>
+      <c r="C69" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D68" s="70" t="s">
-        <v>102</v>
-      </c>
-      <c r="E68" s="66" t="s">
+      <c r="D69" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="F68" s="67"/>
-    </row>
-    <row r="69" ht="47.25" customHeight="1">
-      <c r="A69" s="71" t="s">
+      <c r="E69" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="F69" s="70"/>
+    </row>
+    <row r="70" ht="47.25" customHeight="1">
+      <c r="A70" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="C69" s="73">
+      <c r="B70" s="75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="76">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D69" s="73">
+      <c r="D70" s="76">
         <v>0.14999999999999999</v>
       </c>
-      <c r="E69" s="74">
+      <c r="E70" s="77">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F69" s="67"/>
-    </row>
-    <row r="70" ht="149.30000000000001" customHeight="1">
-      <c r="A70" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="B70" s="75" t="s">
+      <c r="F70" s="70"/>
+    </row>
+    <row r="71" ht="149.30000000000001" customHeight="1">
+      <c r="A71" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="C70" s="76" t="s">
+      <c r="B71" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="D70" s="57" t="s">
+      <c r="C71" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="E70" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F70" s="67"/>
-    </row>
-    <row r="71" ht="71.25">
-      <c r="A71" s="71" t="s">
+      <c r="D71" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F71" s="70"/>
+    </row>
+    <row r="72" ht="71.25">
+      <c r="A72" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="78" t="s">
+      <c r="B72" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" s="82">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D72" s="82">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="E72" s="83">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F72" s="70"/>
+    </row>
+    <row r="73" ht="57">
+      <c r="A73" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" s="82">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D73" s="82">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="E73" s="83">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F73" s="70"/>
+    </row>
+    <row r="74" ht="57">
+      <c r="A74" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="78" t="s">
+        <v>112</v>
+      </c>
+      <c r="C74" s="82">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D74" s="82">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="E74" s="83">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F74" s="70"/>
+    </row>
+    <row r="75" ht="42.75">
+      <c r="A75" s="74" t="s">
+        <v>41</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="E75" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="F75" s="70"/>
+    </row>
+    <row r="76" ht="114">
+      <c r="A76" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="B76" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="79" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="C71" s="79">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D71" s="79">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="E71" s="80">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F71" s="67"/>
-    </row>
-    <row r="72" ht="57">
-      <c r="A72" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B72" s="75" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="79">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D72" s="79">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="E72" s="80">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F72" s="67"/>
-    </row>
-    <row r="73" ht="57">
-      <c r="A73" s="81" t="s">
-        <v>67</v>
-      </c>
-      <c r="B73" s="75" t="s">
+      <c r="E76" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="70"/>
+    </row>
+    <row r="77" ht="14.25">
+      <c r="A77" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="C73" s="79">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D73" s="79">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="E73" s="80">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F73" s="67"/>
-    </row>
-    <row r="74" ht="42.75">
-      <c r="A74" s="71" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="D74" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="E74" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="F74" s="67"/>
-    </row>
-    <row r="75" ht="114">
-      <c r="A75" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="B75" s="78" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="76" t="s">
-        <v>118</v>
-      </c>
-      <c r="D75" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E75" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F75" s="67"/>
-    </row>
-    <row r="76" ht="14.25">
-      <c r="A76" s="71" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="82" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="D76" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E76" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F76" s="67"/>
-    </row>
-    <row r="77" ht="14.25">
-      <c r="A77" s="71" t="s">
+      <c r="C77" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="B77" s="82" t="s">
+      <c r="D77" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E77" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="70"/>
+    </row>
+    <row r="78" ht="14.25">
+      <c r="A78" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="B78" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="D77" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E77" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F77" s="67"/>
-    </row>
-    <row r="78" ht="127.2" customHeight="1">
-      <c r="A78" s="83" t="s">
+      <c r="C78" s="79" t="s">
+        <v>123</v>
+      </c>
+      <c r="D78" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E78" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" s="70"/>
+    </row>
+    <row r="79" ht="127.2" customHeight="1">
+      <c r="A79" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="84" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" s="85" t="s">
-        <v>119</v>
-      </c>
-      <c r="D78" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E78" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F78" s="67"/>
-    </row>
-    <row r="79" ht="70.200000000000003" customHeight="1">
-      <c r="A79" s="83" t="s">
+      <c r="B79" s="87" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E79" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="70"/>
+    </row>
+    <row r="80" ht="70.200000000000003" customHeight="1">
+      <c r="A80" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="B79" s="86" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="D79" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E79" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F79" s="67"/>
-    </row>
-    <row r="80" ht="14.25">
-      <c r="A80" s="83" t="s">
+      <c r="B80" s="89" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E80" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" s="70"/>
+    </row>
+    <row r="81" ht="14.25">
+      <c r="A81" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="B80" s="84" t="s">
-        <v>125</v>
-      </c>
-      <c r="C80" s="85" t="s">
+      <c r="B81" s="87" t="s">
         <v>126</v>
       </c>
-      <c r="D80" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E80" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F80" s="67"/>
-    </row>
-    <row r="81" ht="14.25">
-      <c r="A81" s="83" t="s">
+      <c r="C81" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E81" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F81" s="70"/>
+    </row>
+    <row r="82" ht="14.25">
+      <c r="A82" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="84" t="s">
+      <c r="B82" s="87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" s="88" t="s">
         <v>127</v>
       </c>
-      <c r="C81" s="85" t="s">
-        <v>126</v>
-      </c>
-      <c r="D81" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E81" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F81" s="67"/>
-    </row>
-    <row r="82" ht="14.25">
-      <c r="A82" s="83" t="s">
-        <v>128</v>
-      </c>
-      <c r="B82" s="86" t="s">
+      <c r="D82" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E82" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" s="70"/>
+    </row>
+    <row r="83" ht="14.25">
+      <c r="A83" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="C82" s="85" t="s">
+      <c r="B83" s="89" t="s">
         <v>130</v>
       </c>
-      <c r="D82" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E82" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F82" s="67"/>
-    </row>
-    <row r="83" ht="14.25">
-      <c r="A83" s="83" t="s">
+      <c r="C83" s="88" t="s">
+        <v>131</v>
+      </c>
+      <c r="D83" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F83" s="70"/>
+    </row>
+    <row r="84" ht="14.25">
+      <c r="A84" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="86" t="s">
-        <v>131</v>
-      </c>
-      <c r="C83" s="87" t="s">
-        <v>119</v>
-      </c>
-      <c r="D83" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E83" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F83" s="67"/>
-    </row>
-    <row r="84" ht="14.25">
-      <c r="A84" s="83" t="s">
+      <c r="B84" s="89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84" s="90" t="s">
+        <v>120</v>
+      </c>
+      <c r="D84" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E84" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F84" s="70"/>
+    </row>
+    <row r="85" ht="14.25">
+      <c r="A85" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="86" t="s">
-        <v>132</v>
-      </c>
-      <c r="C84" s="87" t="s">
-        <v>126</v>
-      </c>
-      <c r="D84" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E84" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F84" s="67"/>
-    </row>
-    <row r="85" ht="14.25">
-      <c r="A85" s="83" t="s">
+      <c r="B85" s="89" t="s">
+        <v>133</v>
+      </c>
+      <c r="C85" s="90" t="s">
+        <v>127</v>
+      </c>
+      <c r="D85" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E85" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F85" s="70"/>
+    </row>
+    <row r="86" ht="14.25">
+      <c r="A86" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="B85" s="86" t="s">
-        <v>133</v>
-      </c>
-      <c r="C85" s="87" t="s">
+      <c r="B86" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="D85" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E85" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F85" s="67"/>
-    </row>
-    <row r="86" ht="78.400000000000006" customHeight="1">
-      <c r="A86" s="83" t="s">
+      <c r="C86" s="90" t="s">
+        <v>135</v>
+      </c>
+      <c r="D86" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E86" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F86" s="70"/>
+    </row>
+    <row r="87" ht="78.400000000000006" customHeight="1">
+      <c r="A87" s="86" t="s">
         <v>94</v>
       </c>
-      <c r="B86" s="86" t="s">
-        <v>135</v>
-      </c>
-      <c r="C86" s="87" t="s">
+      <c r="B87" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="D86" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E86" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F86" s="67"/>
-    </row>
-    <row r="87" ht="78.400000000000006" customHeight="1">
-      <c r="A87" s="88" t="s">
+      <c r="C87" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E87" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F87" s="70"/>
+    </row>
+    <row r="88" ht="78.400000000000006" customHeight="1">
+      <c r="A88" s="91" t="s">
         <v>96</v>
-      </c>
-      <c r="B87" s="89" t="s">
-        <v>137</v>
-      </c>
-      <c r="C87" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="D87" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E87" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F87" s="67"/>
-    </row>
-    <row r="88" ht="58.899999999999999" customHeight="1">
-      <c r="A88" s="90" t="s">
-        <v>97</v>
       </c>
       <c r="B88" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="C88" s="85" t="s">
-        <v>134</v>
+      <c r="C88" s="88" t="s">
+        <v>135</v>
       </c>
       <c r="D88" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E88" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="F88" s="67"/>
-    </row>
-    <row r="89" ht="14.25">
+        <v>109</v>
+      </c>
+      <c r="E88" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F88" s="70"/>
+    </row>
+    <row r="89" ht="58.899999999999999" customHeight="1">
       <c r="A89" s="91" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" s="89" t="s">
+        <v>139</v>
+      </c>
+      <c r="C89" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="D89" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="E89" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="F89" s="70"/>
+    </row>
+    <row r="90" ht="58.899999999999999" customHeight="1">
+      <c r="A90" s="92" t="s">
         <v>98</v>
       </c>
-      <c r="B89" s="92" t="s">
-        <v>139</v>
-      </c>
-      <c r="C89" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="D89" s="94" t="s">
-        <v>108</v>
-      </c>
-      <c r="E89" s="95" t="s">
-        <v>108</v>
-      </c>
-      <c r="F89" s="67"/>
-    </row>
-    <row r="90" ht="14.25">
-      <c r="A90" s="67"/>
-      <c r="B90" s="67"/>
-      <c r="C90" s="67"/>
-      <c r="D90" s="67"/>
-      <c r="E90" s="67"/>
-      <c r="F90" s="67"/>
+      <c r="B90" s="93" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="D90" s="57"/>
+      <c r="E90" s="80"/>
+      <c r="F90" s="70"/>
     </row>
     <row r="91" ht="14.25">
-      <c r="A91" s="67"/>
-      <c r="B91" s="67"/>
-      <c r="C91" s="67"/>
-      <c r="D91" s="67"/>
-      <c r="E91" s="67"/>
-      <c r="F91" s="67"/>
+      <c r="A91" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="B91" s="96" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="97" t="s">
+        <v>143</v>
+      </c>
+      <c r="D91" s="98" t="s">
+        <v>109</v>
+      </c>
+      <c r="E91" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="F91" s="70"/>
     </row>
     <row r="92" ht="14.25">
-      <c r="A92" s="67"/>
-      <c r="B92" s="67"/>
-      <c r="C92" s="67"/>
-      <c r="D92" s="67"/>
-      <c r="E92" s="67"/>
-      <c r="F92" s="67"/>
+      <c r="A92" s="70"/>
+      <c r="B92" s="70"/>
+      <c r="C92" s="70"/>
+      <c r="D92" s="70"/>
+      <c r="E92" s="70"/>
+      <c r="F92" s="70"/>
     </row>
     <row r="93" ht="14.25">
-      <c r="A93" s="67"/>
-      <c r="B93" s="67"/>
-      <c r="C93" s="67"/>
-      <c r="D93" s="67"/>
-      <c r="E93" s="67"/>
-      <c r="F93" s="67"/>
+      <c r="A93" s="70"/>
+      <c r="B93" s="70"/>
+      <c r="C93" s="70"/>
+      <c r="D93" s="70"/>
+      <c r="E93" s="70"/>
+      <c r="F93" s="70"/>
     </row>
     <row r="94" ht="14.25">
-      <c r="A94" s="67"/>
-      <c r="B94" s="67"/>
-      <c r="C94" s="67"/>
-      <c r="D94" s="67"/>
-      <c r="E94" s="67"/>
-      <c r="F94" s="67"/>
+      <c r="A94" s="70"/>
+      <c r="B94" s="70"/>
+      <c r="C94" s="70"/>
+      <c r="D94" s="70"/>
+      <c r="E94" s="70"/>
+      <c r="F94" s="70"/>
     </row>
     <row r="95" ht="14.25">
-      <c r="A95" s="67"/>
-      <c r="B95" s="67"/>
-      <c r="C95" s="67"/>
-      <c r="D95" s="67"/>
-      <c r="E95" s="67"/>
-      <c r="F95" s="67"/>
+      <c r="A95" s="70"/>
+      <c r="B95" s="70"/>
+      <c r="C95" s="70"/>
+      <c r="D95" s="70"/>
+      <c r="E95" s="70"/>
+      <c r="F95" s="70"/>
     </row>
     <row r="96" ht="14.25">
-      <c r="A96" s="67"/>
-      <c r="B96" s="67"/>
-      <c r="C96" s="67"/>
-      <c r="D96" s="67"/>
-      <c r="E96" s="67"/>
-      <c r="F96" s="67"/>
+      <c r="A96" s="70"/>
+      <c r="B96" s="70"/>
+      <c r="C96" s="70"/>
+      <c r="D96" s="70"/>
+      <c r="E96" s="70"/>
+      <c r="F96" s="70"/>
     </row>
     <row r="97" ht="14.25">
-      <c r="A97" s="67"/>
-      <c r="B97" s="67"/>
-      <c r="C97" s="67"/>
-      <c r="D97" s="67"/>
-      <c r="E97" s="67"/>
-      <c r="F97" s="67"/>
+      <c r="A97" s="70"/>
+      <c r="B97" s="70"/>
+      <c r="C97" s="70"/>
+      <c r="D97" s="70"/>
+      <c r="E97" s="70"/>
+      <c r="F97" s="70"/>
     </row>
     <row r="98" ht="14.25">
-      <c r="A98" s="67"/>
-      <c r="B98" s="67"/>
-      <c r="C98" s="67"/>
-      <c r="D98" s="67"/>
-      <c r="E98" s="67"/>
-      <c r="F98" s="67"/>
+      <c r="A98" s="70"/>
+      <c r="B98" s="70"/>
+      <c r="C98" s="70"/>
+      <c r="D98" s="70"/>
+      <c r="E98" s="70"/>
+      <c r="F98" s="70"/>
     </row>
     <row r="99" ht="14.25">
-      <c r="A99" s="67"/>
-      <c r="B99" s="67"/>
-      <c r="C99" s="67"/>
-      <c r="D99" s="67"/>
-      <c r="E99" s="67"/>
-      <c r="F99" s="67"/>
+      <c r="A99" s="70"/>
+      <c r="B99" s="70"/>
+      <c r="C99" s="70"/>
+      <c r="D99" s="70"/>
+      <c r="E99" s="70"/>
+      <c r="F99" s="70"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="A100" s="67"/>
-      <c r="B100" s="67"/>
-      <c r="C100" s="67"/>
-      <c r="D100" s="67"/>
-      <c r="E100" s="67"/>
-      <c r="F100" s="67"/>
+      <c r="A100" s="70"/>
+      <c r="B100" s="70"/>
+      <c r="C100" s="70"/>
+      <c r="D100" s="70"/>
+      <c r="E100" s="70"/>
+      <c r="F100" s="70"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="67"/>
-      <c r="B101" s="67"/>
-      <c r="C101" s="67"/>
-      <c r="D101" s="67"/>
-      <c r="E101" s="67"/>
-      <c r="F101" s="67"/>
+      <c r="A101" s="70"/>
+      <c r="B101" s="70"/>
+      <c r="C101" s="70"/>
+      <c r="D101" s="70"/>
+      <c r="E101" s="70"/>
+      <c r="F101" s="70"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="A102" s="67"/>
-      <c r="B102" s="67"/>
-      <c r="C102" s="67"/>
-      <c r="D102" s="67"/>
-      <c r="E102" s="67"/>
-      <c r="F102" s="67"/>
+      <c r="A102" s="70"/>
+      <c r="B102" s="70"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="70"/>
+      <c r="E102" s="70"/>
+      <c r="F102" s="70"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="A103" s="67"/>
-      <c r="B103" s="67"/>
-      <c r="C103" s="67"/>
-      <c r="D103" s="67"/>
-      <c r="E103" s="67"/>
-      <c r="F103" s="67"/>
+      <c r="A103" s="70"/>
+      <c r="B103" s="70"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="70"/>
+      <c r="E103" s="70"/>
+      <c r="F103" s="70"/>
     </row>
     <row r="104" ht="14.25">
-      <c r="A104" s="67"/>
-      <c r="B104" s="67"/>
-      <c r="C104" s="67"/>
-      <c r="D104" s="67"/>
-      <c r="E104" s="67"/>
-      <c r="F104" s="67"/>
+      <c r="A104" s="70"/>
+      <c r="B104" s="70"/>
+      <c r="C104" s="70"/>
+      <c r="D104" s="70"/>
+      <c r="E104" s="70"/>
+      <c r="F104" s="70"/>
     </row>
     <row r="105" ht="14.25">
-      <c r="A105" s="67"/>
-      <c r="B105" s="67"/>
-      <c r="C105" s="67"/>
-      <c r="D105" s="67"/>
-      <c r="E105" s="67"/>
-      <c r="F105" s="67"/>
+      <c r="A105" s="70"/>
+      <c r="B105" s="70"/>
+      <c r="C105" s="70"/>
+      <c r="D105" s="70"/>
+      <c r="E105" s="70"/>
+      <c r="F105" s="70"/>
     </row>
     <row r="106" ht="14.25">
-      <c r="A106" s="67"/>
-      <c r="B106" s="67"/>
-      <c r="C106" s="67"/>
-      <c r="D106" s="67"/>
-      <c r="E106" s="67"/>
-      <c r="F106" s="67"/>
+      <c r="A106" s="70"/>
+      <c r="B106" s="70"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="70"/>
+      <c r="E106" s="70"/>
+      <c r="F106" s="70"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="A107" s="67"/>
-      <c r="B107" s="67"/>
-      <c r="C107" s="67"/>
-      <c r="D107" s="67"/>
-      <c r="E107" s="67"/>
-      <c r="F107" s="67"/>
+      <c r="A107" s="70"/>
+      <c r="B107" s="70"/>
+      <c r="C107" s="70"/>
+      <c r="D107" s="70"/>
+      <c r="E107" s="70"/>
+      <c r="F107" s="70"/>
     </row>
     <row r="108" ht="14.25">
-      <c r="A108" s="67"/>
-      <c r="B108" s="67"/>
-      <c r="C108" s="67"/>
-      <c r="D108" s="67"/>
-      <c r="E108" s="67"/>
-      <c r="F108" s="67"/>
+      <c r="A108" s="70"/>
+      <c r="B108" s="70"/>
+      <c r="C108" s="70"/>
+      <c r="D108" s="70"/>
+      <c r="E108" s="70"/>
+      <c r="F108" s="70"/>
     </row>
     <row r="109" ht="14.25">
-      <c r="A109" s="67"/>
-      <c r="B109" s="67"/>
-      <c r="C109" s="67"/>
-      <c r="D109" s="67"/>
-      <c r="E109" s="67"/>
-      <c r="F109" s="67"/>
+      <c r="A109" s="70"/>
+      <c r="B109" s="70"/>
+      <c r="C109" s="70"/>
+      <c r="D109" s="70"/>
+      <c r="E109" s="70"/>
+      <c r="F109" s="70"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="A110" s="67"/>
-      <c r="B110" s="67"/>
-      <c r="C110" s="67"/>
-      <c r="D110" s="67"/>
-      <c r="E110" s="67"/>
-      <c r="F110" s="67"/>
+      <c r="A110" s="70"/>
+      <c r="B110" s="70"/>
+      <c r="C110" s="70"/>
+      <c r="D110" s="70"/>
+      <c r="E110" s="70"/>
+      <c r="F110" s="70"/>
     </row>
     <row r="111" ht="14.25">
-      <c r="A111" s="67"/>
-      <c r="B111" s="67"/>
-      <c r="C111" s="67"/>
-      <c r="D111" s="67"/>
-      <c r="E111" s="67"/>
-      <c r="F111" s="67"/>
+      <c r="A111" s="70"/>
+      <c r="B111" s="70"/>
+      <c r="C111" s="70"/>
+      <c r="D111" s="70"/>
+      <c r="E111" s="70"/>
+      <c r="F111" s="70"/>
     </row>
     <row r="112" ht="14.25">
-      <c r="A112" s="67"/>
-      <c r="B112" s="67"/>
-      <c r="C112" s="67"/>
-      <c r="D112" s="67"/>
-      <c r="E112" s="67"/>
-      <c r="F112" s="67"/>
+      <c r="A112" s="70"/>
+      <c r="B112" s="70"/>
+      <c r="C112" s="70"/>
+      <c r="D112" s="70"/>
+      <c r="E112" s="70"/>
+      <c r="F112" s="70"/>
     </row>
     <row r="113" ht="14.25">
-      <c r="A113" s="67"/>
-      <c r="B113" s="67"/>
-      <c r="C113" s="67"/>
-      <c r="D113" s="67"/>
-      <c r="E113" s="67"/>
-      <c r="F113" s="67"/>
+      <c r="A113" s="70"/>
+      <c r="B113" s="70"/>
+      <c r="C113" s="70"/>
+      <c r="D113" s="70"/>
+      <c r="E113" s="70"/>
+      <c r="F113" s="70"/>
     </row>
     <row r="114" ht="14.25">
-      <c r="A114" s="67"/>
-      <c r="B114" s="67"/>
-      <c r="C114" s="67"/>
-      <c r="D114" s="67"/>
-      <c r="E114" s="67"/>
-      <c r="F114" s="67"/>
+      <c r="A114" s="70"/>
+      <c r="B114" s="70"/>
+      <c r="C114" s="70"/>
+      <c r="D114" s="70"/>
+      <c r="E114" s="70"/>
+      <c r="F114" s="70"/>
     </row>
     <row r="115" ht="14.25">
-      <c r="A115" s="67"/>
-      <c r="B115" s="67"/>
-      <c r="C115" s="67"/>
-      <c r="D115" s="67"/>
-      <c r="E115" s="67"/>
-      <c r="F115" s="67"/>
+      <c r="A115" s="70"/>
+      <c r="B115" s="70"/>
+      <c r="C115" s="70"/>
+      <c r="D115" s="70"/>
+      <c r="E115" s="70"/>
+      <c r="F115" s="70"/>
     </row>
     <row r="116" ht="14.25">
-      <c r="A116" s="67"/>
-      <c r="B116" s="67"/>
-      <c r="C116" s="67"/>
-      <c r="D116" s="67"/>
-      <c r="E116" s="67"/>
-      <c r="F116" s="67"/>
+      <c r="A116" s="70"/>
+      <c r="B116" s="70"/>
+      <c r="C116" s="70"/>
+      <c r="D116" s="70"/>
+      <c r="E116" s="70"/>
+      <c r="F116" s="70"/>
     </row>
     <row r="117" ht="14.25">
-      <c r="A117" s="67"/>
-      <c r="B117" s="67"/>
-      <c r="C117" s="67"/>
-      <c r="D117" s="67"/>
-      <c r="E117" s="67"/>
-      <c r="F117" s="67"/>
+      <c r="A117" s="70"/>
+      <c r="B117" s="70"/>
+      <c r="C117" s="70"/>
+      <c r="D117" s="70"/>
+      <c r="E117" s="70"/>
+      <c r="F117" s="70"/>
     </row>
     <row r="118" ht="14.25">
-      <c r="A118" s="67"/>
-      <c r="B118" s="67"/>
-      <c r="C118" s="67"/>
-      <c r="D118" s="67"/>
-      <c r="E118" s="67"/>
-      <c r="F118" s="67"/>
+      <c r="A118" s="70"/>
+      <c r="B118" s="70"/>
+      <c r="C118" s="70"/>
+      <c r="D118" s="70"/>
+      <c r="E118" s="70"/>
+      <c r="F118" s="70"/>
     </row>
     <row r="119" ht="14.25">
-      <c r="A119" s="67"/>
-      <c r="B119" s="67"/>
-      <c r="C119" s="67"/>
-      <c r="D119" s="67"/>
-      <c r="E119" s="67"/>
-      <c r="F119" s="67"/>
+      <c r="A119" s="70"/>
+      <c r="B119" s="70"/>
+      <c r="C119" s="70"/>
+      <c r="D119" s="70"/>
+      <c r="E119" s="70"/>
+      <c r="F119" s="70"/>
     </row>
     <row r="120" ht="14.25">
-      <c r="A120" s="67"/>
-      <c r="B120" s="67"/>
-      <c r="C120" s="67"/>
-      <c r="D120" s="67"/>
-      <c r="E120" s="67"/>
-      <c r="F120" s="67"/>
+      <c r="A120" s="70"/>
+      <c r="B120" s="70"/>
+      <c r="C120" s="70"/>
+      <c r="D120" s="70"/>
+      <c r="E120" s="70"/>
+      <c r="F120" s="70"/>
     </row>
     <row r="121" ht="14.25">
-      <c r="A121" s="67"/>
-      <c r="B121" s="67"/>
-      <c r="C121" s="67"/>
-      <c r="D121" s="67"/>
-      <c r="E121" s="67"/>
-      <c r="F121" s="67"/>
+      <c r="A121" s="70"/>
+      <c r="B121" s="70"/>
+      <c r="C121" s="70"/>
+      <c r="D121" s="70"/>
+      <c r="E121" s="70"/>
+      <c r="F121" s="70"/>
     </row>
     <row r="122" ht="14.25">
-      <c r="A122" s="67"/>
-      <c r="B122" s="67"/>
-      <c r="C122" s="67"/>
-      <c r="D122" s="67"/>
-      <c r="E122" s="67"/>
-      <c r="F122" s="67"/>
+      <c r="A122" s="70"/>
+      <c r="B122" s="70"/>
+      <c r="C122" s="70"/>
+      <c r="D122" s="70"/>
+      <c r="E122" s="70"/>
+      <c r="F122" s="70"/>
     </row>
     <row r="123" ht="14.25">
-      <c r="A123" s="67"/>
-      <c r="B123" s="67"/>
-      <c r="C123" s="67"/>
-      <c r="D123" s="67"/>
-      <c r="E123" s="67"/>
-      <c r="F123" s="67"/>
+      <c r="A123" s="70"/>
+      <c r="B123" s="70"/>
+      <c r="C123" s="70"/>
+      <c r="D123" s="70"/>
+      <c r="E123" s="70"/>
+      <c r="F123" s="70"/>
     </row>
     <row r="124" ht="14.25">
-      <c r="A124" s="67"/>
-      <c r="B124" s="67"/>
-      <c r="C124" s="67"/>
-      <c r="D124" s="67"/>
-      <c r="E124" s="67"/>
-      <c r="F124" s="67"/>
+      <c r="A124" s="70"/>
+      <c r="B124" s="70"/>
+      <c r="C124" s="70"/>
+      <c r="D124" s="70"/>
+      <c r="E124" s="70"/>
+      <c r="F124" s="70"/>
     </row>
     <row r="125" ht="14.25">
-      <c r="A125" s="67"/>
-      <c r="B125" s="67"/>
-      <c r="C125" s="67"/>
-      <c r="D125" s="67"/>
-      <c r="E125" s="67"/>
-      <c r="F125" s="67"/>
+      <c r="A125" s="70"/>
+      <c r="B125" s="70"/>
+      <c r="C125" s="70"/>
+      <c r="D125" s="70"/>
+      <c r="E125" s="70"/>
+      <c r="F125" s="70"/>
+    </row>
+    <row r="126" ht="14.25">
+      <c r="A126" s="70"/>
+      <c r="B126" s="70"/>
+      <c r="C126" s="70"/>
+      <c r="D126" s="70"/>
+      <c r="E126" s="70"/>
+      <c r="F126" s="70"/>
+    </row>
+    <row r="127" ht="14.25">
+      <c r="A127" s="70"/>
+      <c r="B127" s="70"/>
+      <c r="C127" s="70"/>
+      <c r="D127" s="70"/>
+      <c r="E127" s="70"/>
+      <c r="F127" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5708,7 +5829,7 @@
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A61:A64"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Latest state of evaluation
</commit_message>
<xml_diff>
--- a/experiments/experiments.xlsx
+++ b/experiments/experiments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>Network</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>LASTEN2VGIE</t>
+  </si>
+  <si>
+    <t>LASTEN2VGF</t>
+  </si>
+  <si>
+    <t>LASTEN2VGFI</t>
   </si>
   <si>
     <t>Possibilities</t>
@@ -453,6 +459,12 @@
   </si>
   <si>
     <t xml:space="preserve">1840 images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like LASTEN2VGN but more precise images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Like LASTEN2VGN but interpolated</t>
   </si>
 </sst>
 </file>
@@ -822,9 +834,7 @@
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color theme="1"/>
       </bottom>
@@ -839,7 +849,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="96">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,19 +1022,13 @@
     <xf fontId="0" fillId="28" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="28" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="24" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="28" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="28" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1033,20 +1037,17 @@
     <xf fontId="0" fillId="24" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1098,15 +1099,8 @@
     <xf fontId="0" fillId="24" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="24" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1558,8 +1552,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="1" max="1" style="0" width="22"/>
-    <col customWidth="1" min="2" max="2" style="0" width="45.9296875"/>
-    <col customWidth="1" min="3" max="3" style="0" width="10.8515625"/>
+    <col customWidth="1" min="2" max="2" style="0" width="53.00390625"/>
+    <col customWidth="1" min="3" max="3" style="0" width="18.57421875"/>
     <col customWidth="1" min="4" max="4" style="0" width="31.9296875"/>
     <col customWidth="1" min="5" max="5" style="0" width="24.00390625"/>
     <col customWidth="1" min="6" max="6" style="0" width="29.00390625"/>
@@ -4830,13 +4824,13 @@
       <c r="U60" s="10"/>
     </row>
     <row r="61" ht="14.25">
-      <c r="A61" s="51" t="s">
+      <c r="A61" s="40" t="s">
         <v>95</v>
       </c>
       <c r="B61" s="8">
         <v>1</v>
       </c>
-      <c r="C61" s="13"/>
+      <c r="C61" s="3"/>
       <c r="D61" s="13"/>
       <c r="E61" s="59" t="s">
         <v>96</v>
@@ -4887,13 +4881,13 @@
       <c r="U61" s="15"/>
     </row>
     <row r="62" ht="14.25">
-      <c r="A62" s="7"/>
+      <c r="A62" s="60"/>
       <c r="B62" s="11">
         <v>2</v>
       </c>
-      <c r="C62" s="1"/>
+      <c r="C62" s="9"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="60" t="s">
+      <c r="E62" s="61" t="s">
         <v>97</v>
       </c>
       <c r="F62" s="1">
@@ -4911,44 +4905,44 @@
       <c r="J62" s="1">
         <v>32</v>
       </c>
-      <c r="K62" s="61" t="s">
+      <c r="K62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L62" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="M62" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="N62" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="O62" s="61" t="s">
+      <c r="L62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O62" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P62" s="61" t="s">
+      <c r="P62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q62" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="R62" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="S62" s="62" t="s">
+      <c r="Q62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S62" s="48" t="s">
         <v>22</v>
       </c>
       <c r="T62" s="1"/>
       <c r="U62" s="10"/>
     </row>
     <row r="63" ht="14.25">
-      <c r="A63" s="7"/>
+      <c r="A63" s="60"/>
       <c r="B63" s="11">
         <v>3</v>
       </c>
-      <c r="C63" s="1"/>
+      <c r="C63" s="9"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="63" t="s">
+      <c r="E63" s="61" t="s">
         <v>98</v>
       </c>
       <c r="F63" s="1">
@@ -4997,827 +4991,961 @@
       <c r="U63" s="10"/>
     </row>
     <row r="64" ht="14.25">
-      <c r="A64" s="64"/>
-      <c r="B64" s="17">
-        <v>4</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="65" t="s">
+      <c r="A64" s="60"/>
+      <c r="B64" s="11">
+        <v>4</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="F64" s="19">
+      <c r="F64" s="1">
         <v>840</v>
       </c>
-      <c r="G64" s="19">
+      <c r="G64" s="1">
         <v>100</v>
       </c>
-      <c r="H64" s="19">
-        <v>4</v>
-      </c>
-      <c r="I64" s="19">
-        <v>4</v>
-      </c>
-      <c r="J64" s="19">
-        <v>32</v>
-      </c>
-      <c r="K64" s="19" t="s">
+      <c r="H64" s="1">
+        <v>4</v>
+      </c>
+      <c r="I64" s="1">
+        <v>4</v>
+      </c>
+      <c r="J64" s="1">
+        <v>32</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L64" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="M64" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="N64" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="O64" s="19" t="s">
+      <c r="L64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O64" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P64" s="19" t="s">
+      <c r="P64" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q64" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="R64" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="S64" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="T64" s="19"/>
-      <c r="U64" s="20"/>
+      <c r="Q64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S64" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T64" s="1"/>
+      <c r="U64" s="10"/>
     </row>
     <row r="65" ht="14.25">
-      <c r="A65" s="67"/>
-      <c r="B65" s="17" t="s">
+      <c r="A65" s="60"/>
+      <c r="B65" s="11">
+        <v>5</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="C65" s="4"/>
-      <c r="D65" s="68"/>
-      <c r="E65" s="19">
+      <c r="F65" s="1">
+        <v>800</v>
+      </c>
+      <c r="G65" s="1">
+        <v>100</v>
+      </c>
+      <c r="H65" s="1">
+        <v>4</v>
+      </c>
+      <c r="I65" s="1">
+        <v>4</v>
+      </c>
+      <c r="J65" s="1">
+        <v>32</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S65" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="T65" s="1"/>
+      <c r="U65" s="10"/>
+    </row>
+    <row r="66" ht="14.25">
+      <c r="A66" s="62"/>
+      <c r="B66" s="17">
+        <v>6</v>
+      </c>
+      <c r="C66" s="18"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="F66" s="19">
+        <v>800</v>
+      </c>
+      <c r="G66" s="19">
+        <v>100</v>
+      </c>
+      <c r="H66" s="19">
+        <v>4</v>
+      </c>
+      <c r="I66" s="19">
+        <v>4</v>
+      </c>
+      <c r="J66" s="19">
+        <v>32</v>
+      </c>
+      <c r="K66" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="N66" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O66" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P66" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q66" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="R66" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="S66" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="T66" s="19"/>
+      <c r="U66" s="20"/>
+    </row>
+    <row r="67" ht="14.25">
+      <c r="A67" s="65"/>
+      <c r="B67" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="66"/>
+      <c r="E67" s="19">
         <v>3</v>
       </c>
-      <c r="F65" s="5">
+      <c r="F67" s="19">
         <v>1</v>
       </c>
-      <c r="G65" s="5">
+      <c r="G67" s="19">
         <v>1</v>
       </c>
-      <c r="H65" s="5">
+      <c r="H67" s="19">
         <v>1</v>
       </c>
-      <c r="I65" s="5">
+      <c r="I67" s="19">
         <v>2</v>
       </c>
-      <c r="J65" s="5">
+      <c r="J67" s="19">
         <v>2</v>
       </c>
-      <c r="K65" s="5">
+      <c r="K67" s="19">
         <v>2</v>
       </c>
-      <c r="L65" s="5">
+      <c r="L67" s="19">
         <v>2</v>
       </c>
-      <c r="M65" s="5">
+      <c r="M67" s="19">
         <v>2</v>
       </c>
-      <c r="N65" s="5">
+      <c r="N67" s="19">
         <v>1</v>
       </c>
-      <c r="O65" s="5">
+      <c r="O67" s="19">
         <v>2</v>
       </c>
-      <c r="P65" s="5">
+      <c r="P67" s="19">
         <v>3</v>
       </c>
-      <c r="Q65" s="5">
+      <c r="Q67" s="19">
         <v>2</v>
       </c>
-      <c r="R65" s="5">
+      <c r="R67" s="19">
         <v>2</v>
       </c>
-      <c r="S65" s="5">
+      <c r="S67" s="19">
         <v>2</v>
       </c>
-      <c r="T65" s="5"/>
-      <c r="U65" s="69">
-        <f>PRODUCT(E65:S65)</f>
+      <c r="T67" s="19"/>
+      <c r="U67" s="20">
+        <f>PRODUCT(E67:S67)</f>
         <v>4608</v>
       </c>
     </row>
-    <row r="66" ht="14.25">
-      <c r="U66" s="70"/>
-    </row>
-    <row r="67" ht="14.25"/>
     <row r="68" ht="14.25">
-      <c r="A68" s="70"/>
-      <c r="B68" s="70"/>
-      <c r="C68" s="70"/>
-      <c r="D68" s="70"/>
-      <c r="E68" s="70"/>
-      <c r="F68" s="70"/>
-    </row>
-    <row r="69" ht="13.800000000000001">
-      <c r="A69" s="71" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69" s="72" t="s">
-        <v>102</v>
-      </c>
-      <c r="C69" s="73" t="s">
+      <c r="U68" s="67"/>
+    </row>
+    <row r="69" ht="14.25"/>
+    <row r="70" ht="14.25">
+      <c r="A70" s="67"/>
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="67"/>
+      <c r="F70" s="67"/>
+    </row>
+    <row r="71" ht="13.800000000000001">
+      <c r="A71" s="68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D69" s="73" t="s">
-        <v>103</v>
-      </c>
-      <c r="E69" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="F69" s="70"/>
-    </row>
-    <row r="70" ht="47.25" customHeight="1">
-      <c r="A70" s="74" t="s">
+      <c r="D71" s="70" t="s">
+        <v>105</v>
+      </c>
+      <c r="E71" s="71" t="s">
+        <v>106</v>
+      </c>
+      <c r="F71" s="67"/>
+    </row>
+    <row r="72" ht="47.25" customHeight="1">
+      <c r="A72" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B70" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="C70" s="76">
+      <c r="B72" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="73">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D70" s="76">
+      <c r="D72" s="73">
         <v>0.14999999999999999</v>
       </c>
-      <c r="E70" s="77">
+      <c r="E72" s="74">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F70" s="70"/>
-    </row>
-    <row r="71" ht="149.30000000000001" customHeight="1">
-      <c r="A71" s="74" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="C71" s="79" t="s">
+      <c r="F72" s="67"/>
+    </row>
+    <row r="73" ht="149.30000000000001" customHeight="1">
+      <c r="A73" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="57" t="s">
+      <c r="B73" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="E71" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F71" s="70"/>
-    </row>
-    <row r="72" ht="71.25">
-      <c r="A72" s="74" t="s">
+      <c r="C73" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E73" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F73" s="67"/>
+    </row>
+    <row r="74" ht="71.25">
+      <c r="A74" s="60" t="s">
         <v>64</v>
-      </c>
-      <c r="B72" s="81" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="82">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D72" s="82">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="E72" s="83">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F72" s="70"/>
-    </row>
-    <row r="73" ht="57">
-      <c r="A73" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="78" t="s">
-        <v>111</v>
-      </c>
-      <c r="C73" s="82">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="D73" s="82">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="E73" s="83">
-        <v>0.14999999999999999</v>
-      </c>
-      <c r="F73" s="70"/>
-    </row>
-    <row r="74" ht="57">
-      <c r="A74" s="84" t="s">
-        <v>67</v>
       </c>
       <c r="B74" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C74" s="82">
+      <c r="C74" s="79">
         <v>0.69999999999999996</v>
       </c>
-      <c r="D74" s="82">
+      <c r="D74" s="79">
         <v>0.14999999999999999</v>
       </c>
-      <c r="E74" s="83">
+      <c r="E74" s="80">
         <v>0.14999999999999999</v>
       </c>
-      <c r="F74" s="70"/>
-    </row>
-    <row r="75" ht="42.75">
-      <c r="A75" s="74" t="s">
+      <c r="F74" s="67"/>
+    </row>
+    <row r="75" ht="57">
+      <c r="A75" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" s="79">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D75" s="79">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="E75" s="80">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F75" s="67"/>
+    </row>
+    <row r="76" ht="57">
+      <c r="A76" s="81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="75" t="s">
+        <v>114</v>
+      </c>
+      <c r="C76" s="79">
+        <v>0.69999999999999996</v>
+      </c>
+      <c r="D76" s="79">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="E76" s="80">
+        <v>0.14999999999999999</v>
+      </c>
+      <c r="F76" s="67"/>
+    </row>
+    <row r="77" ht="42.75">
+      <c r="A77" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B77" s="75" t="s">
+        <v>115</v>
+      </c>
+      <c r="C77" s="57" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E77" s="77" t="s">
+        <v>118</v>
+      </c>
+      <c r="F77" s="67"/>
+    </row>
+    <row r="78" ht="114">
+      <c r="A78" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B78" s="78" t="s">
+        <v>120</v>
+      </c>
+      <c r="C78" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="D78" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E78" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" s="67"/>
+    </row>
+    <row r="79" ht="14.25">
+      <c r="A79" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="C75" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="D75" s="57" t="s">
-        <v>115</v>
-      </c>
-      <c r="E75" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="F75" s="70"/>
-    </row>
-    <row r="76" ht="114">
-      <c r="A76" s="74" t="s">
-        <v>117</v>
-      </c>
-      <c r="B76" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" s="79" t="s">
-        <v>119</v>
-      </c>
-      <c r="D76" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E76" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" s="70"/>
-    </row>
-    <row r="77" ht="14.25">
-      <c r="A77" s="74" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="85" t="s">
+      <c r="C79" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="D79" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C77" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="D77" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E77" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F77" s="70"/>
-    </row>
-    <row r="78" ht="14.25">
-      <c r="A78" s="74" t="s">
-        <v>121</v>
-      </c>
-      <c r="B78" s="85" t="s">
+      <c r="E79" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" s="67"/>
+    </row>
+    <row r="80" ht="14.25">
+      <c r="A80" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="82" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="76" t="s">
+        <v>125</v>
+      </c>
+      <c r="D80" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E80" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F80" s="67"/>
+    </row>
+    <row r="81" ht="127.2" customHeight="1">
+      <c r="A81" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81" s="84" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="D78" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E78" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F78" s="70"/>
-    </row>
-    <row r="79" ht="127.2" customHeight="1">
-      <c r="A79" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="87" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79" s="88" t="s">
-        <v>120</v>
-      </c>
-      <c r="D79" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E79" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F79" s="70"/>
-    </row>
-    <row r="80" ht="70.200000000000003" customHeight="1">
-      <c r="A80" s="86" t="s">
+      <c r="D81" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E81" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F81" s="67"/>
+    </row>
+    <row r="82" ht="70.200000000000003" customHeight="1">
+      <c r="A82" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="89" t="s">
-        <v>125</v>
-      </c>
-      <c r="C80" s="57" t="s">
-        <v>120</v>
-      </c>
-      <c r="D80" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E80" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F80" s="70"/>
-    </row>
-    <row r="81" ht="14.25">
-      <c r="A81" s="86" t="s">
+      <c r="B82" s="86" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="57" t="s">
+        <v>122</v>
+      </c>
+      <c r="D82" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E82" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F82" s="67"/>
+    </row>
+    <row r="83" ht="14.25">
+      <c r="A83" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="87" t="s">
-        <v>126</v>
-      </c>
-      <c r="C81" s="88" t="s">
-        <v>127</v>
-      </c>
-      <c r="D81" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E81" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F81" s="70"/>
-    </row>
-    <row r="82" ht="14.25">
-      <c r="A82" s="86" t="s">
+      <c r="B83" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E83" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F83" s="67"/>
+    </row>
+    <row r="84" ht="14.25">
+      <c r="A84" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="B82" s="87" t="s">
-        <v>128</v>
-      </c>
-      <c r="C82" s="88" t="s">
-        <v>127</v>
-      </c>
-      <c r="D82" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E82" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F82" s="70"/>
-    </row>
-    <row r="83" ht="14.25">
-      <c r="A83" s="86" t="s">
+      <c r="B84" s="84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" s="85" t="s">
         <v>129</v>
       </c>
-      <c r="B83" s="89" t="s">
-        <v>130</v>
-      </c>
-      <c r="C83" s="88" t="s">
+      <c r="D84" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E84" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F84" s="67"/>
+    </row>
+    <row r="85" ht="14.25">
+      <c r="A85" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="D83" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E83" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F83" s="70"/>
-    </row>
-    <row r="84" ht="14.25">
-      <c r="A84" s="86" t="s">
+      <c r="B85" s="86" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="D85" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E85" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F85" s="67"/>
+    </row>
+    <row r="86" ht="14.25">
+      <c r="A86" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="B84" s="89" t="s">
-        <v>132</v>
-      </c>
-      <c r="C84" s="90" t="s">
-        <v>120</v>
-      </c>
-      <c r="D84" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E84" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F84" s="70"/>
-    </row>
-    <row r="85" ht="14.25">
-      <c r="A85" s="86" t="s">
+      <c r="B86" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="C86" s="87" t="s">
+        <v>122</v>
+      </c>
+      <c r="D86" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E86" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F86" s="67"/>
+    </row>
+    <row r="87" ht="14.25">
+      <c r="A87" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="B85" s="89" t="s">
-        <v>133</v>
-      </c>
-      <c r="C85" s="90" t="s">
-        <v>127</v>
-      </c>
-      <c r="D85" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E85" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F85" s="70"/>
-    </row>
-    <row r="86" ht="14.25">
-      <c r="A86" s="86" t="s">
+      <c r="B87" s="86" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="D87" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E87" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F87" s="67"/>
+    </row>
+    <row r="88" ht="14.25">
+      <c r="A88" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="B86" s="89" t="s">
-        <v>134</v>
-      </c>
-      <c r="C86" s="90" t="s">
-        <v>135</v>
-      </c>
-      <c r="D86" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E86" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F86" s="70"/>
-    </row>
-    <row r="87" ht="78.400000000000006" customHeight="1">
-      <c r="A87" s="86" t="s">
+      <c r="B88" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" s="87" t="s">
+        <v>137</v>
+      </c>
+      <c r="D88" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E88" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F88" s="67"/>
+    </row>
+    <row r="89" ht="78.400000000000006" customHeight="1">
+      <c r="A89" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="B87" s="89" t="s">
-        <v>136</v>
-      </c>
-      <c r="C87" s="90" t="s">
+      <c r="B89" s="86" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="D89" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E89" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F89" s="67"/>
+    </row>
+    <row r="90" ht="78.400000000000006" customHeight="1">
+      <c r="A90" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90" s="86" t="s">
+        <v>140</v>
+      </c>
+      <c r="C90" s="85" t="s">
         <v>137</v>
       </c>
-      <c r="D87" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E87" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F87" s="70"/>
-    </row>
-    <row r="88" ht="78.400000000000006" customHeight="1">
-      <c r="A88" s="91" t="s">
-        <v>96</v>
-      </c>
-      <c r="B88" s="89" t="s">
-        <v>138</v>
-      </c>
-      <c r="C88" s="88" t="s">
-        <v>135</v>
-      </c>
-      <c r="D88" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E88" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F88" s="70"/>
-    </row>
-    <row r="89" ht="58.899999999999999" customHeight="1">
-      <c r="A89" s="91" t="s">
+      <c r="D90" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E90" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="67"/>
+    </row>
+    <row r="91" ht="58.899999999999999" customHeight="1">
+      <c r="A91" s="88" t="s">
         <v>97</v>
       </c>
-      <c r="B89" s="89" t="s">
-        <v>139</v>
-      </c>
-      <c r="C89" s="88" t="s">
-        <v>135</v>
-      </c>
-      <c r="D89" s="57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E89" s="80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F89" s="70"/>
-    </row>
-    <row r="90" ht="58.899999999999999" customHeight="1">
-      <c r="A90" s="92" t="s">
+      <c r="B91" s="86" t="s">
+        <v>141</v>
+      </c>
+      <c r="C91" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D91" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E91" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F91" s="67"/>
+    </row>
+    <row r="92" ht="58.899999999999999" customHeight="1">
+      <c r="A92" s="88" t="s">
         <v>98</v>
       </c>
-      <c r="B90" s="93" t="s">
-        <v>140</v>
-      </c>
-      <c r="C90" s="94" t="s">
-        <v>141</v>
-      </c>
-      <c r="D90" s="57"/>
-      <c r="E90" s="80"/>
-      <c r="F90" s="70"/>
-    </row>
-    <row r="91" ht="14.25">
-      <c r="A91" s="95" t="s">
+      <c r="B92" s="86" t="s">
+        <v>142</v>
+      </c>
+      <c r="C92" s="85" t="s">
+        <v>143</v>
+      </c>
+      <c r="D92" s="57"/>
+      <c r="E92" s="77"/>
+      <c r="F92" s="67"/>
+    </row>
+    <row r="93" ht="14.25">
+      <c r="A93" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="B91" s="96" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" s="97" t="s">
-        <v>143</v>
-      </c>
-      <c r="D91" s="98" t="s">
-        <v>109</v>
-      </c>
-      <c r="E91" s="99" t="s">
-        <v>109</v>
-      </c>
-      <c r="F91" s="70"/>
-    </row>
-    <row r="92" ht="14.25">
-      <c r="A92" s="70"/>
-      <c r="B92" s="70"/>
-      <c r="C92" s="70"/>
-      <c r="D92" s="70"/>
-      <c r="E92" s="70"/>
-      <c r="F92" s="70"/>
-    </row>
-    <row r="93" ht="14.25">
-      <c r="A93" s="70"/>
-      <c r="B93" s="70"/>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="70"/>
+      <c r="B93" s="90" t="s">
+        <v>144</v>
+      </c>
+      <c r="C93" s="85" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E93" s="77" t="s">
+        <v>111</v>
+      </c>
+      <c r="F93" s="67"/>
     </row>
     <row r="94" ht="14.25">
-      <c r="A94" s="70"/>
-      <c r="B94" s="70"/>
-      <c r="C94" s="70"/>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70"/>
-      <c r="F94" s="70"/>
+      <c r="A94" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="90" t="s">
+        <v>146</v>
+      </c>
+      <c r="C94" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D94" s="57"/>
+      <c r="E94" s="77"/>
+      <c r="F94" s="67"/>
     </row>
     <row r="95" ht="14.25">
-      <c r="A95" s="70"/>
-      <c r="B95" s="70"/>
-      <c r="C95" s="70"/>
-      <c r="D95" s="70"/>
-      <c r="E95" s="70"/>
-      <c r="F95" s="70"/>
+      <c r="A95" s="91" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" s="92" t="s">
+        <v>147</v>
+      </c>
+      <c r="C95" s="93" t="s">
+        <v>137</v>
+      </c>
+      <c r="D95" s="94" t="s">
+        <v>111</v>
+      </c>
+      <c r="E95" s="95" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="67"/>
     </row>
     <row r="96" ht="14.25">
-      <c r="A96" s="70"/>
-      <c r="B96" s="70"/>
-      <c r="C96" s="70"/>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70"/>
-      <c r="F96" s="70"/>
+      <c r="A96" s="67"/>
+      <c r="B96" s="67"/>
+      <c r="C96" s="67"/>
+      <c r="D96" s="67"/>
+      <c r="E96" s="67"/>
+      <c r="F96" s="67"/>
     </row>
     <row r="97" ht="14.25">
-      <c r="A97" s="70"/>
-      <c r="B97" s="70"/>
-      <c r="C97" s="70"/>
-      <c r="D97" s="70"/>
-      <c r="E97" s="70"/>
-      <c r="F97" s="70"/>
+      <c r="A97" s="67"/>
+      <c r="B97" s="67"/>
+      <c r="C97" s="67"/>
+      <c r="D97" s="67"/>
+      <c r="E97" s="67"/>
+      <c r="F97" s="67"/>
     </row>
     <row r="98" ht="14.25">
-      <c r="A98" s="70"/>
-      <c r="B98" s="70"/>
-      <c r="C98" s="70"/>
-      <c r="D98" s="70"/>
-      <c r="E98" s="70"/>
-      <c r="F98" s="70"/>
+      <c r="A98" s="67"/>
+      <c r="B98" s="67"/>
+      <c r="C98" s="67"/>
+      <c r="D98" s="67"/>
+      <c r="E98" s="67"/>
+      <c r="F98" s="67"/>
     </row>
     <row r="99" ht="14.25">
-      <c r="A99" s="70"/>
-      <c r="B99" s="70"/>
-      <c r="C99" s="70"/>
-      <c r="D99" s="70"/>
-      <c r="E99" s="70"/>
-      <c r="F99" s="70"/>
+      <c r="A99" s="67"/>
+      <c r="B99" s="67"/>
+      <c r="C99" s="67"/>
+      <c r="D99" s="67"/>
+      <c r="E99" s="67"/>
+      <c r="F99" s="67"/>
     </row>
     <row r="100" ht="14.25">
-      <c r="A100" s="70"/>
-      <c r="B100" s="70"/>
-      <c r="C100" s="70"/>
-      <c r="D100" s="70"/>
-      <c r="E100" s="70"/>
-      <c r="F100" s="70"/>
+      <c r="A100" s="67"/>
+      <c r="B100" s="67"/>
+      <c r="C100" s="67"/>
+      <c r="D100" s="67"/>
+      <c r="E100" s="67"/>
+      <c r="F100" s="67"/>
     </row>
     <row r="101" ht="14.25">
-      <c r="A101" s="70"/>
-      <c r="B101" s="70"/>
-      <c r="C101" s="70"/>
-      <c r="D101" s="70"/>
-      <c r="E101" s="70"/>
-      <c r="F101" s="70"/>
+      <c r="A101" s="67"/>
+      <c r="B101" s="67"/>
+      <c r="C101" s="67"/>
+      <c r="D101" s="67"/>
+      <c r="E101" s="67"/>
+      <c r="F101" s="67"/>
     </row>
     <row r="102" ht="14.25">
-      <c r="A102" s="70"/>
-      <c r="B102" s="70"/>
-      <c r="C102" s="70"/>
-      <c r="D102" s="70"/>
-      <c r="E102" s="70"/>
-      <c r="F102" s="70"/>
+      <c r="A102" s="67"/>
+      <c r="B102" s="67"/>
+      <c r="C102" s="67"/>
+      <c r="D102" s="67"/>
+      <c r="E102" s="67"/>
+      <c r="F102" s="67"/>
     </row>
     <row r="103" ht="14.25">
-      <c r="A103" s="70"/>
-      <c r="B103" s="70"/>
-      <c r="C103" s="70"/>
-      <c r="D103" s="70"/>
-      <c r="E103" s="70"/>
-      <c r="F103" s="70"/>
+      <c r="A103" s="67"/>
+      <c r="B103" s="67"/>
+      <c r="C103" s="67"/>
+      <c r="D103" s="67"/>
+      <c r="E103" s="67"/>
+      <c r="F103" s="67"/>
     </row>
     <row r="104" ht="14.25">
-      <c r="A104" s="70"/>
-      <c r="B104" s="70"/>
-      <c r="C104" s="70"/>
-      <c r="D104" s="70"/>
-      <c r="E104" s="70"/>
-      <c r="F104" s="70"/>
+      <c r="A104" s="67"/>
+      <c r="B104" s="67"/>
+      <c r="C104" s="67"/>
+      <c r="D104" s="67"/>
+      <c r="E104" s="67"/>
+      <c r="F104" s="67"/>
     </row>
     <row r="105" ht="14.25">
-      <c r="A105" s="70"/>
-      <c r="B105" s="70"/>
-      <c r="C105" s="70"/>
-      <c r="D105" s="70"/>
-      <c r="E105" s="70"/>
-      <c r="F105" s="70"/>
+      <c r="A105" s="67"/>
+      <c r="B105" s="67"/>
+      <c r="C105" s="67"/>
+      <c r="D105" s="67"/>
+      <c r="E105" s="67"/>
+      <c r="F105" s="67"/>
     </row>
     <row r="106" ht="14.25">
-      <c r="A106" s="70"/>
-      <c r="B106" s="70"/>
-      <c r="C106" s="70"/>
-      <c r="D106" s="70"/>
-      <c r="E106" s="70"/>
-      <c r="F106" s="70"/>
+      <c r="A106" s="67"/>
+      <c r="B106" s="67"/>
+      <c r="C106" s="67"/>
+      <c r="D106" s="67"/>
+      <c r="E106" s="67"/>
+      <c r="F106" s="67"/>
     </row>
     <row r="107" ht="14.25">
-      <c r="A107" s="70"/>
-      <c r="B107" s="70"/>
-      <c r="C107" s="70"/>
-      <c r="D107" s="70"/>
-      <c r="E107" s="70"/>
-      <c r="F107" s="70"/>
+      <c r="A107" s="67"/>
+      <c r="B107" s="67"/>
+      <c r="C107" s="67"/>
+      <c r="D107" s="67"/>
+      <c r="E107" s="67"/>
+      <c r="F107" s="67"/>
     </row>
     <row r="108" ht="14.25">
-      <c r="A108" s="70"/>
-      <c r="B108" s="70"/>
-      <c r="C108" s="70"/>
-      <c r="D108" s="70"/>
-      <c r="E108" s="70"/>
-      <c r="F108" s="70"/>
+      <c r="A108" s="67"/>
+      <c r="B108" s="67"/>
+      <c r="C108" s="67"/>
+      <c r="D108" s="67"/>
+      <c r="E108" s="67"/>
+      <c r="F108" s="67"/>
     </row>
     <row r="109" ht="14.25">
-      <c r="A109" s="70"/>
-      <c r="B109" s="70"/>
-      <c r="C109" s="70"/>
-      <c r="D109" s="70"/>
-      <c r="E109" s="70"/>
-      <c r="F109" s="70"/>
+      <c r="A109" s="67"/>
+      <c r="B109" s="67"/>
+      <c r="C109" s="67"/>
+      <c r="D109" s="67"/>
+      <c r="E109" s="67"/>
+      <c r="F109" s="67"/>
     </row>
     <row r="110" ht="14.25">
-      <c r="A110" s="70"/>
-      <c r="B110" s="70"/>
-      <c r="C110" s="70"/>
-      <c r="D110" s="70"/>
-      <c r="E110" s="70"/>
-      <c r="F110" s="70"/>
+      <c r="A110" s="67"/>
+      <c r="B110" s="67"/>
+      <c r="C110" s="67"/>
+      <c r="D110" s="67"/>
+      <c r="E110" s="67"/>
+      <c r="F110" s="67"/>
     </row>
     <row r="111" ht="14.25">
-      <c r="A111" s="70"/>
-      <c r="B111" s="70"/>
-      <c r="C111" s="70"/>
-      <c r="D111" s="70"/>
-      <c r="E111" s="70"/>
-      <c r="F111" s="70"/>
+      <c r="A111" s="67"/>
+      <c r="B111" s="67"/>
+      <c r="C111" s="67"/>
+      <c r="D111" s="67"/>
+      <c r="E111" s="67"/>
+      <c r="F111" s="67"/>
     </row>
     <row r="112" ht="14.25">
-      <c r="A112" s="70"/>
-      <c r="B112" s="70"/>
-      <c r="C112" s="70"/>
-      <c r="D112" s="70"/>
-      <c r="E112" s="70"/>
-      <c r="F112" s="70"/>
+      <c r="A112" s="67"/>
+      <c r="B112" s="67"/>
+      <c r="C112" s="67"/>
+      <c r="D112" s="67"/>
+      <c r="E112" s="67"/>
+      <c r="F112" s="67"/>
     </row>
     <row r="113" ht="14.25">
-      <c r="A113" s="70"/>
-      <c r="B113" s="70"/>
-      <c r="C113" s="70"/>
-      <c r="D113" s="70"/>
-      <c r="E113" s="70"/>
-      <c r="F113" s="70"/>
+      <c r="A113" s="67"/>
+      <c r="B113" s="67"/>
+      <c r="C113" s="67"/>
+      <c r="D113" s="67"/>
+      <c r="E113" s="67"/>
+      <c r="F113" s="67"/>
     </row>
     <row r="114" ht="14.25">
-      <c r="A114" s="70"/>
-      <c r="B114" s="70"/>
-      <c r="C114" s="70"/>
-      <c r="D114" s="70"/>
-      <c r="E114" s="70"/>
-      <c r="F114" s="70"/>
+      <c r="A114" s="67"/>
+      <c r="B114" s="67"/>
+      <c r="C114" s="67"/>
+      <c r="D114" s="67"/>
+      <c r="E114" s="67"/>
+      <c r="F114" s="67"/>
     </row>
     <row r="115" ht="14.25">
-      <c r="A115" s="70"/>
-      <c r="B115" s="70"/>
-      <c r="C115" s="70"/>
-      <c r="D115" s="70"/>
-      <c r="E115" s="70"/>
-      <c r="F115" s="70"/>
+      <c r="A115" s="67"/>
+      <c r="B115" s="67"/>
+      <c r="C115" s="67"/>
+      <c r="D115" s="67"/>
+      <c r="E115" s="67"/>
+      <c r="F115" s="67"/>
     </row>
     <row r="116" ht="14.25">
-      <c r="A116" s="70"/>
-      <c r="B116" s="70"/>
-      <c r="C116" s="70"/>
-      <c r="D116" s="70"/>
-      <c r="E116" s="70"/>
-      <c r="F116" s="70"/>
+      <c r="A116" s="67"/>
+      <c r="B116" s="67"/>
+      <c r="C116" s="67"/>
+      <c r="D116" s="67"/>
+      <c r="E116" s="67"/>
+      <c r="F116" s="67"/>
     </row>
     <row r="117" ht="14.25">
-      <c r="A117" s="70"/>
-      <c r="B117" s="70"/>
-      <c r="C117" s="70"/>
-      <c r="D117" s="70"/>
-      <c r="E117" s="70"/>
-      <c r="F117" s="70"/>
+      <c r="A117" s="67"/>
+      <c r="B117" s="67"/>
+      <c r="C117" s="67"/>
+      <c r="D117" s="67"/>
+      <c r="E117" s="67"/>
+      <c r="F117" s="67"/>
     </row>
     <row r="118" ht="14.25">
-      <c r="A118" s="70"/>
-      <c r="B118" s="70"/>
-      <c r="C118" s="70"/>
-      <c r="D118" s="70"/>
-      <c r="E118" s="70"/>
-      <c r="F118" s="70"/>
+      <c r="A118" s="67"/>
+      <c r="B118" s="67"/>
+      <c r="C118" s="67"/>
+      <c r="D118" s="67"/>
+      <c r="E118" s="67"/>
+      <c r="F118" s="67"/>
     </row>
     <row r="119" ht="14.25">
-      <c r="A119" s="70"/>
-      <c r="B119" s="70"/>
-      <c r="C119" s="70"/>
-      <c r="D119" s="70"/>
-      <c r="E119" s="70"/>
-      <c r="F119" s="70"/>
+      <c r="A119" s="67"/>
+      <c r="B119" s="67"/>
+      <c r="C119" s="67"/>
+      <c r="D119" s="67"/>
+      <c r="E119" s="67"/>
+      <c r="F119" s="67"/>
     </row>
     <row r="120" ht="14.25">
-      <c r="A120" s="70"/>
-      <c r="B120" s="70"/>
-      <c r="C120" s="70"/>
-      <c r="D120" s="70"/>
-      <c r="E120" s="70"/>
-      <c r="F120" s="70"/>
+      <c r="A120" s="67"/>
+      <c r="B120" s="67"/>
+      <c r="C120" s="67"/>
+      <c r="D120" s="67"/>
+      <c r="E120" s="67"/>
+      <c r="F120" s="67"/>
     </row>
     <row r="121" ht="14.25">
-      <c r="A121" s="70"/>
-      <c r="B121" s="70"/>
-      <c r="C121" s="70"/>
-      <c r="D121" s="70"/>
-      <c r="E121" s="70"/>
-      <c r="F121" s="70"/>
+      <c r="A121" s="67"/>
+      <c r="B121" s="67"/>
+      <c r="C121" s="67"/>
+      <c r="D121" s="67"/>
+      <c r="E121" s="67"/>
+      <c r="F121" s="67"/>
     </row>
     <row r="122" ht="14.25">
-      <c r="A122" s="70"/>
-      <c r="B122" s="70"/>
-      <c r="C122" s="70"/>
-      <c r="D122" s="70"/>
-      <c r="E122" s="70"/>
-      <c r="F122" s="70"/>
+      <c r="A122" s="67"/>
+      <c r="B122" s="67"/>
+      <c r="C122" s="67"/>
+      <c r="D122" s="67"/>
+      <c r="E122" s="67"/>
+      <c r="F122" s="67"/>
     </row>
     <row r="123" ht="14.25">
-      <c r="A123" s="70"/>
-      <c r="B123" s="70"/>
-      <c r="C123" s="70"/>
-      <c r="D123" s="70"/>
-      <c r="E123" s="70"/>
-      <c r="F123" s="70"/>
+      <c r="A123" s="67"/>
+      <c r="B123" s="67"/>
+      <c r="C123" s="67"/>
+      <c r="D123" s="67"/>
+      <c r="E123" s="67"/>
+      <c r="F123" s="67"/>
     </row>
     <row r="124" ht="14.25">
-      <c r="A124" s="70"/>
-      <c r="B124" s="70"/>
-      <c r="C124" s="70"/>
-      <c r="D124" s="70"/>
-      <c r="E124" s="70"/>
-      <c r="F124" s="70"/>
+      <c r="A124" s="67"/>
+      <c r="B124" s="67"/>
+      <c r="C124" s="67"/>
+      <c r="D124" s="67"/>
+      <c r="E124" s="67"/>
+      <c r="F124" s="67"/>
     </row>
     <row r="125" ht="14.25">
-      <c r="A125" s="70"/>
-      <c r="B125" s="70"/>
-      <c r="C125" s="70"/>
-      <c r="D125" s="70"/>
-      <c r="E125" s="70"/>
-      <c r="F125" s="70"/>
+      <c r="A125" s="67"/>
+      <c r="B125" s="67"/>
+      <c r="C125" s="67"/>
+      <c r="D125" s="67"/>
+      <c r="E125" s="67"/>
+      <c r="F125" s="67"/>
     </row>
     <row r="126" ht="14.25">
-      <c r="A126" s="70"/>
-      <c r="B126" s="70"/>
-      <c r="C126" s="70"/>
-      <c r="D126" s="70"/>
-      <c r="E126" s="70"/>
-      <c r="F126" s="70"/>
+      <c r="A126" s="67"/>
+      <c r="B126" s="67"/>
+      <c r="C126" s="67"/>
+      <c r="D126" s="67"/>
+      <c r="E126" s="67"/>
+      <c r="F126" s="67"/>
     </row>
     <row r="127" ht="14.25">
-      <c r="A127" s="70"/>
-      <c r="B127" s="70"/>
-      <c r="C127" s="70"/>
-      <c r="D127" s="70"/>
-      <c r="E127" s="70"/>
-      <c r="F127" s="70"/>
+      <c r="A127" s="67"/>
+      <c r="B127" s="67"/>
+      <c r="C127" s="67"/>
+      <c r="D127" s="67"/>
+      <c r="E127" s="67"/>
+      <c r="F127" s="67"/>
+    </row>
+    <row r="128" ht="14.25">
+      <c r="A128" s="67"/>
+      <c r="B128" s="67"/>
+      <c r="C128" s="67"/>
+      <c r="D128" s="67"/>
+      <c r="E128" s="67"/>
+      <c r="F128" s="67"/>
+    </row>
+    <row r="129" ht="14.25">
+      <c r="A129" s="67"/>
+      <c r="B129" s="67"/>
+      <c r="C129" s="67"/>
+      <c r="D129" s="67"/>
+      <c r="E129" s="67"/>
+      <c r="F129" s="67"/>
+    </row>
+    <row r="130" ht="14.25">
+      <c r="A130" s="67"/>
+      <c r="B130" s="67"/>
+      <c r="C130" s="67"/>
+      <c r="D130" s="67"/>
+      <c r="E130" s="67"/>
+      <c r="F130" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -5829,7 +5957,7 @@
     <mergeCell ref="A41:A51"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A61:A66"/>
   </mergeCells>
   <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.70069444444444395" right="0.70069444444444395" top="0.75208333333333299" bottom="0.75208333333333299" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>